<commit_message>
Addition of FromLineWeight and ToLineWeight added additions to the Excel Data files for testing
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9667AA17-BA8E-4A3B-81DE-0BBF4BBA11FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECCE914-0970-4F54-B554-D40EF5E19636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24675" yWindow="150" windowWidth="24165" windowHeight="15300" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-27090" yWindow="615" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="265">
   <si>
     <t>mach_name</t>
   </si>
@@ -424,9 +424,6 @@
   </si>
   <si>
     <t>Stencil</t>
-  </si>
-  <si>
-    <t>;Visio Section</t>
   </si>
   <si>
     <t>C:\Omnicell_Blueprinting_Tool\Data\Templates\OC_BlueprintingTemplate.vstx</t>
@@ -969,6 +966,102 @@
   </si>
   <si>
     <t>OC_TableCell:48</t>
+  </si>
+  <si>
+    <t>From Line Weight</t>
+  </si>
+  <si>
+    <t>To Line Weight</t>
+  </si>
+  <si>
+    <t>Line Weight</t>
+  </si>
+  <si>
+    <t>1.5 pt</t>
+  </si>
+  <si>
+    <t>2.0 pt</t>
+  </si>
+  <si>
+    <t>2.25 pt</t>
+  </si>
+  <si>
+    <t>3.0 pt</t>
+  </si>
+  <si>
+    <t>4.0 pt</t>
+  </si>
+  <si>
+    <t>6.0 pt</t>
+  </si>
+  <si>
+    <t>;Color Section</t>
+  </si>
+  <si>
+    <t>OC_CPM:51</t>
+  </si>
+  <si>
+    <t>OC_AIO:50</t>
+  </si>
+  <si>
+    <t>OC_AIO:52</t>
+  </si>
+  <si>
+    <t>OC_CPM:53</t>
+  </si>
+  <si>
+    <t>OC_AIO:54</t>
+  </si>
+  <si>
+    <t>OC_CPM:55</t>
+  </si>
+  <si>
+    <t>OC_AIO:56</t>
+  </si>
+  <si>
+    <t>OC_CPM:57</t>
+  </si>
+  <si>
+    <t>OC_AIO:58</t>
+  </si>
+  <si>
+    <t>OC_CPM:59</t>
+  </si>
+  <si>
+    <t>OC_AIO:60</t>
+  </si>
+  <si>
+    <t>OC_CPM:61</t>
+  </si>
+  <si>
+    <t>OC_AIO:62</t>
+  </si>
+  <si>
+    <t>OC_CPM:63</t>
+  </si>
+  <si>
+    <t>;Line weight</t>
+  </si>
+  <si>
+    <t>1.0 pt.</t>
+  </si>
+  <si>
+    <t>2.0 pt.</t>
+  </si>
+  <si>
+    <t>3.0 pt.</t>
+  </si>
+  <si>
+    <t>2.25 pt.</t>
+  </si>
+  <si>
+    <t>1.5 pt.</t>
+  </si>
+  <si>
+    <t>4.0 pt.</t>
+  </si>
+  <si>
+    <t>6.0 pt.</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1304,6 +1397,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1325,22 +1435,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1657,11 +1756,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AH174"/>
+  <dimension ref="A1:AJ189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W34" sqref="W34"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,14 +1780,14 @@
     <col min="26" max="26" width="13.28515625" customWidth="1"/>
     <col min="27" max="27" width="14.42578125" customWidth="1"/>
     <col min="28" max="28" width="13.28515625" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" customWidth="1"/>
-    <col min="30" max="30" width="15.7109375" customWidth="1"/>
-    <col min="31" max="31" width="11" customWidth="1"/>
-    <col min="32" max="32" width="12" customWidth="1"/>
-    <col min="34" max="34" width="11.7109375" customWidth="1"/>
+    <col min="29" max="30" width="10.28515625" customWidth="1"/>
+    <col min="31" max="31" width="15.7109375" customWidth="1"/>
+    <col min="32" max="32" width="11" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="35" max="36" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>32</v>
       </c>
@@ -1696,19 +1795,19 @@
         <v>31</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D1" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
@@ -1756,43 +1855,49 @@
         <v>13</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="Z1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AC1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AD1" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="19" t="s">
+      <c r="AG1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="AF1" s="19" t="s">
+      <c r="AH1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="AG1" s="19" t="s">
+      <c r="AI1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AJ1" s="19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>65</v>
       </c>
@@ -1829,20 +1934,22 @@
       <c r="AF2" s="16"/>
       <c r="AG2" s="16"/>
       <c r="AH2" s="16"/>
-    </row>
-    <row r="3" spans="1:34" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="AI2" s="16"/>
+      <c r="AJ2" s="16"/>
+    </row>
+    <row r="3" spans="1:36" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1878,21 +1985,23 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7"/>
-      <c r="AF3" s="11"/>
+      <c r="AF3" s="7"/>
       <c r="AG3" s="11"/>
-      <c r="AH3" s="7"/>
-    </row>
-    <row r="4" spans="1:34" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+    </row>
+    <row r="4" spans="1:36" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F4" s="35"/>
       <c r="G4" s="8"/>
@@ -1928,23 +2037,25 @@
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
       <c r="AE4" s="7"/>
-      <c r="AF4" s="11"/>
+      <c r="AF4" s="7"/>
       <c r="AG4" s="11"/>
-      <c r="AH4" s="7"/>
-    </row>
-    <row r="5" spans="1:34" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+    </row>
+    <row r="5" spans="1:36" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="35" t="s">
         <v>84</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>85</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="35"/>
       <c r="G5" s="8"/>
@@ -1980,23 +2091,25 @@
       <c r="AC5" s="7"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="7"/>
-      <c r="AF5" s="11"/>
+      <c r="AF5" s="7"/>
       <c r="AG5" s="11"/>
-      <c r="AH5" s="7"/>
-    </row>
-    <row r="6" spans="1:34" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+    </row>
+    <row r="6" spans="1:36" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>179</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>180</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="8"/>
@@ -2032,13 +2145,15 @@
       <c r="AC6" s="7"/>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7"/>
-      <c r="AF6" s="11"/>
+      <c r="AF6" s="7"/>
       <c r="AG6" s="11"/>
-      <c r="AH6" s="7"/>
-    </row>
-    <row r="7" spans="1:34" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+    </row>
+    <row r="7" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>68</v>
+        <v>242</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -2073,20 +2188,22 @@
       <c r="AF7" s="16"/>
       <c r="AG7" s="16"/>
       <c r="AH7" s="16"/>
-    </row>
-    <row r="8" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI7" s="16"/>
+      <c r="AJ7" s="16"/>
+    </row>
+    <row r="8" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="8" t="s">
@@ -2116,7 +2233,7 @@
         <v>0.25</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="X8" s="10"/>
       <c r="Y8" s="8"/>
@@ -2126,20 +2243,22 @@
       <c r="AC8" s="7"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="7"/>
-      <c r="AF8" s="11"/>
+      <c r="AF8" s="7"/>
       <c r="AG8" s="11"/>
-      <c r="AH8" s="7"/>
-    </row>
-    <row r="9" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH8" s="11"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+    </row>
+    <row r="9" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>17</v>
@@ -2182,23 +2301,25 @@
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="7"/>
-      <c r="AF9" s="11"/>
+      <c r="AF9" s="7"/>
       <c r="AG9" s="11"/>
-      <c r="AH9" s="7"/>
-    </row>
-    <row r="10" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH9" s="11"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+    </row>
+    <row r="10" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="8" t="s">
@@ -2228,7 +2349,7 @@
         <v>0.25</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
@@ -2238,25 +2359,27 @@
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
       <c r="AE10" s="7"/>
-      <c r="AF10" s="11"/>
+      <c r="AF10" s="7"/>
       <c r="AG10" s="11"/>
-      <c r="AH10" s="7"/>
-    </row>
-    <row r="11" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="AH10" s="11"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+    </row>
+    <row r="11" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E11" s="64" t="s">
-        <v>216</v>
-      </c>
-      <c r="F11" s="64"/>
+        <v>188</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>215</v>
+      </c>
+      <c r="F11" s="51"/>
       <c r="G11" s="8" t="s">
         <v>36</v>
       </c>
@@ -2268,8 +2391,8 @@
       <c r="M11" s="43"/>
       <c r="N11" s="43"/>
       <c r="O11" s="43"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
+      <c r="P11" s="52"/>
+      <c r="Q11" s="52"/>
       <c r="R11" s="11"/>
       <c r="S11" s="10">
         <v>1</v>
@@ -2284,7 +2407,7 @@
         <v>0.25</v>
       </c>
       <c r="W11" s="44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X11" s="44"/>
       <c r="Y11" s="43"/>
@@ -2292,25 +2415,27 @@
       <c r="AA11" s="11"/>
       <c r="AB11" s="11"/>
       <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
+      <c r="AD11" s="7"/>
       <c r="AE11" s="11"/>
       <c r="AF11" s="11"/>
       <c r="AG11" s="11"/>
       <c r="AH11" s="11"/>
-    </row>
-    <row r="12" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI11" s="11"/>
+      <c r="AJ11" s="7"/>
+    </row>
+    <row r="12" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="43" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E12" s="64" t="s">
-        <v>217</v>
+        <v>188</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>216</v>
       </c>
       <c r="F12" s="43"/>
       <c r="G12" s="8" t="s">
@@ -2324,8 +2449,8 @@
       <c r="M12" s="43"/>
       <c r="N12" s="43"/>
       <c r="O12" s="43"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
       <c r="R12" s="11"/>
       <c r="S12" s="10">
         <v>1</v>
@@ -2340,7 +2465,7 @@
         <v>0.25</v>
       </c>
       <c r="W12" s="44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X12" s="44"/>
       <c r="Y12" s="43"/>
@@ -2348,24 +2473,26 @@
       <c r="AA12" s="11"/>
       <c r="AB12" s="11"/>
       <c r="AC12" s="11"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="11"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="43"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="11"/>
       <c r="AH12" s="11"/>
-    </row>
-    <row r="13" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI12" s="11"/>
+      <c r="AJ12" s="7"/>
+    </row>
+    <row r="13" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E13" s="64" t="s">
+        <v>188</v>
+      </c>
+      <c r="E13" s="51" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="43"/>
@@ -2380,8 +2507,8 @@
       <c r="M13" s="43"/>
       <c r="N13" s="43"/>
       <c r="O13" s="43"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
+      <c r="P13" s="52"/>
+      <c r="Q13" s="52"/>
       <c r="R13" s="11"/>
       <c r="S13" s="10">
         <v>1</v>
@@ -2404,24 +2531,26 @@
       <c r="AA13" s="11"/>
       <c r="AB13" s="11"/>
       <c r="AC13" s="11"/>
-      <c r="AD13" s="43"/>
-      <c r="AE13" s="11"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="43"/>
       <c r="AF13" s="11"/>
       <c r="AG13" s="11"/>
       <c r="AH13" s="11"/>
-    </row>
-    <row r="14" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI13" s="11"/>
+      <c r="AJ13" s="7"/>
+    </row>
+    <row r="14" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="64" t="s">
+        <v>188</v>
+      </c>
+      <c r="E14" s="51" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="43"/>
@@ -2436,8 +2565,8 @@
       <c r="M14" s="43"/>
       <c r="N14" s="43"/>
       <c r="O14" s="43"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="65"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
       <c r="R14" s="11"/>
       <c r="S14" s="10">
         <v>1</v>
@@ -2460,25 +2589,27 @@
       <c r="AA14" s="11"/>
       <c r="AB14" s="11"/>
       <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
+      <c r="AD14" s="7"/>
       <c r="AE14" s="11"/>
       <c r="AF14" s="11"/>
       <c r="AG14" s="11"/>
       <c r="AH14" s="11"/>
-    </row>
-    <row r="15" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI14" s="11"/>
+      <c r="AJ14" s="7"/>
+    </row>
+    <row r="15" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E15" s="64" t="s">
-        <v>149</v>
+      <c r="E15" s="51" t="s">
+        <v>148</v>
       </c>
       <c r="F15" s="43"/>
       <c r="G15" s="8" t="s">
@@ -2492,8 +2623,8 @@
       <c r="M15" s="43"/>
       <c r="N15" s="43"/>
       <c r="O15" s="43"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
       <c r="R15" s="11"/>
       <c r="S15" s="10">
         <v>1</v>
@@ -2508,7 +2639,7 @@
         <v>0.25</v>
       </c>
       <c r="W15" s="44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X15" s="44"/>
       <c r="Y15" s="43"/>
@@ -2516,25 +2647,27 @@
       <c r="AA15" s="11"/>
       <c r="AB15" s="11"/>
       <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
+      <c r="AD15" s="7"/>
       <c r="AE15" s="11"/>
       <c r="AF15" s="11"/>
       <c r="AG15" s="11"/>
       <c r="AH15" s="11"/>
-    </row>
-    <row r="16" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="7"/>
+    </row>
+    <row r="16" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43"/>
       <c r="B16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>166</v>
+        <v>188</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>165</v>
       </c>
       <c r="F16" s="43"/>
       <c r="G16" s="8" t="s">
@@ -2548,8 +2681,8 @@
       <c r="M16" s="43"/>
       <c r="N16" s="43"/>
       <c r="O16" s="43"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="65"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
       <c r="R16" s="11"/>
       <c r="S16" s="10">
         <v>1</v>
@@ -2564,7 +2697,7 @@
         <v>0.25</v>
       </c>
       <c r="W16" s="44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X16" s="44"/>
       <c r="Y16" s="43"/>
@@ -2572,25 +2705,27 @@
       <c r="AA16" s="11"/>
       <c r="AB16" s="11"/>
       <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
+      <c r="AD16" s="34"/>
       <c r="AE16" s="11"/>
       <c r="AF16" s="11"/>
       <c r="AG16" s="11"/>
       <c r="AH16" s="11"/>
-    </row>
-    <row r="17" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI16" s="11"/>
+      <c r="AJ16" s="34"/>
+    </row>
+    <row r="17" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43"/>
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E17" s="64" t="s">
-        <v>218</v>
+        <v>188</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>217</v>
       </c>
       <c r="F17" s="43"/>
       <c r="G17" s="8" t="s">
@@ -2604,8 +2739,8 @@
       <c r="M17" s="43"/>
       <c r="N17" s="43"/>
       <c r="O17" s="43"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="65"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
       <c r="R17" s="11"/>
       <c r="S17" s="10">
         <v>1</v>
@@ -2620,7 +2755,7 @@
         <v>0.25</v>
       </c>
       <c r="W17" s="44" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X17" s="44"/>
       <c r="Y17" s="43"/>
@@ -2628,25 +2763,27 @@
       <c r="AA17" s="11"/>
       <c r="AB17" s="11"/>
       <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
+      <c r="AD17" s="7"/>
       <c r="AE17" s="11"/>
       <c r="AF17" s="11"/>
       <c r="AG17" s="11"/>
       <c r="AH17" s="11"/>
-    </row>
-    <row r="18" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI17" s="11"/>
+      <c r="AJ17" s="7"/>
+    </row>
+    <row r="18" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43"/>
       <c r="B18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E18" s="64" t="s">
-        <v>219</v>
+        <v>188</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>218</v>
       </c>
       <c r="F18" s="43"/>
       <c r="G18" s="8" t="s">
@@ -2660,8 +2797,8 @@
       <c r="M18" s="43"/>
       <c r="N18" s="43"/>
       <c r="O18" s="43"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="65"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
       <c r="R18" s="11"/>
       <c r="S18" s="10">
         <v>1</v>
@@ -2676,7 +2813,7 @@
         <v>0.25</v>
       </c>
       <c r="W18" s="44" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X18" s="44"/>
       <c r="Y18" s="43"/>
@@ -2684,22 +2821,24 @@
       <c r="AA18" s="11"/>
       <c r="AB18" s="11"/>
       <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
+      <c r="AD18" s="7"/>
       <c r="AE18" s="11"/>
       <c r="AF18" s="11"/>
       <c r="AG18" s="11"/>
       <c r="AH18" s="11"/>
-    </row>
-    <row r="19" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI18" s="11"/>
+      <c r="AJ18" s="7"/>
+    </row>
+    <row r="19" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E19" s="21" t="s">
         <v>40</v>
@@ -2742,25 +2881,27 @@
       <c r="AC19" s="7"/>
       <c r="AD19" s="7"/>
       <c r="AE19" s="7"/>
-      <c r="AF19" s="11"/>
+      <c r="AF19" s="7"/>
       <c r="AG19" s="11"/>
-      <c r="AH19" s="7"/>
-    </row>
-    <row r="20" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7"/>
+    </row>
+    <row r="20" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E20" s="68" t="s">
-        <v>157</v>
-      </c>
-      <c r="F20" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20" s="55"/>
       <c r="G20" s="5" t="s">
         <v>38</v>
       </c>
@@ -2774,49 +2915,51 @@
       <c r="O20" s="5"/>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="70">
+      <c r="R20" s="56"/>
+      <c r="S20" s="57">
         <v>2.25</v>
       </c>
-      <c r="T20" s="70">
+      <c r="T20" s="57">
         <v>10.5</v>
       </c>
-      <c r="U20" s="70">
-        <v>0</v>
-      </c>
-      <c r="V20" s="70">
+      <c r="U20" s="57">
+        <v>0</v>
+      </c>
+      <c r="V20" s="57">
         <v>0.25</v>
       </c>
-      <c r="W20" s="70" t="s">
-        <v>157</v>
-      </c>
-      <c r="X20" s="70"/>
+      <c r="W20" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="X20" s="57"/>
       <c r="Y20" s="5"/>
-      <c r="Z20" s="69"/>
+      <c r="Z20" s="56"/>
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
       <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
+      <c r="AD20" s="13"/>
       <c r="AE20" s="7"/>
-      <c r="AF20" s="11"/>
+      <c r="AF20" s="7"/>
       <c r="AG20" s="11"/>
-      <c r="AH20" s="7"/>
-    </row>
-    <row r="21" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH20" s="11"/>
+      <c r="AI20" s="7"/>
+      <c r="AJ20" s="13"/>
+    </row>
+    <row r="21" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E21" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="F21" s="55"/>
       <c r="G21" s="5" t="s">
         <v>38</v>
       </c>
@@ -2831,48 +2974,50 @@
       <c r="P21" s="19"/>
       <c r="Q21" s="19"/>
       <c r="R21" s="5"/>
-      <c r="S21" s="70">
+      <c r="S21" s="57">
         <v>2.25</v>
       </c>
-      <c r="T21" s="70">
+      <c r="T21" s="57">
         <v>10</v>
       </c>
-      <c r="U21" s="70">
-        <v>0</v>
-      </c>
-      <c r="V21" s="70">
+      <c r="U21" s="57">
+        <v>0</v>
+      </c>
+      <c r="V21" s="57">
         <v>0.25</v>
       </c>
       <c r="W21" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="X21" s="70"/>
+        <v>149</v>
+      </c>
+      <c r="X21" s="57"/>
       <c r="Y21" s="5"/>
-      <c r="Z21" s="69"/>
+      <c r="Z21" s="56"/>
       <c r="AA21" s="11"/>
       <c r="AB21" s="11"/>
       <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
+      <c r="AD21" s="13"/>
       <c r="AE21" s="7"/>
-      <c r="AF21" s="11"/>
+      <c r="AF21" s="7"/>
       <c r="AG21" s="11"/>
-      <c r="AH21" s="7"/>
-    </row>
-    <row r="22" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH21" s="11"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="13"/>
+    </row>
+    <row r="22" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E22" s="68" t="s">
-        <v>231</v>
-      </c>
-      <c r="F22" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E22" s="55" t="s">
+        <v>230</v>
+      </c>
+      <c r="F22" s="55"/>
       <c r="G22" s="5" t="s">
         <v>38</v>
       </c>
@@ -2887,48 +3032,50 @@
       <c r="P22" s="19"/>
       <c r="Q22" s="19"/>
       <c r="R22" s="5"/>
-      <c r="S22" s="70">
+      <c r="S22" s="57">
         <v>2.25</v>
       </c>
-      <c r="T22" s="70">
+      <c r="T22" s="57">
         <v>9.5</v>
       </c>
-      <c r="U22" s="70">
-        <v>0</v>
-      </c>
-      <c r="V22" s="70">
+      <c r="U22" s="57">
+        <v>0</v>
+      </c>
+      <c r="V22" s="57">
         <v>0.25</v>
       </c>
       <c r="W22" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="X22" s="70"/>
+        <v>219</v>
+      </c>
+      <c r="X22" s="57"/>
       <c r="Y22" s="5"/>
-      <c r="Z22" s="69"/>
+      <c r="Z22" s="56"/>
       <c r="AA22" s="11"/>
       <c r="AB22" s="11"/>
       <c r="AC22" s="7"/>
-      <c r="AD22" s="7"/>
+      <c r="AD22" s="13"/>
       <c r="AE22" s="7"/>
-      <c r="AF22" s="11"/>
+      <c r="AF22" s="7"/>
       <c r="AG22" s="11"/>
-      <c r="AH22" s="7"/>
-    </row>
-    <row r="23" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH22" s="11"/>
+      <c r="AI22" s="7"/>
+      <c r="AJ22" s="13"/>
+    </row>
+    <row r="23" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E23" s="68" t="s">
-        <v>221</v>
-      </c>
-      <c r="F23" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E23" s="55" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="55"/>
       <c r="G23" s="5" t="s">
         <v>38</v>
       </c>
@@ -2943,48 +3090,50 @@
       <c r="P23" s="19"/>
       <c r="Q23" s="19"/>
       <c r="R23" s="5"/>
-      <c r="S23" s="70">
+      <c r="S23" s="57">
         <v>2.25</v>
       </c>
-      <c r="T23" s="70">
+      <c r="T23" s="57">
         <v>9</v>
       </c>
-      <c r="U23" s="70">
-        <v>0</v>
-      </c>
-      <c r="V23" s="70">
+      <c r="U23" s="57">
+        <v>0</v>
+      </c>
+      <c r="V23" s="57">
         <v>0.25</v>
       </c>
       <c r="W23" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="X23" s="70"/>
+        <v>220</v>
+      </c>
+      <c r="X23" s="57"/>
       <c r="Y23" s="5"/>
-      <c r="Z23" s="69"/>
+      <c r="Z23" s="56"/>
       <c r="AA23" s="11"/>
       <c r="AB23" s="11"/>
       <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
+      <c r="AD23" s="13"/>
       <c r="AE23" s="7"/>
-      <c r="AF23" s="11"/>
+      <c r="AF23" s="7"/>
       <c r="AG23" s="11"/>
-      <c r="AH23" s="7"/>
-    </row>
-    <row r="24" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH23" s="11"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="13"/>
+    </row>
+    <row r="24" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E24" s="68" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="55"/>
       <c r="G24" s="5" t="s">
         <v>38</v>
       </c>
@@ -2999,48 +3148,50 @@
       <c r="P24" s="19"/>
       <c r="Q24" s="19"/>
       <c r="R24" s="5"/>
-      <c r="S24" s="70">
+      <c r="S24" s="57">
         <v>2.25</v>
       </c>
-      <c r="T24" s="70">
+      <c r="T24" s="57">
         <v>8.5</v>
       </c>
-      <c r="U24" s="70">
-        <v>0</v>
-      </c>
-      <c r="V24" s="70">
+      <c r="U24" s="57">
+        <v>0</v>
+      </c>
+      <c r="V24" s="57">
         <v>0.25</v>
       </c>
       <c r="W24" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="X24" s="70"/>
+        <v>150</v>
+      </c>
+      <c r="X24" s="57"/>
       <c r="Y24" s="5"/>
-      <c r="Z24" s="69"/>
+      <c r="Z24" s="56"/>
       <c r="AA24" s="11"/>
       <c r="AB24" s="11"/>
       <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
+      <c r="AD24" s="13"/>
       <c r="AE24" s="7"/>
-      <c r="AF24" s="11"/>
+      <c r="AF24" s="7"/>
       <c r="AG24" s="11"/>
-      <c r="AH24" s="7"/>
-    </row>
-    <row r="25" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH24" s="11"/>
+      <c r="AI24" s="7"/>
+      <c r="AJ24" s="13"/>
+    </row>
+    <row r="25" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E25" s="68" t="s">
-        <v>152</v>
-      </c>
-      <c r="F25" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E25" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="55"/>
       <c r="G25" s="5" t="s">
         <v>38</v>
       </c>
@@ -3055,48 +3206,50 @@
       <c r="P25" s="19"/>
       <c r="Q25" s="19"/>
       <c r="R25" s="5"/>
-      <c r="S25" s="70">
+      <c r="S25" s="57">
         <v>2.25</v>
       </c>
-      <c r="T25" s="70">
+      <c r="T25" s="57">
         <v>8</v>
       </c>
-      <c r="U25" s="70">
-        <v>0</v>
-      </c>
-      <c r="V25" s="70">
+      <c r="U25" s="57">
+        <v>0</v>
+      </c>
+      <c r="V25" s="57">
         <v>0.25</v>
       </c>
       <c r="W25" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="X25" s="70"/>
+        <v>151</v>
+      </c>
+      <c r="X25" s="57"/>
       <c r="Y25" s="5"/>
-      <c r="Z25" s="69"/>
+      <c r="Z25" s="56"/>
       <c r="AA25" s="11"/>
       <c r="AB25" s="11"/>
       <c r="AC25" s="7"/>
-      <c r="AD25" s="7"/>
+      <c r="AD25" s="13"/>
       <c r="AE25" s="7"/>
-      <c r="AF25" s="11"/>
+      <c r="AF25" s="7"/>
       <c r="AG25" s="11"/>
-      <c r="AH25" s="7"/>
-    </row>
-    <row r="26" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH25" s="11"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="13"/>
+    </row>
+    <row r="26" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E26" s="68" t="s">
-        <v>222</v>
-      </c>
-      <c r="F26" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E26" s="55" t="s">
+        <v>221</v>
+      </c>
+      <c r="F26" s="55"/>
       <c r="G26" s="5" t="s">
         <v>38</v>
       </c>
@@ -3111,48 +3264,50 @@
       <c r="P26" s="19"/>
       <c r="Q26" s="19"/>
       <c r="R26" s="5"/>
-      <c r="S26" s="70">
+      <c r="S26" s="57">
         <v>2.25</v>
       </c>
-      <c r="T26" s="70">
+      <c r="T26" s="57">
         <v>7.5</v>
       </c>
-      <c r="U26" s="70">
-        <v>0</v>
-      </c>
-      <c r="V26" s="70">
+      <c r="U26" s="57">
+        <v>0</v>
+      </c>
+      <c r="V26" s="57">
         <v>0.25</v>
       </c>
       <c r="W26" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="X26" s="70"/>
+        <v>221</v>
+      </c>
+      <c r="X26" s="57"/>
       <c r="Y26" s="5"/>
-      <c r="Z26" s="69"/>
+      <c r="Z26" s="56"/>
       <c r="AA26" s="11"/>
       <c r="AB26" s="11"/>
       <c r="AC26" s="7"/>
-      <c r="AD26" s="7"/>
+      <c r="AD26" s="13"/>
       <c r="AE26" s="7"/>
-      <c r="AF26" s="11"/>
+      <c r="AF26" s="7"/>
       <c r="AG26" s="11"/>
-      <c r="AH26" s="7"/>
-    </row>
-    <row r="27" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH26" s="11"/>
+      <c r="AI26" s="7"/>
+      <c r="AJ26" s="13"/>
+    </row>
+    <row r="27" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="68"/>
+      <c r="F27" s="55"/>
       <c r="G27" s="5" t="s">
         <v>38</v>
       </c>
@@ -3167,48 +3322,50 @@
       <c r="P27" s="19"/>
       <c r="Q27" s="19"/>
       <c r="R27" s="5"/>
-      <c r="S27" s="70">
+      <c r="S27" s="57">
         <v>2.25</v>
       </c>
-      <c r="T27" s="70">
+      <c r="T27" s="57">
         <v>7</v>
       </c>
-      <c r="U27" s="70">
-        <v>0</v>
-      </c>
-      <c r="V27" s="70">
+      <c r="U27" s="57">
+        <v>0</v>
+      </c>
+      <c r="V27" s="57">
         <v>0.25</v>
       </c>
       <c r="W27" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="X27" s="70"/>
+      <c r="X27" s="57"/>
       <c r="Y27" s="5"/>
-      <c r="Z27" s="69"/>
+      <c r="Z27" s="56"/>
       <c r="AA27" s="11"/>
       <c r="AB27" s="11"/>
       <c r="AC27" s="7"/>
-      <c r="AD27" s="7"/>
+      <c r="AD27" s="13"/>
       <c r="AE27" s="7"/>
-      <c r="AF27" s="11"/>
+      <c r="AF27" s="7"/>
       <c r="AG27" s="11"/>
-      <c r="AH27" s="7"/>
-    </row>
-    <row r="28" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH27" s="11"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="13"/>
+    </row>
+    <row r="28" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>155</v>
-      </c>
-      <c r="F28" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="55"/>
       <c r="G28" s="5" t="s">
         <v>38</v>
       </c>
@@ -3223,46 +3380,48 @@
       <c r="P28" s="19"/>
       <c r="Q28" s="19"/>
       <c r="R28" s="5"/>
-      <c r="S28" s="70">
+      <c r="S28" s="57">
         <v>2.25</v>
       </c>
-      <c r="T28" s="70">
+      <c r="T28" s="57">
         <v>6.5</v>
       </c>
-      <c r="U28" s="70">
-        <v>0</v>
-      </c>
-      <c r="V28" s="70">
+      <c r="U28" s="57">
+        <v>0</v>
+      </c>
+      <c r="V28" s="57">
         <v>0.25</v>
       </c>
       <c r="W28" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="X28" s="70"/>
+        <v>154</v>
+      </c>
+      <c r="X28" s="57"/>
       <c r="Y28" s="5"/>
-      <c r="Z28" s="69"/>
+      <c r="Z28" s="56"/>
       <c r="AA28" s="11"/>
       <c r="AB28" s="11"/>
       <c r="AC28" s="7"/>
-      <c r="AD28" s="7"/>
+      <c r="AD28" s="13"/>
       <c r="AE28" s="7"/>
-      <c r="AF28" s="11"/>
+      <c r="AF28" s="7"/>
       <c r="AG28" s="11"/>
-      <c r="AH28" s="7"/>
-    </row>
-    <row r="29" spans="1:34" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH28" s="11"/>
+      <c r="AI28" s="7"/>
+      <c r="AJ28" s="13"/>
+    </row>
+    <row r="29" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="50"/>
       <c r="B29" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E29" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F29" s="49"/>
       <c r="G29" s="35" t="s">
@@ -3292,7 +3451,7 @@
         <v>0.25</v>
       </c>
       <c r="W29" s="50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X29" s="45"/>
       <c r="Y29" s="35"/>
@@ -3300,25 +3459,27 @@
       <c r="AA29" s="11"/>
       <c r="AB29" s="11"/>
       <c r="AC29" s="11"/>
-      <c r="AD29" s="11"/>
+      <c r="AD29" s="13"/>
       <c r="AE29" s="11"/>
       <c r="AF29" s="11"/>
       <c r="AG29" s="11"/>
       <c r="AH29" s="11"/>
-    </row>
-    <row r="30" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AI29" s="11"/>
+      <c r="AJ29" s="13"/>
+    </row>
+    <row r="30" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
       <c r="B30" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E30" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F30" s="49"/>
       <c r="G30" s="35" t="s">
@@ -3348,7 +3509,7 @@
         <v>0.25</v>
       </c>
       <c r="W30" s="50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X30" s="45"/>
       <c r="Y30" s="35"/>
@@ -3356,25 +3517,27 @@
       <c r="AA30" s="11"/>
       <c r="AB30" s="11"/>
       <c r="AC30" s="7"/>
-      <c r="AD30" s="7"/>
+      <c r="AD30" s="13"/>
       <c r="AE30" s="7"/>
-      <c r="AF30" s="11"/>
+      <c r="AF30" s="7"/>
       <c r="AG30" s="11"/>
-      <c r="AH30" s="7"/>
-    </row>
-    <row r="31" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH30" s="11"/>
+      <c r="AI30" s="7"/>
+      <c r="AJ30" s="13"/>
+    </row>
+    <row r="31" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
       <c r="B31" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E31" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F31" s="49"/>
       <c r="G31" s="35" t="s">
@@ -3404,7 +3567,7 @@
         <v>0.25</v>
       </c>
       <c r="W31" s="50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X31" s="45"/>
       <c r="Y31" s="35"/>
@@ -3412,25 +3575,27 @@
       <c r="AA31" s="11"/>
       <c r="AB31" s="11"/>
       <c r="AC31" s="7"/>
-      <c r="AD31" s="7"/>
+      <c r="AD31" s="13"/>
       <c r="AE31" s="7"/>
-      <c r="AF31" s="11"/>
+      <c r="AF31" s="7"/>
       <c r="AG31" s="11"/>
-      <c r="AH31" s="7"/>
-    </row>
-    <row r="32" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="13"/>
+    </row>
+    <row r="32" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="50"/>
       <c r="B32" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E32" s="49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F32" s="49"/>
       <c r="G32" s="35" t="s">
@@ -3460,7 +3625,7 @@
         <v>0.25</v>
       </c>
       <c r="W32" s="50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X32" s="45"/>
       <c r="Y32" s="35"/>
@@ -3468,25 +3633,27 @@
       <c r="AA32" s="11"/>
       <c r="AB32" s="11"/>
       <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
+      <c r="AD32" s="13"/>
       <c r="AE32" s="7"/>
-      <c r="AF32" s="11"/>
+      <c r="AF32" s="7"/>
       <c r="AG32" s="11"/>
-      <c r="AH32" s="7"/>
-    </row>
-    <row r="33" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH32" s="11"/>
+      <c r="AI32" s="7"/>
+      <c r="AJ32" s="13"/>
+    </row>
+    <row r="33" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="50"/>
       <c r="B33" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F33" s="49"/>
       <c r="G33" s="35" t="s">
@@ -3516,7 +3683,7 @@
         <v>0.25</v>
       </c>
       <c r="W33" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X33" s="45"/>
       <c r="Y33" s="35"/>
@@ -3524,25 +3691,27 @@
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
       <c r="AC33" s="7"/>
-      <c r="AD33" s="7"/>
+      <c r="AD33" s="13"/>
       <c r="AE33" s="7"/>
-      <c r="AF33" s="11"/>
+      <c r="AF33" s="7"/>
       <c r="AG33" s="11"/>
-      <c r="AH33" s="7"/>
-    </row>
-    <row r="34" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH33" s="11"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="13"/>
+    </row>
+    <row r="34" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50"/>
       <c r="B34" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E34" s="49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F34" s="49"/>
       <c r="G34" s="35" t="s">
@@ -3572,7 +3741,7 @@
         <v>0.25</v>
       </c>
       <c r="W34" s="50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="X34" s="45"/>
       <c r="Y34" s="35"/>
@@ -3580,25 +3749,27 @@
       <c r="AA34" s="11"/>
       <c r="AB34" s="11"/>
       <c r="AC34" s="7"/>
-      <c r="AD34" s="7"/>
+      <c r="AD34" s="13"/>
       <c r="AE34" s="7"/>
-      <c r="AF34" s="11"/>
+      <c r="AF34" s="7"/>
       <c r="AG34" s="11"/>
-      <c r="AH34" s="7"/>
-    </row>
-    <row r="35" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH34" s="11"/>
+      <c r="AI34" s="7"/>
+      <c r="AJ34" s="13"/>
+    </row>
+    <row r="35" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="50"/>
       <c r="B35" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E35" s="49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F35" s="49"/>
       <c r="G35" s="35" t="s">
@@ -3628,7 +3799,7 @@
         <v>0.25</v>
       </c>
       <c r="W35" s="50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="X35" s="45"/>
       <c r="Y35" s="35"/>
@@ -3636,25 +3807,27 @@
       <c r="AA35" s="11"/>
       <c r="AB35" s="11"/>
       <c r="AC35" s="7"/>
-      <c r="AD35" s="7"/>
+      <c r="AD35" s="13"/>
       <c r="AE35" s="7"/>
-      <c r="AF35" s="11"/>
+      <c r="AF35" s="7"/>
       <c r="AG35" s="11"/>
-      <c r="AH35" s="7"/>
-    </row>
-    <row r="36" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH35" s="11"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="13"/>
+    </row>
+    <row r="36" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="50"/>
       <c r="B36" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F36" s="49"/>
       <c r="G36" s="35" t="s">
@@ -3684,7 +3857,7 @@
         <v>0.25</v>
       </c>
       <c r="W36" s="50" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="X36" s="45"/>
       <c r="Y36" s="35"/>
@@ -3692,25 +3865,27 @@
       <c r="AA36" s="11"/>
       <c r="AB36" s="11"/>
       <c r="AC36" s="7"/>
-      <c r="AD36" s="7"/>
+      <c r="AD36" s="13"/>
       <c r="AE36" s="7"/>
-      <c r="AF36" s="11"/>
+      <c r="AF36" s="7"/>
       <c r="AG36" s="11"/>
-      <c r="AH36" s="7"/>
-    </row>
-    <row r="37" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH36" s="11"/>
+      <c r="AI36" s="7"/>
+      <c r="AJ36" s="13"/>
+    </row>
+    <row r="37" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="50"/>
       <c r="B37" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E37" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F37" s="49"/>
       <c r="G37" s="35" t="s">
@@ -3740,7 +3915,7 @@
         <v>0.25</v>
       </c>
       <c r="W37" s="50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="X37" s="45"/>
       <c r="Y37" s="35"/>
@@ -3748,25 +3923,27 @@
       <c r="AA37" s="11"/>
       <c r="AB37" s="11"/>
       <c r="AC37" s="7"/>
-      <c r="AD37" s="7"/>
+      <c r="AD37" s="13"/>
       <c r="AE37" s="7"/>
-      <c r="AF37" s="11"/>
+      <c r="AF37" s="7"/>
       <c r="AG37" s="11"/>
-      <c r="AH37" s="7"/>
-    </row>
-    <row r="38" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH37" s="11"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="13"/>
+    </row>
+    <row r="38" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50"/>
       <c r="B38" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E38" s="49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F38" s="49"/>
       <c r="G38" s="35" t="s">
@@ -3796,7 +3973,7 @@
         <v>0.25</v>
       </c>
       <c r="W38" s="50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X38" s="45"/>
       <c r="Y38" s="35"/>
@@ -3804,25 +3981,27 @@
       <c r="AA38" s="11"/>
       <c r="AB38" s="11"/>
       <c r="AC38" s="7"/>
-      <c r="AD38" s="7"/>
+      <c r="AD38" s="13"/>
       <c r="AE38" s="7"/>
-      <c r="AF38" s="11"/>
+      <c r="AF38" s="7"/>
       <c r="AG38" s="11"/>
-      <c r="AH38" s="7"/>
-    </row>
-    <row r="39" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH38" s="11"/>
+      <c r="AI38" s="7"/>
+      <c r="AJ38" s="13"/>
+    </row>
+    <row r="39" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50"/>
       <c r="B39" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E39" s="49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F39" s="49"/>
       <c r="G39" s="35" t="s">
@@ -3852,7 +4031,7 @@
         <v>0.25</v>
       </c>
       <c r="W39" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X39" s="45"/>
       <c r="Y39" s="35"/>
@@ -3860,22 +4039,24 @@
       <c r="AA39" s="11"/>
       <c r="AB39" s="11"/>
       <c r="AC39" s="7"/>
-      <c r="AD39" s="7"/>
+      <c r="AD39" s="13"/>
       <c r="AE39" s="7"/>
-      <c r="AF39" s="11"/>
+      <c r="AF39" s="7"/>
       <c r="AG39" s="11"/>
-      <c r="AH39" s="7"/>
-    </row>
-    <row r="40" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH39" s="11"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="13"/>
+    </row>
+    <row r="40" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50"/>
       <c r="B40" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E40" s="49" t="s">
         <v>18</v>
@@ -3916,27 +4097,29 @@
       <c r="AA40" s="11"/>
       <c r="AB40" s="11"/>
       <c r="AC40" s="7"/>
-      <c r="AD40" s="7"/>
+      <c r="AD40" s="13"/>
       <c r="AE40" s="7"/>
-      <c r="AF40" s="11"/>
+      <c r="AF40" s="7"/>
       <c r="AG40" s="11"/>
-      <c r="AH40" s="7"/>
-    </row>
-    <row r="41" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH40" s="11"/>
+      <c r="AI40" s="7"/>
+      <c r="AJ40" s="13"/>
+    </row>
+    <row r="41" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
       <c r="B41" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E41" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="F41" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="F41" s="55"/>
       <c r="G41" s="5" t="s">
         <v>38</v>
       </c>
@@ -3951,48 +4134,50 @@
       <c r="P41" s="19"/>
       <c r="Q41" s="19"/>
       <c r="R41" s="5"/>
-      <c r="S41" s="70">
+      <c r="S41" s="57">
         <v>4.75</v>
       </c>
-      <c r="T41" s="70">
+      <c r="T41" s="57">
         <v>10.5</v>
       </c>
-      <c r="U41" s="70">
-        <v>0</v>
-      </c>
-      <c r="V41" s="70">
+      <c r="U41" s="57">
+        <v>0</v>
+      </c>
+      <c r="V41" s="57">
         <v>0.25</v>
       </c>
       <c r="W41" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="X41" s="70"/>
+        <v>163</v>
+      </c>
+      <c r="X41" s="57"/>
       <c r="Y41" s="5"/>
-      <c r="Z41" s="69"/>
+      <c r="Z41" s="56"/>
       <c r="AA41" s="11"/>
       <c r="AB41" s="11"/>
       <c r="AC41" s="7"/>
-      <c r="AD41" s="7"/>
+      <c r="AD41" s="13"/>
       <c r="AE41" s="7"/>
-      <c r="AF41" s="11"/>
+      <c r="AF41" s="7"/>
       <c r="AG41" s="11"/>
-      <c r="AH41" s="7"/>
-    </row>
-    <row r="42" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH41" s="11"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="13"/>
+    </row>
+    <row r="42" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
       <c r="B42" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E42" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="F42" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E42" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" s="55"/>
       <c r="G42" s="5" t="s">
         <v>38</v>
       </c>
@@ -4007,48 +4192,50 @@
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
       <c r="R42" s="5"/>
-      <c r="S42" s="70">
+      <c r="S42" s="57">
         <v>4.75</v>
       </c>
-      <c r="T42" s="70">
+      <c r="T42" s="57">
         <v>10</v>
       </c>
-      <c r="U42" s="70">
-        <v>0</v>
-      </c>
-      <c r="V42" s="70">
+      <c r="U42" s="57">
+        <v>0</v>
+      </c>
+      <c r="V42" s="57">
         <v>0.25</v>
       </c>
       <c r="W42" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="X42" s="70"/>
+        <v>162</v>
+      </c>
+      <c r="X42" s="57"/>
       <c r="Y42" s="5"/>
-      <c r="Z42" s="69"/>
+      <c r="Z42" s="56"/>
       <c r="AA42" s="11"/>
       <c r="AB42" s="11"/>
       <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
+      <c r="AD42" s="13"/>
       <c r="AE42" s="7"/>
-      <c r="AF42" s="11"/>
+      <c r="AF42" s="7"/>
       <c r="AG42" s="11"/>
-      <c r="AH42" s="7"/>
-    </row>
-    <row r="43" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH42" s="11"/>
+      <c r="AI42" s="7"/>
+      <c r="AJ42" s="13"/>
+    </row>
+    <row r="43" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E43" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="68"/>
+      <c r="F43" s="55"/>
       <c r="G43" s="5" t="s">
         <v>38</v>
       </c>
@@ -4063,48 +4250,50 @@
       <c r="P43" s="19"/>
       <c r="Q43" s="19"/>
       <c r="R43" s="5"/>
-      <c r="S43" s="70">
+      <c r="S43" s="57">
         <v>4.75</v>
       </c>
-      <c r="T43" s="70">
+      <c r="T43" s="57">
         <v>9.5</v>
       </c>
-      <c r="U43" s="70">
-        <v>0</v>
-      </c>
-      <c r="V43" s="70">
+      <c r="U43" s="57">
+        <v>0</v>
+      </c>
+      <c r="V43" s="57">
         <v>0.25</v>
       </c>
       <c r="W43" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="X43" s="70"/>
+      <c r="X43" s="57"/>
       <c r="Y43" s="5"/>
-      <c r="Z43" s="69"/>
+      <c r="Z43" s="56"/>
       <c r="AA43" s="11"/>
       <c r="AB43" s="11"/>
       <c r="AC43" s="7"/>
-      <c r="AD43" s="7"/>
+      <c r="AD43" s="13"/>
       <c r="AE43" s="7"/>
-      <c r="AF43" s="11"/>
+      <c r="AF43" s="7"/>
       <c r="AG43" s="11"/>
-      <c r="AH43" s="7"/>
-    </row>
-    <row r="44" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH43" s="11"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="13"/>
+    </row>
+    <row r="44" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
       <c r="B44" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="F44" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E44" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="55"/>
       <c r="G44" s="5" t="s">
         <v>38</v>
       </c>
@@ -4119,48 +4308,50 @@
       <c r="P44" s="19"/>
       <c r="Q44" s="19"/>
       <c r="R44" s="5"/>
-      <c r="S44" s="70">
+      <c r="S44" s="57">
         <v>4.75</v>
       </c>
-      <c r="T44" s="70">
+      <c r="T44" s="57">
         <v>9</v>
       </c>
-      <c r="U44" s="70">
-        <v>0</v>
-      </c>
-      <c r="V44" s="70">
+      <c r="U44" s="57">
+        <v>0</v>
+      </c>
+      <c r="V44" s="57">
         <v>0.25</v>
       </c>
       <c r="W44" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="X44" s="70"/>
+        <v>164</v>
+      </c>
+      <c r="X44" s="57"/>
       <c r="Y44" s="5"/>
-      <c r="Z44" s="69"/>
+      <c r="Z44" s="56"/>
       <c r="AA44" s="11"/>
       <c r="AB44" s="11"/>
       <c r="AC44" s="7"/>
-      <c r="AD44" s="7"/>
+      <c r="AD44" s="13"/>
       <c r="AE44" s="7"/>
-      <c r="AF44" s="11"/>
+      <c r="AF44" s="7"/>
       <c r="AG44" s="11"/>
-      <c r="AH44" s="7"/>
-    </row>
-    <row r="45" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH44" s="11"/>
+      <c r="AI44" s="7"/>
+      <c r="AJ44" s="13"/>
+    </row>
+    <row r="45" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E45" s="68" t="s">
-        <v>168</v>
-      </c>
-      <c r="F45" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E45" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" s="55"/>
       <c r="G45" s="5" t="s">
         <v>38</v>
       </c>
@@ -4175,48 +4366,50 @@
       <c r="P45" s="19"/>
       <c r="Q45" s="19"/>
       <c r="R45" s="5"/>
-      <c r="S45" s="70">
+      <c r="S45" s="57">
         <v>4.75</v>
       </c>
-      <c r="T45" s="70">
+      <c r="T45" s="57">
         <v>8.5</v>
       </c>
-      <c r="U45" s="70">
-        <v>0</v>
-      </c>
-      <c r="V45" s="70">
+      <c r="U45" s="57">
+        <v>0</v>
+      </c>
+      <c r="V45" s="57">
         <v>0.25</v>
       </c>
       <c r="W45" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="X45" s="70"/>
+        <v>167</v>
+      </c>
+      <c r="X45" s="57"/>
       <c r="Y45" s="5"/>
-      <c r="Z45" s="69"/>
+      <c r="Z45" s="56"/>
       <c r="AA45" s="11"/>
       <c r="AB45" s="11"/>
       <c r="AC45" s="7"/>
-      <c r="AD45" s="7"/>
+      <c r="AD45" s="13"/>
       <c r="AE45" s="7"/>
-      <c r="AF45" s="11"/>
+      <c r="AF45" s="7"/>
       <c r="AG45" s="11"/>
-      <c r="AH45" s="7"/>
-    </row>
-    <row r="46" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH45" s="11"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="13"/>
+    </row>
+    <row r="46" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E46" s="68" t="s">
-        <v>169</v>
-      </c>
-      <c r="F46" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E46" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="F46" s="55"/>
       <c r="G46" s="5" t="s">
         <v>38</v>
       </c>
@@ -4231,48 +4424,50 @@
       <c r="P46" s="19"/>
       <c r="Q46" s="19"/>
       <c r="R46" s="5"/>
-      <c r="S46" s="70">
+      <c r="S46" s="57">
         <v>4.75</v>
       </c>
-      <c r="T46" s="70">
+      <c r="T46" s="57">
         <v>8</v>
       </c>
-      <c r="U46" s="70">
-        <v>0</v>
-      </c>
-      <c r="V46" s="70">
+      <c r="U46" s="57">
+        <v>0</v>
+      </c>
+      <c r="V46" s="57">
         <v>0.25</v>
       </c>
       <c r="W46" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="X46" s="70"/>
+        <v>168</v>
+      </c>
+      <c r="X46" s="57"/>
       <c r="Y46" s="5"/>
-      <c r="Z46" s="69"/>
+      <c r="Z46" s="56"/>
       <c r="AA46" s="11"/>
       <c r="AB46" s="11"/>
       <c r="AC46" s="7"/>
-      <c r="AD46" s="7"/>
+      <c r="AD46" s="13"/>
       <c r="AE46" s="7"/>
-      <c r="AF46" s="11"/>
+      <c r="AF46" s="7"/>
       <c r="AG46" s="11"/>
-      <c r="AH46" s="7"/>
-    </row>
-    <row r="47" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH46" s="11"/>
+      <c r="AI46" s="7"/>
+      <c r="AJ46" s="13"/>
+    </row>
+    <row r="47" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E47" s="68" t="s">
-        <v>170</v>
-      </c>
-      <c r="F47" s="68"/>
+        <v>188</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="F47" s="55"/>
       <c r="G47" s="5" t="s">
         <v>38</v>
       </c>
@@ -4287,48 +4482,50 @@
       <c r="P47" s="19"/>
       <c r="Q47" s="19"/>
       <c r="R47" s="5"/>
-      <c r="S47" s="70">
+      <c r="S47" s="57">
         <v>4.75</v>
       </c>
-      <c r="T47" s="70">
+      <c r="T47" s="57">
         <v>7.5</v>
       </c>
-      <c r="U47" s="70">
-        <v>0</v>
-      </c>
-      <c r="V47" s="70">
+      <c r="U47" s="57">
+        <v>0</v>
+      </c>
+      <c r="V47" s="57">
         <v>0.25</v>
       </c>
       <c r="W47" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="X47" s="70"/>
+        <v>169</v>
+      </c>
+      <c r="X47" s="57"/>
       <c r="Y47" s="5"/>
-      <c r="Z47" s="69"/>
+      <c r="Z47" s="56"/>
       <c r="AA47" s="11"/>
       <c r="AB47" s="11"/>
       <c r="AC47" s="7"/>
-      <c r="AD47" s="7"/>
+      <c r="AD47" s="13"/>
       <c r="AE47" s="7"/>
-      <c r="AF47" s="11"/>
+      <c r="AF47" s="7"/>
       <c r="AG47" s="11"/>
-      <c r="AH47" s="7"/>
-    </row>
-    <row r="48" spans="1:34" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH47" s="11"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="13"/>
+    </row>
+    <row r="48" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E48" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="68"/>
+      <c r="F48" s="55"/>
       <c r="G48" s="5" t="s">
         <v>38</v>
       </c>
@@ -4343,49 +4540,886 @@
       <c r="P48" s="19"/>
       <c r="Q48" s="19"/>
       <c r="R48" s="5"/>
-      <c r="S48" s="70">
+      <c r="S48" s="57">
         <v>4.75</v>
       </c>
-      <c r="T48" s="70">
+      <c r="T48" s="57">
         <v>7</v>
       </c>
-      <c r="U48" s="70">
-        <v>0</v>
-      </c>
-      <c r="V48" s="70">
+      <c r="U48" s="57">
+        <v>0</v>
+      </c>
+      <c r="V48" s="57">
         <v>0.25</v>
       </c>
       <c r="W48" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="X48" s="70"/>
+      <c r="X48" s="57"/>
       <c r="Y48" s="5"/>
-      <c r="Z48" s="69"/>
+      <c r="Z48" s="56"/>
       <c r="AA48" s="11"/>
       <c r="AB48" s="11"/>
       <c r="AC48" s="7"/>
-      <c r="AD48" s="7"/>
+      <c r="AD48" s="13"/>
       <c r="AE48" s="7"/>
-      <c r="AF48" s="11"/>
+      <c r="AF48" s="7"/>
       <c r="AG48" s="11"/>
-      <c r="AH48" s="7"/>
-    </row>
-    <row r="49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AH48" s="11"/>
+      <c r="AI48" s="7"/>
+      <c r="AJ48" s="13"/>
+    </row>
+    <row r="49" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="14"/>
+      <c r="O49" s="14"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+      <c r="W49" s="17"/>
+      <c r="X49" s="17"/>
+      <c r="Y49" s="14"/>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="16"/>
+      <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
+      <c r="AG49" s="16"/>
+      <c r="AH49" s="16"/>
+      <c r="AI49" s="16"/>
+      <c r="AJ49" s="16"/>
+    </row>
+    <row r="50" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="50"/>
+      <c r="B50" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="35"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="35"/>
+      <c r="S50" s="45">
+        <v>1</v>
+      </c>
+      <c r="T50" s="45">
+        <v>4</v>
+      </c>
+      <c r="U50" s="45">
+        <v>0</v>
+      </c>
+      <c r="V50" s="45">
+        <v>0</v>
+      </c>
+      <c r="W50" s="50"/>
+      <c r="X50" s="45"/>
+      <c r="Y50" s="35"/>
+      <c r="Z50" s="34"/>
+      <c r="AA50" s="11"/>
+      <c r="AB50" s="11"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="13"/>
+      <c r="AE50" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF50" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG50" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH50" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI50" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ50" s="13"/>
+    </row>
+    <row r="51" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="50"/>
+      <c r="B51" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="35"/>
+      <c r="S51" s="45">
+        <v>2.25</v>
+      </c>
+      <c r="T51" s="45">
+        <v>4</v>
+      </c>
+      <c r="U51" s="45">
+        <v>0</v>
+      </c>
+      <c r="V51" s="45">
+        <v>0</v>
+      </c>
+      <c r="W51" s="50"/>
+      <c r="X51" s="45"/>
+      <c r="Y51" s="35"/>
+      <c r="Z51" s="34"/>
+      <c r="AA51" s="11"/>
+      <c r="AB51" s="11"/>
+      <c r="AC51" s="7"/>
+      <c r="AD51" s="13"/>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="11"/>
+      <c r="AH51" s="11"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="13"/>
+    </row>
+    <row r="52" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="50"/>
+      <c r="B52" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="35"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="35"/>
+      <c r="S52" s="45">
+        <v>1</v>
+      </c>
+      <c r="T52" s="45">
+        <v>3.5</v>
+      </c>
+      <c r="U52" s="45">
+        <v>0</v>
+      </c>
+      <c r="V52" s="45">
+        <v>0</v>
+      </c>
+      <c r="W52" s="50"/>
+      <c r="X52" s="45"/>
+      <c r="Y52" s="35"/>
+      <c r="Z52" s="34"/>
+      <c r="AA52" s="11"/>
+      <c r="AB52" s="11"/>
+      <c r="AC52" s="7"/>
+      <c r="AD52" s="13"/>
+      <c r="AE52" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF52" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG52" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH52" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI52" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ52" s="13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="50"/>
+      <c r="B53" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="35"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="35"/>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="35"/>
+      <c r="S53" s="45">
+        <v>2.25</v>
+      </c>
+      <c r="T53" s="45">
+        <v>3.5</v>
+      </c>
+      <c r="U53" s="45">
+        <v>0</v>
+      </c>
+      <c r="V53" s="45">
+        <v>0</v>
+      </c>
+      <c r="W53" s="50"/>
+      <c r="X53" s="45"/>
+      <c r="Y53" s="35"/>
+      <c r="Z53" s="34"/>
+      <c r="AA53" s="11"/>
+      <c r="AB53" s="11"/>
+      <c r="AC53" s="7"/>
+      <c r="AD53" s="13"/>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="11"/>
+      <c r="AH53" s="11"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="13"/>
+    </row>
+    <row r="54" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="50"/>
+      <c r="B54" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="50"/>
+      <c r="R54" s="35"/>
+      <c r="S54" s="45">
+        <v>1</v>
+      </c>
+      <c r="T54" s="45">
+        <v>3</v>
+      </c>
+      <c r="U54" s="45">
+        <v>0</v>
+      </c>
+      <c r="V54" s="45">
+        <v>0</v>
+      </c>
+      <c r="W54" s="50"/>
+      <c r="X54" s="45"/>
+      <c r="Y54" s="35"/>
+      <c r="Z54" s="34"/>
+      <c r="AA54" s="11"/>
+      <c r="AB54" s="11"/>
+      <c r="AC54" s="7"/>
+      <c r="AD54" s="13"/>
+      <c r="AE54" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF54" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="AG54" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH54" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI54" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ54" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="50"/>
+      <c r="B55" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="35"/>
+      <c r="S55" s="45">
+        <v>2.25</v>
+      </c>
+      <c r="T55" s="45">
+        <v>3</v>
+      </c>
+      <c r="U55" s="45">
+        <v>0</v>
+      </c>
+      <c r="V55" s="45">
+        <v>0</v>
+      </c>
+      <c r="W55" s="50"/>
+      <c r="X55" s="45"/>
+      <c r="Y55" s="35"/>
+      <c r="Z55" s="34"/>
+      <c r="AA55" s="11"/>
+      <c r="AB55" s="11"/>
+      <c r="AC55" s="7"/>
+      <c r="AD55" s="13"/>
+      <c r="AE55" s="7"/>
+      <c r="AF55" s="7"/>
+      <c r="AG55" s="11"/>
+      <c r="AH55" s="11"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="13"/>
+    </row>
+    <row r="56" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="50"/>
+      <c r="B56" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="35"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="35"/>
+      <c r="S56" s="45">
+        <v>1</v>
+      </c>
+      <c r="T56" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="U56" s="45">
+        <v>0</v>
+      </c>
+      <c r="V56" s="45">
+        <v>0</v>
+      </c>
+      <c r="W56" s="50"/>
+      <c r="X56" s="45"/>
+      <c r="Y56" s="35"/>
+      <c r="Z56" s="34"/>
+      <c r="AA56" s="11"/>
+      <c r="AB56" s="11"/>
+      <c r="AC56" s="7"/>
+      <c r="AD56" s="13"/>
+      <c r="AE56" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF56" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="AG56" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH56" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI56" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ56" s="13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="50"/>
+      <c r="B57" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="35"/>
+      <c r="M57" s="35"/>
+      <c r="N57" s="35"/>
+      <c r="O57" s="35"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="50"/>
+      <c r="R57" s="35"/>
+      <c r="S57" s="45">
+        <v>2.25</v>
+      </c>
+      <c r="T57" s="45">
+        <v>2.5</v>
+      </c>
+      <c r="U57" s="45">
+        <v>0</v>
+      </c>
+      <c r="V57" s="45">
+        <v>0</v>
+      </c>
+      <c r="W57" s="50"/>
+      <c r="X57" s="45"/>
+      <c r="Y57" s="35"/>
+      <c r="Z57" s="34"/>
+      <c r="AA57" s="11"/>
+      <c r="AB57" s="11"/>
+      <c r="AC57" s="7"/>
+      <c r="AD57" s="13"/>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="11"/>
+      <c r="AH57" s="11"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="13"/>
+    </row>
+    <row r="58" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E58" s="71"/>
+      <c r="F58" s="71"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="T58" s="3">
+        <v>4</v>
+      </c>
+      <c r="U58" s="3">
+        <v>0</v>
+      </c>
+      <c r="V58" s="3">
+        <v>0</v>
+      </c>
+      <c r="W58" s="2"/>
+      <c r="X58" s="3"/>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="72"/>
+      <c r="AA58" s="11"/>
+      <c r="AB58" s="11"/>
+      <c r="AC58" s="7"/>
+      <c r="AD58" s="13"/>
+      <c r="AE58" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF58" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="AG58" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI58" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ58" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="71"/>
+      <c r="F59" s="71"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="T59" s="3">
+        <v>4</v>
+      </c>
+      <c r="U59" s="3">
+        <v>0</v>
+      </c>
+      <c r="V59" s="3">
+        <v>0</v>
+      </c>
+      <c r="W59" s="2"/>
+      <c r="X59" s="3"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="72"/>
+      <c r="AA59" s="11"/>
+      <c r="AB59" s="11"/>
+      <c r="AC59" s="7"/>
+      <c r="AD59" s="13"/>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="11"/>
+      <c r="AH59" s="11"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="13"/>
+    </row>
+    <row r="60" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E60" s="71"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="T60" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="U60" s="3">
+        <v>0</v>
+      </c>
+      <c r="V60" s="3">
+        <v>0</v>
+      </c>
+      <c r="W60" s="2"/>
+      <c r="X60" s="3"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="72"/>
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="11"/>
+      <c r="AC60" s="7"/>
+      <c r="AD60" s="13"/>
+      <c r="AE60" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF60" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="AG60" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI60" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ60" s="13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="71"/>
+      <c r="F61" s="71"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="T61" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="U61" s="3">
+        <v>0</v>
+      </c>
+      <c r="V61" s="3">
+        <v>0</v>
+      </c>
+      <c r="W61" s="2"/>
+      <c r="X61" s="3"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="72"/>
+      <c r="AA61" s="11"/>
+      <c r="AB61" s="11"/>
+      <c r="AC61" s="7"/>
+      <c r="AD61" s="13"/>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="11"/>
+      <c r="AH61" s="11"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="13"/>
+    </row>
+    <row r="62" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" s="71"/>
+      <c r="F62" s="71"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="T62" s="3">
+        <v>3</v>
+      </c>
+      <c r="U62" s="3">
+        <v>0</v>
+      </c>
+      <c r="V62" s="3">
+        <v>0</v>
+      </c>
+      <c r="W62" s="2"/>
+      <c r="X62" s="3"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="72"/>
+      <c r="AA62" s="11"/>
+      <c r="AB62" s="11"/>
+      <c r="AC62" s="7"/>
+      <c r="AD62" s="13"/>
+      <c r="AE62" s="35" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF62" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="AG62" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH62" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI62" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ62" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="71"/>
+      <c r="F63" s="71"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="T63" s="3">
+        <v>3</v>
+      </c>
+      <c r="U63" s="3">
+        <v>0</v>
+      </c>
+      <c r="V63" s="3">
+        <v>0</v>
+      </c>
+      <c r="W63" s="2"/>
+      <c r="X63" s="3"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="72"/>
+      <c r="AA63" s="11"/>
+      <c r="AB63" s="11"/>
+      <c r="AC63" s="7"/>
+      <c r="AD63" s="13"/>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="11"/>
+      <c r="AH63" s="11"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="13"/>
+    </row>
+    <row r="64" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4496,9 +5530,24 @@
     <row r="172" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="173" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="174" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X2:X20" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X2:X20 X49" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4510,55 +5559,55 @@
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Y7 Y2:Y5</xm:sqref>
+          <xm:sqref>Y7 Y2:Y5 Y49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AF2:AF5 AA2:AA5 AF7 AA7</xm:sqref>
+          <xm:sqref>AA2:AA63 AG2:AG63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AB2:AB5 AG2:AG5 AB7 AG7</xm:sqref>
+          <xm:sqref>AB2:AB63 AH2:AH63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D20E3002-F58D-4FAD-9CC5-854E38BB1BD9}">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F7</xm:sqref>
+          <xm:sqref>F2:F63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
           <x14:formula1>
             <xm:f>Tables!$K$2:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B7</xm:sqref>
+          <xm:sqref>B2:B63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
           <x14:formula1>
-            <xm:f>Tables!$N$2:$N$57</xm:f>
+            <xm:f>Tables!$O$2:$O$57</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4D3802DC-9280-4A12-B1FF-B1C073FCAE84}">
-          <x14:formula1>
-            <xm:f>Tables!$A$2:$A$42</xm:f>
-          </x14:formula1>
-          <xm:sqref>AH2:AH7 AC2:AC7</xm:sqref>
+          <xm:sqref>D2:D63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{0B95AA9E-6EAC-4E79-9737-4C4B42A3B143}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W48</xm:sqref>
+          <xm:sqref>W2:W63 E7:E63 AC2:AC63 AI2:AI63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6AE078-B717-4B67-83B7-999D58BC2953}">
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G48</xm:sqref>
+          <xm:sqref>G2:G63</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{434DCAEE-02F3-44B7-8757-503F2F2EE546}">
+          <x14:formula1>
+            <xm:f>Tables!$M$2:$M$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>AD2:AD63 AJ2:AJ63</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4583,12 +5632,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="G1" s="29"/>
@@ -4609,12 +5658,12 @@
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
@@ -4655,19 +5704,19 @@
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
@@ -4753,55 +5802,55 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="55"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="62"/>
       <c r="K15" s="26">
         <f>SUM(K12:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="60" t="s">
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="60"/>
-      <c r="J16" s="61"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="68"/>
       <c r="K16" s="27">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="62"/>
       <c r="K17" s="25">
         <f>SUM(K15:K16)</f>
         <v>150</v>
@@ -4838,10 +5887,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="70"/>
       <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4891,10 +5940,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7C7130-C7ED-4E34-8ED2-CC717737ADA7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4904,11 +5953,11 @@
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="48" customWidth="1"/>
+    <col min="12" max="13" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>64</v>
       </c>
@@ -4919,34 +5968,38 @@
         <v>30</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H1"/>
       <c r="I1" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J1"/>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="32" t="s">
         <v>31</v>
       </c>
       <c r="L1"/>
-      <c r="M1"/>
-      <c r="N1" s="46" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="N1"/>
+      <c r="O1" s="46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="G2" s="11"/>
       <c r="I2" s="11"/>
       <c r="K2" s="11"/>
-      <c r="N2" s="41"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="11"/>
+      <c r="O2" s="41"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>15</v>
@@ -4955,20 +6008,23 @@
         <v>6</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>66</v>
       </c>
       <c r="L3" s="6"/>
-      <c r="N3" s="41" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>17</v>
       </c>
@@ -4979,20 +6035,23 @@
         <v>33</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>67</v>
       </c>
       <c r="L4" s="6"/>
-      <c r="N4" s="41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="O4" s="41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
@@ -5003,19 +6062,22 @@
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="N5" s="41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M5" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="O5" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>24</v>
@@ -5024,427 +6086,436 @@
         <v>34</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="6"/>
-      <c r="N6" s="41" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E7" s="11">
         <v>9</v>
       </c>
-      <c r="N7" s="41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="O7" s="41" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="N8" s="41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M8" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="O8" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="11">
         <v>10</v>
       </c>
-      <c r="N9" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N10" s="42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="11">
         <v>11</v>
       </c>
-      <c r="N11" s="41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>40</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N12" s="41" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E13" s="11">
         <v>12</v>
       </c>
-      <c r="N13" s="41" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
-        <v>219</v>
+      <c r="O13" s="41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
+        <v>218</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N14" s="41" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="11">
         <v>14</v>
       </c>
-      <c r="N15" s="41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E16" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="N16" s="42" t="s">
+      <c r="O16" s="42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="O17" s="41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="O18" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="O19" s="41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="O20" s="41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="O21" s="41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="O22" s="41" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="N17" s="41" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="N18" s="41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
-        <v>222</v>
-      </c>
-      <c r="N19" s="41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
-        <v>151</v>
-      </c>
-      <c r="N20" s="41" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
-        <v>152</v>
-      </c>
-      <c r="N21" s="41" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="N22" s="41" t="s">
+      <c r="O23" s="41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="O24" s="41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="N23" s="41" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="N24" s="41" t="s">
+      <c r="O25" s="41" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="N25" s="41" t="s">
+      <c r="O26" s="41" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="N26" s="41" t="s">
+      <c r="O27" s="41" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="N27" s="41" t="s">
+      <c r="O28" s="41" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="N28" s="41" t="s">
+      <c r="O29" s="42" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="N29" s="42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="N30" s="41" t="s">
+      <c r="O30" s="41" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="O31" s="41" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="O32" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="N31" s="41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
-        <v>223</v>
-      </c>
-      <c r="N32" s="42" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="O33" s="41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="N33" s="41" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="O34" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="N34" s="41" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="N35" s="41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O35" s="41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="N36" s="41" t="s">
+      <c r="O36" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="O37" s="41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="O38" s="41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="O39" s="41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="O40" s="41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="O41" s="41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="O42" s="41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="O43" s="41" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="N37" s="41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="N38" s="41" t="s">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O44" s="41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O45" s="41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O46" s="41" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="N39" s="41" t="s">
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O47" s="41" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="N40" s="41" t="s">
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O48" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O49" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O50" s="47" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="N41" s="41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="N42" s="41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="N43" s="41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N44" s="41" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N45" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N46" s="41" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N47" s="41" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N48" s="41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N49" s="41" t="s">
+    <row r="51" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O51" s="41" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N50" s="47" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="51" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N51" s="41" t="s">
+    <row r="52" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O52" s="41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O53" s="41" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N52" s="41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N53" s="41" t="s">
+    <row r="54" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O54" s="41" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N54" s="41" t="s">
+    <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O55" s="41" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N55" s="41" t="s">
+    <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O56" s="41" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N56" s="41" t="s">
+    <row r="57" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O57" s="41" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N57" s="41" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="58" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M3:M57">
-    <sortCondition ref="M3:M57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N3:N57">
+    <sortCondition ref="N3:N57"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed up the excel data templates Tables sheet Line Weights values
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECCE914-0970-4F54-B554-D40EF5E19636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834F9C18-B50C-4932-8C28-C4D51BDE93D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27090" yWindow="615" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-27435" yWindow="270" windowWidth="26550" windowHeight="14445" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="269">
   <si>
     <t>mach_name</t>
   </si>
@@ -1062,6 +1062,18 @@
   </si>
   <si>
     <t>6.0 pt.</t>
+  </si>
+  <si>
+    <t>2 pt</t>
+  </si>
+  <si>
+    <t>3 pt</t>
+  </si>
+  <si>
+    <t>4 pt</t>
+  </si>
+  <si>
+    <t>6 pt</t>
   </si>
 </sst>
 </file>
@@ -1414,6 +1426,12 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1434,12 +1452,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1759,8 +1771,8 @@
   <dimension ref="A1:AJ189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,8 +5094,8 @@
       <c r="D58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E58" s="71"/>
-      <c r="F58" s="71"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="58"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -5111,7 +5123,7 @@
       <c r="W58" s="2"/>
       <c r="X58" s="3"/>
       <c r="Y58" s="1"/>
-      <c r="Z58" s="72"/>
+      <c r="Z58" s="59"/>
       <c r="AA58" s="11"/>
       <c r="AB58" s="11"/>
       <c r="AC58" s="7"/>
@@ -5146,8 +5158,8 @@
       <c r="D59" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E59" s="71"/>
-      <c r="F59" s="71"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="58"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -5175,7 +5187,7 @@
       <c r="W59" s="2"/>
       <c r="X59" s="3"/>
       <c r="Y59" s="1"/>
-      <c r="Z59" s="72"/>
+      <c r="Z59" s="59"/>
       <c r="AA59" s="11"/>
       <c r="AB59" s="11"/>
       <c r="AC59" s="7"/>
@@ -5198,8 +5210,8 @@
       <c r="D60" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E60" s="71"/>
-      <c r="F60" s="71"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -5227,7 +5239,7 @@
       <c r="W60" s="2"/>
       <c r="X60" s="3"/>
       <c r="Y60" s="1"/>
-      <c r="Z60" s="72"/>
+      <c r="Z60" s="59"/>
       <c r="AA60" s="11"/>
       <c r="AB60" s="11"/>
       <c r="AC60" s="7"/>
@@ -5262,8 +5274,8 @@
       <c r="D61" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E61" s="71"/>
-      <c r="F61" s="71"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -5291,7 +5303,7 @@
       <c r="W61" s="2"/>
       <c r="X61" s="3"/>
       <c r="Y61" s="1"/>
-      <c r="Z61" s="72"/>
+      <c r="Z61" s="59"/>
       <c r="AA61" s="11"/>
       <c r="AB61" s="11"/>
       <c r="AC61" s="7"/>
@@ -5314,8 +5326,8 @@
       <c r="D62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E62" s="71"/>
-      <c r="F62" s="71"/>
+      <c r="E62" s="58"/>
+      <c r="F62" s="58"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -5343,7 +5355,7 @@
       <c r="W62" s="2"/>
       <c r="X62" s="3"/>
       <c r="Y62" s="1"/>
-      <c r="Z62" s="72"/>
+      <c r="Z62" s="59"/>
       <c r="AA62" s="11"/>
       <c r="AB62" s="11"/>
       <c r="AC62" s="7"/>
@@ -5378,8 +5390,8 @@
       <c r="D63" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="71"/>
-      <c r="F63" s="71"/>
+      <c r="E63" s="58"/>
+      <c r="F63" s="58"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -5407,7 +5419,7 @@
       <c r="W63" s="2"/>
       <c r="X63" s="3"/>
       <c r="Y63" s="1"/>
-      <c r="Z63" s="72"/>
+      <c r="Z63" s="59"/>
       <c r="AA63" s="11"/>
       <c r="AB63" s="11"/>
       <c r="AC63" s="7"/>
@@ -5632,12 +5644,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="G1" s="29"/>
@@ -5658,12 +5670,12 @@
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
@@ -5704,19 +5716,19 @@
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
@@ -5802,55 +5814,55 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="62"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="64"/>
       <c r="K15" s="26">
         <f>SUM(K12:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="67" t="s">
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="67"/>
-      <c r="J16" s="68"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="70"/>
       <c r="K16" s="27">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="62"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="64"/>
       <c r="K17" s="25">
         <f>SUM(K15:K16)</f>
         <v>150</v>
@@ -5887,10 +5899,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="70"/>
+      <c r="B1" s="72"/>
       <c r="C1" s="28"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5943,7 +5955,7 @@
   <dimension ref="A1:O69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6045,7 +6057,7 @@
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="13" t="s">
-        <v>237</v>
+        <v>265</v>
       </c>
       <c r="O4" s="41" t="s">
         <v>94</v>
@@ -6093,7 +6105,7 @@
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="13" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
       <c r="O6" s="41" t="s">
         <v>96</v>
@@ -6107,7 +6119,7 @@
         <v>9</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="O7" s="41" t="s">
         <v>97</v>
@@ -6121,7 +6133,7 @@
         <v>35</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="O8" s="41" t="s">
         <v>98</v>

</xml_diff>

<commit_message>
Updated the excel data file temlates  added Disabled for comments Updated a few stencils Group1 color, Ethernet's colors to match Updated the Template with the new stencil
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E94FF0-3869-4FCA-806D-9ACD45796C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD8DB5F-1D49-4116-84F3-2C9B483E5FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6795" yWindow="4980" windowWidth="27225" windowHeight="14730" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-24240" yWindow="420" windowWidth="23535" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="322">
   <si>
     <t>mach_name</t>
   </si>
@@ -1232,6 +1232,12 @@
   </si>
   <si>
     <t>OC_Ethernet2H:1</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Page-2</t>
   </si>
 </sst>
 </file>
@@ -1937,7 +1943,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111:A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2084,9 @@
       <c r="A2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
@@ -2300,7 +2308,9 @@
       <c r="A7" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
@@ -2900,7 +2910,9 @@
       <c r="A18" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B18" s="14"/>
+      <c r="B18" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="61"/>
@@ -3388,7 +3400,9 @@
       <c r="A27" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B27" s="14"/>
+      <c r="B27" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="61"/>
@@ -3826,7 +3840,9 @@
       <c r="A35" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B35" s="14"/>
+      <c r="B35" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="61"/>
@@ -4206,7 +4222,9 @@
       <c r="A42" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B42" s="14"/>
+      <c r="B42" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="61"/>
@@ -4470,7 +4488,9 @@
       <c r="A47" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B47" s="14"/>
+      <c r="B47" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="61"/>
@@ -4734,7 +4754,9 @@
       <c r="A52" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="14"/>
+      <c r="B52" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="61"/>
@@ -5124,7 +5146,9 @@
       <c r="A59" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B59" s="14"/>
+      <c r="B59" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="61"/>
@@ -5396,7 +5420,9 @@
       <c r="A64" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B64" s="14"/>
+      <c r="B64" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="61"/>
@@ -5604,7 +5630,9 @@
       <c r="A68" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="B68" s="14"/>
+      <c r="B68" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
@@ -5641,8 +5669,8 @@
       <c r="AJ68" s="16"/>
     </row>
     <row r="69" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="9">
-        <v>2</v>
+      <c r="A69" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>14</v>
@@ -5701,8 +5729,8 @@
       <c r="AJ69" s="7"/>
     </row>
     <row r="70" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9">
-        <v>2</v>
+      <c r="A70" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>14</v>
@@ -5761,8 +5789,8 @@
       <c r="AJ70" s="7"/>
     </row>
     <row r="71" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="9">
-        <v>2</v>
+      <c r="A71" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>14</v>
@@ -5821,8 +5849,8 @@
       <c r="AJ71" s="7"/>
     </row>
     <row r="72" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="9">
-        <v>2</v>
+      <c r="A72" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>14</v>
@@ -5881,8 +5909,8 @@
       <c r="AJ72" s="7"/>
     </row>
     <row r="73" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="9">
-        <v>2</v>
+      <c r="A73" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>14</v>
@@ -5941,8 +5969,8 @@
       <c r="AJ73" s="7"/>
     </row>
     <row r="74" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="9">
-        <v>2</v>
+      <c r="A74" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>14</v>
@@ -6001,8 +6029,8 @@
       <c r="AJ74" s="7"/>
     </row>
     <row r="75" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="9">
-        <v>2</v>
+      <c r="A75" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>14</v>
@@ -6061,8 +6089,8 @@
       <c r="AJ75" s="7"/>
     </row>
     <row r="76" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="9">
-        <v>2</v>
+      <c r="A76" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>14</v>
@@ -6121,8 +6149,8 @@
       <c r="AJ76" s="7"/>
     </row>
     <row r="77" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="9">
-        <v>2</v>
+      <c r="A77" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>14</v>
@@ -6181,8 +6209,8 @@
       <c r="AJ77" s="34"/>
     </row>
     <row r="78" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="9">
-        <v>2</v>
+      <c r="A78" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>14</v>
@@ -6241,8 +6269,8 @@
       <c r="AJ78" s="7"/>
     </row>
     <row r="79" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="9">
-        <v>2</v>
+      <c r="A79" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>14</v>
@@ -6301,8 +6329,8 @@
       <c r="AJ79" s="7"/>
     </row>
     <row r="80" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="9">
-        <v>2</v>
+      <c r="A80" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>14</v>
@@ -6361,8 +6389,8 @@
       <c r="AJ80" s="7"/>
     </row>
     <row r="81" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="9">
-        <v>2</v>
+      <c r="A81" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>14</v>
@@ -6421,8 +6449,8 @@
       <c r="AJ81" s="13"/>
     </row>
     <row r="82" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="9">
-        <v>2</v>
+      <c r="A82" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>14</v>
@@ -6481,8 +6509,8 @@
       <c r="AJ82" s="13"/>
     </row>
     <row r="83" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="9">
-        <v>2</v>
+      <c r="A83" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>14</v>
@@ -6541,8 +6569,8 @@
       <c r="AJ83" s="13"/>
     </row>
     <row r="84" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="9">
-        <v>2</v>
+      <c r="A84" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>14</v>
@@ -6601,8 +6629,8 @@
       <c r="AJ84" s="13"/>
     </row>
     <row r="85" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="9">
-        <v>2</v>
+      <c r="A85" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>14</v>
@@ -6661,8 +6689,8 @@
       <c r="AJ85" s="13"/>
     </row>
     <row r="86" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="9">
-        <v>2</v>
+      <c r="A86" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>14</v>
@@ -6721,8 +6749,8 @@
       <c r="AJ86" s="13"/>
     </row>
     <row r="87" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="9">
-        <v>2</v>
+      <c r="A87" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>14</v>
@@ -6781,8 +6809,8 @@
       <c r="AJ87" s="13"/>
     </row>
     <row r="88" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="9">
-        <v>2</v>
+      <c r="A88" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>14</v>
@@ -6841,8 +6869,8 @@
       <c r="AJ88" s="13"/>
     </row>
     <row r="89" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="9">
-        <v>2</v>
+      <c r="A89" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>14</v>
@@ -6901,8 +6929,8 @@
       <c r="AJ89" s="13"/>
     </row>
     <row r="90" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="9">
-        <v>2</v>
+      <c r="A90" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B90" s="35" t="s">
         <v>14</v>
@@ -6961,8 +6989,8 @@
       <c r="AJ90" s="13"/>
     </row>
     <row r="91" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="9">
-        <v>2</v>
+      <c r="A91" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B91" s="35" t="s">
         <v>14</v>
@@ -7021,8 +7049,8 @@
       <c r="AJ91" s="13"/>
     </row>
     <row r="92" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="9">
-        <v>2</v>
+      <c r="A92" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B92" s="35" t="s">
         <v>14</v>
@@ -7081,8 +7109,8 @@
       <c r="AJ92" s="13"/>
     </row>
     <row r="93" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="9">
-        <v>2</v>
+      <c r="A93" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B93" s="35" t="s">
         <v>14</v>
@@ -7141,8 +7169,8 @@
       <c r="AJ93" s="13"/>
     </row>
     <row r="94" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="9">
-        <v>2</v>
+      <c r="A94" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B94" s="35" t="s">
         <v>14</v>
@@ -7201,8 +7229,8 @@
       <c r="AJ94" s="13"/>
     </row>
     <row r="95" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="9">
-        <v>2</v>
+      <c r="A95" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B95" s="35" t="s">
         <v>14</v>
@@ -7261,8 +7289,8 @@
       <c r="AJ95" s="13"/>
     </row>
     <row r="96" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="9">
-        <v>2</v>
+      <c r="A96" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B96" s="35" t="s">
         <v>14</v>
@@ -7321,8 +7349,8 @@
       <c r="AJ96" s="13"/>
     </row>
     <row r="97" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="9">
-        <v>2</v>
+      <c r="A97" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B97" s="35" t="s">
         <v>14</v>
@@ -7381,8 +7409,8 @@
       <c r="AJ97" s="13"/>
     </row>
     <row r="98" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="9">
-        <v>2</v>
+      <c r="A98" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B98" s="35" t="s">
         <v>14</v>
@@ -7441,8 +7469,8 @@
       <c r="AJ98" s="13"/>
     </row>
     <row r="99" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="9">
-        <v>2</v>
+      <c r="A99" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B99" s="35" t="s">
         <v>14</v>
@@ -7501,8 +7529,8 @@
       <c r="AJ99" s="13"/>
     </row>
     <row r="100" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="9">
-        <v>2</v>
+      <c r="A100" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B100" s="35" t="s">
         <v>14</v>
@@ -7561,8 +7589,8 @@
       <c r="AJ100" s="13"/>
     </row>
     <row r="101" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="9">
-        <v>2</v>
+      <c r="A101" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B101" s="35" t="s">
         <v>14</v>
@@ -7621,8 +7649,8 @@
       <c r="AJ101" s="13"/>
     </row>
     <row r="102" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="9">
-        <v>2</v>
+      <c r="A102" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>14</v>
@@ -7681,8 +7709,8 @@
       <c r="AJ102" s="13"/>
     </row>
     <row r="103" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="9">
-        <v>2</v>
+      <c r="A103" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>14</v>
@@ -7741,8 +7769,8 @@
       <c r="AJ103" s="13"/>
     </row>
     <row r="104" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="9">
-        <v>2</v>
+      <c r="A104" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>14</v>
@@ -7801,8 +7829,8 @@
       <c r="AJ104" s="13"/>
     </row>
     <row r="105" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="9">
-        <v>2</v>
+      <c r="A105" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>14</v>
@@ -7861,8 +7889,8 @@
       <c r="AJ105" s="13"/>
     </row>
     <row r="106" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="9">
-        <v>2</v>
+      <c r="A106" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>14</v>
@@ -7921,8 +7949,8 @@
       <c r="AJ106" s="13"/>
     </row>
     <row r="107" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="9">
-        <v>2</v>
+      <c r="A107" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>14</v>
@@ -7981,8 +8009,8 @@
       <c r="AJ107" s="13"/>
     </row>
     <row r="108" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="9">
-        <v>2</v>
+      <c r="A108" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>14</v>
@@ -8041,8 +8069,8 @@
       <c r="AJ108" s="13"/>
     </row>
     <row r="109" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="9">
-        <v>2</v>
+      <c r="A109" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>14</v>
@@ -8104,7 +8132,9 @@
       <c r="A110" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="B110" s="14"/>
+      <c r="B110" s="14" t="s">
+        <v>320</v>
+      </c>
       <c r="C110" s="14"/>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
@@ -8141,8 +8171,8 @@
       <c r="AJ110" s="16"/>
     </row>
     <row r="111" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="9">
-        <v>2</v>
+      <c r="A111" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B111" s="35" t="s">
         <v>14</v>
@@ -8205,8 +8235,8 @@
       <c r="AJ111" s="13"/>
     </row>
     <row r="112" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="9">
-        <v>2</v>
+      <c r="A112" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B112" s="35" t="s">
         <v>14</v>
@@ -8259,8 +8289,8 @@
       <c r="AJ112" s="13"/>
     </row>
     <row r="113" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="9">
-        <v>2</v>
+      <c r="A113" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B113" s="35" t="s">
         <v>14</v>
@@ -8325,8 +8355,8 @@
       </c>
     </row>
     <row r="114" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="9">
-        <v>2</v>
+      <c r="A114" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B114" s="35" t="s">
         <v>14</v>
@@ -8379,8 +8409,8 @@
       <c r="AJ114" s="13"/>
     </row>
     <row r="115" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="9">
-        <v>2</v>
+      <c r="A115" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B115" s="35" t="s">
         <v>14</v>
@@ -8445,8 +8475,8 @@
       </c>
     </row>
     <row r="116" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="9">
-        <v>2</v>
+      <c r="A116" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B116" s="35" t="s">
         <v>14</v>
@@ -8499,8 +8529,8 @@
       <c r="AJ116" s="13"/>
     </row>
     <row r="117" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="9">
-        <v>2</v>
+      <c r="A117" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B117" s="35" t="s">
         <v>14</v>
@@ -8565,8 +8595,8 @@
       </c>
     </row>
     <row r="118" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="9">
-        <v>2</v>
+      <c r="A118" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B118" s="35" t="s">
         <v>14</v>
@@ -8619,8 +8649,8 @@
       <c r="AJ118" s="13"/>
     </row>
     <row r="119" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="9">
-        <v>2</v>
+      <c r="A119" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>14</v>
@@ -8685,8 +8715,8 @@
       </c>
     </row>
     <row r="120" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="9">
-        <v>2</v>
+      <c r="A120" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>14</v>
@@ -8739,8 +8769,8 @@
       <c r="AJ120" s="13"/>
     </row>
     <row r="121" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="9">
-        <v>2</v>
+      <c r="A121" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>14</v>
@@ -8805,8 +8835,8 @@
       </c>
     </row>
     <row r="122" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="9">
-        <v>2</v>
+      <c r="A122" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>14</v>
@@ -8859,8 +8889,8 @@
       <c r="AJ122" s="13"/>
     </row>
     <row r="123" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="9">
-        <v>2</v>
+      <c r="A123" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>14</v>
@@ -8925,8 +8955,8 @@
       </c>
     </row>
     <row r="124" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="9">
-        <v>2</v>
+      <c r="A124" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>14</v>
@@ -8989,7 +9019,7 @@
   </sheetData>
   <autoFilter ref="A1:AJ124" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}"/>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X110 X68:X81 X65 X2:X52 X55:X64 E65:E1048576 E1:E64" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X110 X68:X81 X2:X52 X55:X65 E1:E1048576" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9007,49 +9037,49 @@
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AA65:AA124 AA2:AA64 AG65:AG124 AG2:AG64</xm:sqref>
+          <xm:sqref>AA2:AA124 AG2:AG124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AB65:AB124 AB2:AB64 AH65:AH124 AH2:AH64</xm:sqref>
+          <xm:sqref>AB2:AB124 AH2:AH124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D20E3002-F58D-4FAD-9CC5-854E38BB1BD9}">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F65:F124 F2:F64</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
-          <x14:formula1>
-            <xm:f>Tables!$K$2:$K$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B65:B124 B2:B64</xm:sqref>
+          <xm:sqref>F2:F124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{0B95AA9E-6EAC-4E79-9737-4C4B42A3B143}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>AI65:AI124 AI2:AI64 W65:W124 W2:W64 AC65:AC124 AC2:AC64</xm:sqref>
+          <xm:sqref>AI2:AI124 W2:W124 AC2:AC124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6AE078-B717-4B67-83B7-999D58BC2953}">
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>G65:G124 G2:G64</xm:sqref>
+          <xm:sqref>G2:G124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{434DCAEE-02F3-44B7-8757-503F2F2EE546}">
           <x14:formula1>
             <xm:f>Tables!$M$2:$M$8</xm:f>
           </x14:formula1>
-          <xm:sqref>AD65:AD124 AD2:AD64 AJ65:AJ124 AJ2:AJ64</xm:sqref>
+          <xm:sqref>AD2:AD124 AJ2:AJ124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
           <x14:formula1>
             <xm:f>Tables!$O$2:$O$54</xm:f>
           </x14:formula1>
-          <xm:sqref>D65:D124 D2:D64</xm:sqref>
+          <xm:sqref>D2:D124</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
+          <x14:formula1>
+            <xm:f>Tables!$K$2:$K$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B124</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9455,8 +9485,8 @@
       <c r="I3" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="K3" s="11" t="s">
-        <v>66</v>
+      <c r="K3" s="13" t="s">
+        <v>320</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="13" t="s">
@@ -9483,7 +9513,7 @@
         <v>136</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="13" t="s">
@@ -9507,7 +9537,7 @@
         <v>80</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="13" t="s">
@@ -9531,7 +9561,7 @@
         <v>81</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="13" t="s">
@@ -9547,6 +9577,9 @@
       </c>
       <c r="E7" s="11">
         <v>9</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="M7" s="13" t="s">
         <v>258</v>

</xml_diff>

<commit_message>
added a numbe of things. was an issue with not closing excel correctly added comments to a number of functions added calculations for shape resizing and writing to Excel data file
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD8DB5F-1D49-4116-84F3-2C9B483E5FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F89D7-8FF0-4C1B-96C2-005C9FF9AAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24240" yWindow="420" windowWidth="23535" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="322">
   <si>
     <t>mach_name</t>
   </si>
@@ -1942,8 +1942,8 @@
   <dimension ref="A1:AJ132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111:A124"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3591,9 +3591,7 @@
       <c r="V30" s="45">
         <v>0</v>
       </c>
-      <c r="W30" s="45" t="s">
-        <v>18</v>
-      </c>
+      <c r="W30" s="45"/>
       <c r="X30" s="45"/>
       <c r="Y30" s="35"/>
       <c r="Z30" s="34"/>
@@ -3819,9 +3817,7 @@
       <c r="V34" s="45">
         <v>0</v>
       </c>
-      <c r="W34" s="45" t="s">
-        <v>211</v>
-      </c>
+      <c r="W34" s="45"/>
       <c r="X34" s="45"/>
       <c r="Y34" s="35"/>
       <c r="Z34" s="34"/>
@@ -4143,9 +4139,7 @@
       <c r="V40" s="45">
         <v>0</v>
       </c>
-      <c r="W40" s="45" t="s">
-        <v>209</v>
-      </c>
+      <c r="W40" s="45"/>
       <c r="X40" s="45"/>
       <c r="Y40" s="35"/>
       <c r="Z40" s="34"/>
@@ -4201,9 +4195,7 @@
       <c r="V41" s="45">
         <v>0</v>
       </c>
-      <c r="W41" s="45" t="s">
-        <v>210</v>
-      </c>
+      <c r="W41" s="45"/>
       <c r="X41" s="45"/>
       <c r="Y41" s="35"/>
       <c r="Z41" s="34"/>
@@ -4949,9 +4941,7 @@
       <c r="V55" s="45">
         <v>0</v>
       </c>
-      <c r="W55" s="45" t="s">
-        <v>141</v>
-      </c>
+      <c r="W55" s="45"/>
       <c r="X55" s="45"/>
       <c r="Y55" s="35"/>
       <c r="Z55" s="34"/>
@@ -5065,9 +5055,7 @@
       <c r="V57" s="45">
         <v>0</v>
       </c>
-      <c r="W57" s="45" t="s">
-        <v>150</v>
-      </c>
+      <c r="W57" s="45"/>
       <c r="X57" s="45"/>
       <c r="Y57" s="35"/>
       <c r="Z57" s="34"/>
@@ -5125,9 +5113,7 @@
       <c r="V58" s="45">
         <v>0</v>
       </c>
-      <c r="W58" s="45" t="s">
-        <v>214</v>
-      </c>
+      <c r="W58" s="45"/>
       <c r="X58" s="45"/>
       <c r="Y58" s="35"/>
       <c r="Z58" s="34"/>

</xml_diff>

<commit_message>
Modified all the excel files to resize the OC_Group shape
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F89D7-8FF0-4C1B-96C2-005C9FF9AAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6009D4-7123-44F9-A53F-B5BD7014117F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="420" windowWidth="23535" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="4875" yWindow="2565" windowWidth="23535" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -1942,8 +1942,8 @@
   <dimension ref="A1:AJ132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W30" sqref="W30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2123,39 +2123,39 @@
       <c r="AJ2" s="16"/>
     </row>
     <row r="3" spans="1:36" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="8"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="14"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="11"/>
       <c r="AB3" s="11"/>
@@ -2213,39 +2213,39 @@
       <c r="AJ4" s="7"/>
     </row>
     <row r="5" spans="1:36" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="8"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="14"/>
       <c r="Z5" s="7"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>

</xml_diff>

<commit_message>
Fixed up the template script files.  modifications due to slight changes to some of the stencils.  Also the adding of a new stencil
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6009D4-7123-44F9-A53F-B5BD7014117F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF20822C-B2A2-4118-9750-CE29B6E4FB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="2565" windowWidth="23535" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="3240" yWindow="1290" windowWidth="25665" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Tables" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VisioData!$A$1:$AJ$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VisioData!$A$1:$AJ$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="324">
   <si>
     <t>mach_name</t>
   </si>
@@ -1238,6 +1238,12 @@
   </si>
   <si>
     <t>Page-2</t>
+  </si>
+  <si>
+    <t>OC_LabelGreen</t>
+  </si>
+  <si>
+    <t>OC_LabelGreen:1</t>
   </si>
 </sst>
 </file>
@@ -1939,11 +1945,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ132"/>
+  <dimension ref="A1:AJ133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:Y3"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T124" sqref="T124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4964,13 +4970,13 @@
         <v>14</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>108</v>
+        <v>322</v>
       </c>
       <c r="E56" s="49" t="s">
-        <v>108</v>
+        <v>322</v>
       </c>
       <c r="F56" s="49"/>
       <c r="G56" s="35"/>
@@ -4986,10 +4992,10 @@
       <c r="Q56" s="50"/>
       <c r="R56" s="35"/>
       <c r="S56" s="45">
-        <v>6.4329999999999998</v>
+        <v>5.25</v>
       </c>
       <c r="T56" s="45">
-        <v>6.3559999999999999</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="U56" s="45">
         <v>0</v>
@@ -5020,18 +5026,16 @@
         <v>14</v>
       </c>
       <c r="C57" s="35" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="E57" s="49" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F57" s="49"/>
-      <c r="G57" s="35">
-        <v>8</v>
-      </c>
+      <c r="G57" s="35"/>
       <c r="H57" s="35"/>
       <c r="I57" s="35"/>
       <c r="J57" s="35"/>
@@ -5047,7 +5051,7 @@
         <v>6.4329999999999998</v>
       </c>
       <c r="T57" s="45">
-        <v>4.085</v>
+        <v>6.3559999999999999</v>
       </c>
       <c r="U57" s="45">
         <v>0</v>
@@ -5078,13 +5082,13 @@
         <v>14</v>
       </c>
       <c r="C58" s="35" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E58" s="49" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F58" s="49"/>
       <c r="G58" s="35">
@@ -5102,7 +5106,7 @@
       <c r="Q58" s="50"/>
       <c r="R58" s="35"/>
       <c r="S58" s="45">
-        <v>7.3159999999999998</v>
+        <v>6.4329999999999998</v>
       </c>
       <c r="T58" s="45">
         <v>4.085</v>
@@ -5129,104 +5133,104 @@
       <c r="AJ58" s="54"/>
     </row>
     <row r="59" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="50">
+        <v>1</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="D59" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="F59" s="49"/>
+      <c r="G59" s="35">
+        <v>8</v>
+      </c>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="35"/>
+      <c r="P59" s="50"/>
+      <c r="Q59" s="50"/>
+      <c r="R59" s="35"/>
+      <c r="S59" s="45">
+        <v>7.3159999999999998</v>
+      </c>
+      <c r="T59" s="45">
+        <v>4.085</v>
+      </c>
+      <c r="U59" s="45">
+        <v>0</v>
+      </c>
+      <c r="V59" s="45">
+        <v>0</v>
+      </c>
+      <c r="W59" s="45"/>
+      <c r="X59" s="45"/>
+      <c r="Y59" s="35"/>
+      <c r="Z59" s="34"/>
+      <c r="AA59" s="34"/>
+      <c r="AB59" s="34"/>
+      <c r="AC59" s="34"/>
+      <c r="AD59" s="54"/>
+      <c r="AE59" s="34"/>
+      <c r="AF59" s="34"/>
+      <c r="AG59" s="34"/>
+      <c r="AH59" s="34"/>
+      <c r="AI59" s="34"/>
+      <c r="AJ59" s="54"/>
+    </row>
+    <row r="60" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B60" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="14"/>
-      <c r="S59" s="17"/>
-      <c r="T59" s="17"/>
-      <c r="U59" s="17"/>
-      <c r="V59" s="17"/>
-      <c r="W59" s="17"/>
-      <c r="X59" s="17"/>
-      <c r="Y59" s="14"/>
-      <c r="Z59" s="16"/>
-      <c r="AA59" s="16"/>
-      <c r="AB59" s="16"/>
-      <c r="AC59" s="16"/>
-      <c r="AD59" s="62"/>
-      <c r="AE59" s="16"/>
-      <c r="AF59" s="16"/>
-      <c r="AG59" s="16"/>
-      <c r="AH59" s="16"/>
-      <c r="AI59" s="16"/>
-      <c r="AJ59" s="62"/>
-    </row>
-    <row r="60" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="50">
-        <v>1</v>
-      </c>
-      <c r="B60" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="35" t="s">
-        <v>301</v>
-      </c>
-      <c r="D60" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="E60" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F60" s="49"/>
-      <c r="G60" s="35">
-        <v>8</v>
-      </c>
-      <c r="H60" s="35"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="35"/>
-      <c r="K60" s="35"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="35"/>
-      <c r="N60" s="35"/>
-      <c r="O60" s="35"/>
-      <c r="P60" s="50"/>
-      <c r="Q60" s="50"/>
-      <c r="R60" s="35"/>
-      <c r="S60" s="45">
-        <v>1.087</v>
-      </c>
-      <c r="T60" s="45">
-        <v>3.0680000000000001</v>
-      </c>
-      <c r="U60" s="45">
-        <v>0</v>
-      </c>
-      <c r="V60" s="45">
-        <v>0</v>
-      </c>
-      <c r="W60" s="45"/>
-      <c r="X60" s="45"/>
-      <c r="Y60" s="35"/>
-      <c r="Z60" s="34"/>
-      <c r="AA60" s="34"/>
-      <c r="AB60" s="34"/>
-      <c r="AC60" s="34"/>
-      <c r="AD60" s="54"/>
-      <c r="AE60" s="34"/>
-      <c r="AF60" s="34"/>
-      <c r="AG60" s="34"/>
-      <c r="AH60" s="34"/>
-      <c r="AI60" s="34"/>
-      <c r="AJ60" s="54"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="61"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="14"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="14"/>
+      <c r="S60" s="17"/>
+      <c r="T60" s="17"/>
+      <c r="U60" s="17"/>
+      <c r="V60" s="17"/>
+      <c r="W60" s="17"/>
+      <c r="X60" s="17"/>
+      <c r="Y60" s="14"/>
+      <c r="Z60" s="16"/>
+      <c r="AA60" s="16"/>
+      <c r="AB60" s="16"/>
+      <c r="AC60" s="16"/>
+      <c r="AD60" s="62"/>
+      <c r="AE60" s="16"/>
+      <c r="AF60" s="16"/>
+      <c r="AG60" s="16"/>
+      <c r="AH60" s="16"/>
+      <c r="AI60" s="16"/>
+      <c r="AJ60" s="62"/>
     </row>
     <row r="61" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="50">
@@ -5236,13 +5240,13 @@
         <v>14</v>
       </c>
       <c r="C61" s="35" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>318</v>
+        <v>113</v>
       </c>
       <c r="E61" s="49" t="s">
-        <v>318</v>
+        <v>113</v>
       </c>
       <c r="F61" s="49"/>
       <c r="G61" s="35">
@@ -5260,10 +5264,10 @@
       <c r="Q61" s="50"/>
       <c r="R61" s="35"/>
       <c r="S61" s="45">
-        <v>2</v>
+        <v>1.087</v>
       </c>
       <c r="T61" s="45">
-        <v>3.4729999999999999</v>
+        <v>3.0680000000000001</v>
       </c>
       <c r="U61" s="45">
         <v>0</v>
@@ -5294,17 +5298,17 @@
         <v>14</v>
       </c>
       <c r="C62" s="35" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>106</v>
+        <v>318</v>
       </c>
       <c r="E62" s="49" t="s">
-        <v>106</v>
+        <v>318</v>
       </c>
       <c r="F62" s="49"/>
-      <c r="G62" s="35" t="s">
-        <v>33</v>
+      <c r="G62" s="35">
+        <v>8</v>
       </c>
       <c r="H62" s="35"/>
       <c r="I62" s="35"/>
@@ -5318,10 +5322,10 @@
       <c r="Q62" s="50"/>
       <c r="R62" s="35"/>
       <c r="S62" s="45">
-        <v>3.7869999999999999</v>
+        <v>2</v>
       </c>
       <c r="T62" s="45">
-        <v>3.5459999999999998</v>
+        <v>3.4729999999999999</v>
       </c>
       <c r="U62" s="45">
         <v>0</v>
@@ -5352,17 +5356,17 @@
         <v>14</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E63" s="49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F63" s="49"/>
-      <c r="G63" s="35">
-        <v>6</v>
+      <c r="G63" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="H63" s="35"/>
       <c r="I63" s="35"/>
@@ -5376,10 +5380,10 @@
       <c r="Q63" s="50"/>
       <c r="R63" s="35"/>
       <c r="S63" s="45">
-        <v>5.3079999999999998</v>
+        <v>3.7869999999999999</v>
       </c>
       <c r="T63" s="45">
-        <v>3.6259999999999999</v>
+        <v>3.5459999999999998</v>
       </c>
       <c r="U63" s="45">
         <v>0</v>
@@ -5403,104 +5407,106 @@
       <c r="AJ63" s="54"/>
     </row>
     <row r="64" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="50">
+        <v>1</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="D64" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E64" s="49" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="49"/>
+      <c r="G64" s="35">
+        <v>6</v>
+      </c>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="35"/>
+      <c r="K64" s="35"/>
+      <c r="L64" s="35"/>
+      <c r="M64" s="35"/>
+      <c r="N64" s="35"/>
+      <c r="O64" s="35"/>
+      <c r="P64" s="50"/>
+      <c r="Q64" s="50"/>
+      <c r="R64" s="35"/>
+      <c r="S64" s="45">
+        <v>5.3079999999999998</v>
+      </c>
+      <c r="T64" s="45">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="U64" s="45">
+        <v>0</v>
+      </c>
+      <c r="V64" s="45">
+        <v>0</v>
+      </c>
+      <c r="W64" s="45"/>
+      <c r="X64" s="45"/>
+      <c r="Y64" s="35"/>
+      <c r="Z64" s="34"/>
+      <c r="AA64" s="34"/>
+      <c r="AB64" s="34"/>
+      <c r="AC64" s="34"/>
+      <c r="AD64" s="54"/>
+      <c r="AE64" s="34"/>
+      <c r="AF64" s="34"/>
+      <c r="AG64" s="34"/>
+      <c r="AH64" s="34"/>
+      <c r="AI64" s="34"/>
+      <c r="AJ64" s="54"/>
+    </row>
+    <row r="65" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B65" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="61"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="17"/>
-      <c r="T64" s="17"/>
-      <c r="U64" s="17"/>
-      <c r="V64" s="17"/>
-      <c r="W64" s="17"/>
-      <c r="X64" s="17"/>
-      <c r="Y64" s="14"/>
-      <c r="Z64" s="16"/>
-      <c r="AA64" s="16"/>
-      <c r="AB64" s="16"/>
-      <c r="AC64" s="16"/>
-      <c r="AD64" s="62"/>
-      <c r="AE64" s="16"/>
-      <c r="AF64" s="16"/>
-      <c r="AG64" s="16"/>
-      <c r="AH64" s="16"/>
-      <c r="AI64" s="16"/>
-      <c r="AJ64" s="62"/>
-    </row>
-    <row r="65" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="50">
-        <v>1</v>
-      </c>
-      <c r="B65" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C65" s="35" t="s">
-        <v>297</v>
-      </c>
-      <c r="D65" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E65" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="F65" s="49"/>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="35"/>
-      <c r="J65" s="35"/>
-      <c r="K65" s="35"/>
-      <c r="L65" s="35"/>
-      <c r="M65" s="35"/>
-      <c r="N65" s="35"/>
-      <c r="O65" s="35"/>
-      <c r="P65" s="50"/>
-      <c r="Q65" s="50"/>
-      <c r="R65" s="35"/>
-      <c r="S65" s="45">
-        <v>0.25</v>
-      </c>
-      <c r="T65" s="45">
-        <v>2.6829999999999998</v>
-      </c>
-      <c r="U65" s="45">
-        <v>0</v>
-      </c>
-      <c r="V65" s="45">
-        <v>0</v>
-      </c>
-      <c r="W65" s="45"/>
-      <c r="X65" s="45"/>
-      <c r="Y65" s="35"/>
-      <c r="Z65" s="34"/>
-      <c r="AA65" s="34"/>
-      <c r="AB65" s="34"/>
-      <c r="AC65" s="34"/>
-      <c r="AD65" s="54"/>
-      <c r="AE65" s="34"/>
-      <c r="AF65" s="34"/>
-      <c r="AG65" s="34"/>
-      <c r="AH65" s="34"/>
-      <c r="AI65" s="34"/>
-      <c r="AJ65" s="54"/>
-    </row>
-    <row r="66" spans="1:36" s="60" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="61"/>
+      <c r="F65" s="61"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="N65" s="14"/>
+      <c r="O65" s="14"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="14"/>
+      <c r="S65" s="17"/>
+      <c r="T65" s="17"/>
+      <c r="U65" s="17"/>
+      <c r="V65" s="17"/>
+      <c r="W65" s="17"/>
+      <c r="X65" s="17"/>
+      <c r="Y65" s="14"/>
+      <c r="Z65" s="16"/>
+      <c r="AA65" s="16"/>
+      <c r="AB65" s="16"/>
+      <c r="AC65" s="16"/>
+      <c r="AD65" s="62"/>
+      <c r="AE65" s="16"/>
+      <c r="AF65" s="16"/>
+      <c r="AG65" s="16"/>
+      <c r="AH65" s="16"/>
+      <c r="AI65" s="16"/>
+      <c r="AJ65" s="62"/>
+    </row>
+    <row r="66" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="50">
         <v>1</v>
       </c>
@@ -5508,13 +5514,13 @@
         <v>14</v>
       </c>
       <c r="C66" s="35" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E66" s="49" t="s">
-        <v>317</v>
+        <v>88</v>
       </c>
       <c r="F66" s="49"/>
       <c r="G66" s="35"/>
@@ -5530,10 +5536,10 @@
       <c r="Q66" s="50"/>
       <c r="R66" s="35"/>
       <c r="S66" s="45">
-        <v>2.3780000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="T66" s="45">
-        <v>2.887</v>
+        <v>2.6829999999999998</v>
       </c>
       <c r="U66" s="45">
         <v>0</v>
@@ -5556,7 +5562,7 @@
       <c r="AI66" s="34"/>
       <c r="AJ66" s="54"/>
     </row>
-    <row r="67" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" s="60" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="50">
         <v>1</v>
       </c>
@@ -5564,13 +5570,13 @@
         <v>14</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E67" s="49" t="s">
-        <v>90</v>
+        <v>317</v>
       </c>
       <c r="F67" s="49"/>
       <c r="G67" s="35"/>
@@ -5586,10 +5592,10 @@
       <c r="Q67" s="50"/>
       <c r="R67" s="35"/>
       <c r="S67" s="45">
-        <v>0.25</v>
+        <v>2.3780000000000001</v>
       </c>
       <c r="T67" s="45">
-        <v>0.625</v>
+        <v>2.887</v>
       </c>
       <c r="U67" s="45">
         <v>0</v>
@@ -5612,107 +5618,103 @@
       <c r="AI67" s="34"/>
       <c r="AJ67" s="54"/>
     </row>
-    <row r="68" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
+    <row r="68" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="50">
+        <v>1</v>
+      </c>
+      <c r="B68" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D68" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E68" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F68" s="49"/>
+      <c r="G68" s="35"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="35"/>
+      <c r="K68" s="35"/>
+      <c r="L68" s="35"/>
+      <c r="M68" s="35"/>
+      <c r="N68" s="35"/>
+      <c r="O68" s="35"/>
+      <c r="P68" s="50"/>
+      <c r="Q68" s="50"/>
+      <c r="R68" s="35"/>
+      <c r="S68" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="T68" s="45">
+        <v>0.625</v>
+      </c>
+      <c r="U68" s="45">
+        <v>0</v>
+      </c>
+      <c r="V68" s="45">
+        <v>0</v>
+      </c>
+      <c r="W68" s="45"/>
+      <c r="X68" s="45"/>
+      <c r="Y68" s="35"/>
+      <c r="Z68" s="34"/>
+      <c r="AA68" s="34"/>
+      <c r="AB68" s="34"/>
+      <c r="AC68" s="34"/>
+      <c r="AD68" s="54"/>
+      <c r="AE68" s="34"/>
+      <c r="AF68" s="34"/>
+      <c r="AG68" s="34"/>
+      <c r="AH68" s="34"/>
+      <c r="AI68" s="34"/>
+      <c r="AJ68" s="54"/>
+    </row>
+    <row r="69" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B69" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
-      <c r="O68" s="14"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="16"/>
-      <c r="S68" s="17"/>
-      <c r="T68" s="17"/>
-      <c r="U68" s="17"/>
-      <c r="V68" s="17"/>
-      <c r="W68" s="17"/>
-      <c r="X68" s="17"/>
-      <c r="Y68" s="14"/>
-      <c r="Z68" s="16"/>
-      <c r="AA68" s="16"/>
-      <c r="AB68" s="16"/>
-      <c r="AC68" s="16"/>
-      <c r="AD68" s="16"/>
-      <c r="AE68" s="16"/>
-      <c r="AF68" s="16"/>
-      <c r="AG68" s="16"/>
-      <c r="AH68" s="16"/>
-      <c r="AI68" s="16"/>
-      <c r="AJ68" s="16"/>
-    </row>
-    <row r="69" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E69" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="F69" s="21"/>
-      <c r="G69" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="8"/>
-      <c r="O69" s="8"/>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="9"/>
-      <c r="R69" s="7"/>
-      <c r="S69" s="10">
-        <v>1</v>
-      </c>
-      <c r="T69" s="10">
-        <v>10.5</v>
-      </c>
-      <c r="U69" s="10">
-        <v>0</v>
-      </c>
-      <c r="V69" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="W69" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="X69" s="10"/>
-      <c r="Y69" s="8"/>
-      <c r="Z69" s="7"/>
-      <c r="AA69" s="11"/>
-      <c r="AB69" s="11"/>
-      <c r="AC69" s="7"/>
-      <c r="AD69" s="7"/>
-      <c r="AE69" s="7"/>
-      <c r="AF69" s="7"/>
-      <c r="AG69" s="11"/>
-      <c r="AH69" s="11"/>
-      <c r="AI69" s="7"/>
-      <c r="AJ69" s="7"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="14"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="16"/>
+      <c r="S69" s="17"/>
+      <c r="T69" s="17"/>
+      <c r="U69" s="17"/>
+      <c r="V69" s="17"/>
+      <c r="W69" s="17"/>
+      <c r="X69" s="17"/>
+      <c r="Y69" s="14"/>
+      <c r="Z69" s="16"/>
+      <c r="AA69" s="16"/>
+      <c r="AB69" s="16"/>
+      <c r="AC69" s="16"/>
+      <c r="AD69" s="16"/>
+      <c r="AE69" s="16"/>
+      <c r="AF69" s="16"/>
+      <c r="AG69" s="16"/>
+      <c r="AH69" s="16"/>
+      <c r="AI69" s="16"/>
+      <c r="AJ69" s="16"/>
     </row>
     <row r="70" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
@@ -5722,13 +5724,13 @@
         <v>14</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="F70" s="21"/>
       <c r="G70" s="8" t="s">
@@ -5749,16 +5751,16 @@
         <v>1</v>
       </c>
       <c r="T70" s="10">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U70" s="10">
         <v>0</v>
       </c>
       <c r="V70" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W70" s="10" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="X70" s="10"/>
       <c r="Y70" s="8"/>
@@ -5782,13 +5784,13 @@
         <v>14</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="F71" s="21"/>
       <c r="G71" s="8" t="s">
@@ -5804,23 +5806,23 @@
       <c r="O71" s="8"/>
       <c r="P71" s="9"/>
       <c r="Q71" s="9"/>
-      <c r="R71" s="8"/>
+      <c r="R71" s="7"/>
       <c r="S71" s="10">
         <v>1</v>
       </c>
       <c r="T71" s="10">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U71" s="10">
         <v>0</v>
       </c>
       <c r="V71" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="W71" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="X71" s="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="W71" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="X71" s="10"/>
       <c r="Y71" s="8"/>
       <c r="Z71" s="7"/>
       <c r="AA71" s="11"/>
@@ -5834,64 +5836,64 @@
       <c r="AI71" s="7"/>
       <c r="AJ71" s="7"/>
     </row>
-    <row r="72" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>321</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C72" s="43" t="s">
-        <v>179</v>
+      <c r="C72" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E72" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="F72" s="51"/>
+      <c r="E72" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F72" s="21"/>
       <c r="G72" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H72" s="43"/>
-      <c r="I72" s="43"/>
-      <c r="J72" s="43"/>
-      <c r="K72" s="43"/>
-      <c r="L72" s="43"/>
-      <c r="M72" s="43"/>
-      <c r="N72" s="43"/>
-      <c r="O72" s="43"/>
-      <c r="P72" s="52"/>
-      <c r="Q72" s="52"/>
-      <c r="R72" s="11"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="9"/>
+      <c r="R72" s="8"/>
       <c r="S72" s="10">
         <v>1</v>
       </c>
       <c r="T72" s="10">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U72" s="10">
         <v>0</v>
       </c>
       <c r="V72" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="W72" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="X72" s="44"/>
-      <c r="Y72" s="43"/>
-      <c r="Z72" s="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="W72" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="X72" s="8"/>
+      <c r="Y72" s="8"/>
+      <c r="Z72" s="7"/>
       <c r="AA72" s="11"/>
       <c r="AB72" s="11"/>
-      <c r="AC72" s="11"/>
+      <c r="AC72" s="7"/>
       <c r="AD72" s="7"/>
-      <c r="AE72" s="11"/>
-      <c r="AF72" s="11"/>
+      <c r="AE72" s="7"/>
+      <c r="AF72" s="7"/>
       <c r="AG72" s="11"/>
       <c r="AH72" s="11"/>
-      <c r="AI72" s="11"/>
+      <c r="AI72" s="7"/>
       <c r="AJ72" s="7"/>
     </row>
     <row r="73" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5902,15 +5904,15 @@
         <v>14</v>
       </c>
       <c r="C73" s="43" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E73" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="F73" s="43"/>
+        <v>210</v>
+      </c>
+      <c r="F73" s="51"/>
       <c r="G73" s="8" t="s">
         <v>36</v>
       </c>
@@ -5929,16 +5931,16 @@
         <v>1</v>
       </c>
       <c r="T73" s="10">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U73" s="10">
         <v>0</v>
       </c>
       <c r="V73" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W73" s="44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X73" s="44"/>
       <c r="Y73" s="43"/>
@@ -5947,7 +5949,7 @@
       <c r="AB73" s="11"/>
       <c r="AC73" s="11"/>
       <c r="AD73" s="7"/>
-      <c r="AE73" s="43"/>
+      <c r="AE73" s="11"/>
       <c r="AF73" s="11"/>
       <c r="AG73" s="11"/>
       <c r="AH73" s="11"/>
@@ -5962,13 +5964,13 @@
         <v>14</v>
       </c>
       <c r="C74" s="43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E74" s="51" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="F74" s="43"/>
       <c r="G74" s="8" t="s">
@@ -5989,16 +5991,16 @@
         <v>1</v>
       </c>
       <c r="T74" s="10">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U74" s="10">
         <v>0</v>
       </c>
       <c r="V74" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W74" s="44" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="X74" s="44"/>
       <c r="Y74" s="43"/>
@@ -6022,13 +6024,13 @@
         <v>14</v>
       </c>
       <c r="C75" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E75" s="51" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F75" s="43"/>
       <c r="G75" s="8" t="s">
@@ -6049,16 +6051,16 @@
         <v>1</v>
       </c>
       <c r="T75" s="10">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U75" s="10">
         <v>0</v>
       </c>
       <c r="V75" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W75" s="44" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X75" s="44"/>
       <c r="Y75" s="43"/>
@@ -6067,7 +6069,7 @@
       <c r="AB75" s="11"/>
       <c r="AC75" s="11"/>
       <c r="AD75" s="7"/>
-      <c r="AE75" s="11"/>
+      <c r="AE75" s="43"/>
       <c r="AF75" s="11"/>
       <c r="AG75" s="11"/>
       <c r="AH75" s="11"/>
@@ -6082,13 +6084,13 @@
         <v>14</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E76" s="51" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="F76" s="43"/>
       <c r="G76" s="8" t="s">
@@ -6109,16 +6111,16 @@
         <v>1</v>
       </c>
       <c r="T76" s="10">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U76" s="10">
         <v>0</v>
       </c>
       <c r="V76" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W76" s="44" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="X76" s="44"/>
       <c r="Y76" s="43"/>
@@ -6142,13 +6144,13 @@
         <v>14</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E77" s="51" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F77" s="43"/>
       <c r="G77" s="8" t="s">
@@ -6169,16 +6171,16 @@
         <v>1</v>
       </c>
       <c r="T77" s="10">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="U77" s="10">
         <v>0</v>
       </c>
       <c r="V77" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W77" s="44" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="X77" s="44"/>
       <c r="Y77" s="43"/>
@@ -6186,13 +6188,13 @@
       <c r="AA77" s="11"/>
       <c r="AB77" s="11"/>
       <c r="AC77" s="11"/>
-      <c r="AD77" s="34"/>
+      <c r="AD77" s="7"/>
       <c r="AE77" s="11"/>
       <c r="AF77" s="11"/>
       <c r="AG77" s="11"/>
       <c r="AH77" s="11"/>
       <c r="AI77" s="11"/>
-      <c r="AJ77" s="34"/>
+      <c r="AJ77" s="7"/>
     </row>
     <row r="78" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
@@ -6202,13 +6204,13 @@
         <v>14</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E78" s="51" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="F78" s="43"/>
       <c r="G78" s="8" t="s">
@@ -6229,16 +6231,16 @@
         <v>1</v>
       </c>
       <c r="T78" s="10">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="U78" s="10">
         <v>0</v>
       </c>
       <c r="V78" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W78" s="44" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="X78" s="44"/>
       <c r="Y78" s="43"/>
@@ -6246,13 +6248,13 @@
       <c r="AA78" s="11"/>
       <c r="AB78" s="11"/>
       <c r="AC78" s="11"/>
-      <c r="AD78" s="7"/>
+      <c r="AD78" s="34"/>
       <c r="AE78" s="11"/>
       <c r="AF78" s="11"/>
       <c r="AG78" s="11"/>
       <c r="AH78" s="11"/>
       <c r="AI78" s="11"/>
-      <c r="AJ78" s="7"/>
+      <c r="AJ78" s="34"/>
     </row>
     <row r="79" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
@@ -6262,13 +6264,13 @@
         <v>14</v>
       </c>
       <c r="C79" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E79" s="51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F79" s="43"/>
       <c r="G79" s="8" t="s">
@@ -6289,16 +6291,16 @@
         <v>1</v>
       </c>
       <c r="T79" s="10">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="U79" s="10">
         <v>0</v>
       </c>
       <c r="V79" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W79" s="44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X79" s="44"/>
       <c r="Y79" s="43"/>
@@ -6314,125 +6316,125 @@
       <c r="AI79" s="11"/>
       <c r="AJ79" s="7"/>
     </row>
-    <row r="80" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>321</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="8" t="s">
-        <v>185</v>
+      <c r="C80" s="43" t="s">
+        <v>224</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E80" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F80" s="21"/>
+      <c r="E80" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="F80" s="43"/>
       <c r="G80" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="8"/>
-      <c r="M80" s="8"/>
-      <c r="N80" s="8"/>
-      <c r="O80" s="8"/>
-      <c r="P80" s="9"/>
-      <c r="Q80" s="9"/>
-      <c r="R80" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="H80" s="43"/>
+      <c r="I80" s="43"/>
+      <c r="J80" s="43"/>
+      <c r="K80" s="43"/>
+      <c r="L80" s="43"/>
+      <c r="M80" s="43"/>
+      <c r="N80" s="43"/>
+      <c r="O80" s="43"/>
+      <c r="P80" s="52"/>
+      <c r="Q80" s="52"/>
+      <c r="R80" s="11"/>
       <c r="S80" s="10">
         <v>1</v>
       </c>
       <c r="T80" s="10">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="U80" s="10">
         <v>0</v>
       </c>
       <c r="V80" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="W80" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="X80" s="10"/>
-      <c r="Y80" s="8"/>
-      <c r="Z80" s="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="W80" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="X80" s="44"/>
+      <c r="Y80" s="43"/>
+      <c r="Z80" s="11"/>
       <c r="AA80" s="11"/>
       <c r="AB80" s="11"/>
-      <c r="AC80" s="7"/>
+      <c r="AC80" s="11"/>
       <c r="AD80" s="7"/>
-      <c r="AE80" s="7"/>
-      <c r="AF80" s="7"/>
+      <c r="AE80" s="11"/>
+      <c r="AF80" s="11"/>
       <c r="AG80" s="11"/>
       <c r="AH80" s="11"/>
-      <c r="AI80" s="7"/>
+      <c r="AI80" s="11"/>
       <c r="AJ80" s="7"/>
     </row>
     <row r="81" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D81" s="5" t="s">
+      <c r="B81" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E81" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="F81" s="55"/>
-      <c r="G81" s="5" t="s">
+      <c r="E81" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="21"/>
+      <c r="G81" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
-      <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-      <c r="P81" s="19"/>
-      <c r="Q81" s="19"/>
-      <c r="R81" s="56"/>
-      <c r="S81" s="57">
-        <v>2.25</v>
-      </c>
-      <c r="T81" s="57">
-        <v>10.5</v>
-      </c>
-      <c r="U81" s="57">
-        <v>0</v>
-      </c>
-      <c r="V81" s="57">
-        <v>0.25</v>
-      </c>
-      <c r="W81" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="X81" s="57"/>
-      <c r="Y81" s="5"/>
-      <c r="Z81" s="56"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="8"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="8"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="9"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="10">
+        <v>1</v>
+      </c>
+      <c r="T81" s="10">
+        <v>5</v>
+      </c>
+      <c r="U81" s="10">
+        <v>0</v>
+      </c>
+      <c r="V81" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="W81" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="X81" s="10"/>
+      <c r="Y81" s="8"/>
+      <c r="Z81" s="7"/>
       <c r="AA81" s="11"/>
       <c r="AB81" s="11"/>
       <c r="AC81" s="7"/>
-      <c r="AD81" s="13"/>
+      <c r="AD81" s="7"/>
       <c r="AE81" s="7"/>
       <c r="AF81" s="7"/>
       <c r="AG81" s="11"/>
       <c r="AH81" s="11"/>
       <c r="AI81" s="7"/>
-      <c r="AJ81" s="13"/>
+      <c r="AJ81" s="7"/>
     </row>
     <row r="82" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
@@ -6442,13 +6444,13 @@
         <v>14</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E82" s="55" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F82" s="55"/>
       <c r="G82" s="5" t="s">
@@ -6464,21 +6466,21 @@
       <c r="O82" s="5"/>
       <c r="P82" s="19"/>
       <c r="Q82" s="19"/>
-      <c r="R82" s="5"/>
+      <c r="R82" s="56"/>
       <c r="S82" s="57">
         <v>2.25</v>
       </c>
       <c r="T82" s="57">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U82" s="57">
         <v>0</v>
       </c>
       <c r="V82" s="57">
-        <v>0.25</v>
-      </c>
-      <c r="W82" s="19" t="s">
-        <v>144</v>
+        <v>0.5</v>
+      </c>
+      <c r="W82" s="57" t="s">
+        <v>151</v>
       </c>
       <c r="X82" s="57"/>
       <c r="Y82" s="5"/>
@@ -6502,13 +6504,13 @@
         <v>14</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E83" s="55" t="s">
-        <v>225</v>
+        <v>144</v>
       </c>
       <c r="F83" s="55"/>
       <c r="G83" s="5" t="s">
@@ -6529,16 +6531,16 @@
         <v>2.25</v>
       </c>
       <c r="T83" s="57">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U83" s="57">
         <v>0</v>
       </c>
       <c r="V83" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W83" s="19" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
       <c r="X83" s="57"/>
       <c r="Y83" s="5"/>
@@ -6562,13 +6564,13 @@
         <v>14</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E84" s="55" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="F84" s="55"/>
       <c r="G84" s="5" t="s">
@@ -6589,16 +6591,16 @@
         <v>2.25</v>
       </c>
       <c r="T84" s="57">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U84" s="57">
         <v>0</v>
       </c>
       <c r="V84" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W84" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X84" s="57"/>
       <c r="Y84" s="5"/>
@@ -6622,13 +6624,13 @@
         <v>14</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E85" s="55" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="F85" s="55"/>
       <c r="G85" s="5" t="s">
@@ -6649,16 +6651,16 @@
         <v>2.25</v>
       </c>
       <c r="T85" s="57">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U85" s="57">
         <v>0</v>
       </c>
       <c r="V85" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W85" s="19" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="X85" s="57"/>
       <c r="Y85" s="5"/>
@@ -6682,13 +6684,13 @@
         <v>14</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E86" s="55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F86" s="55"/>
       <c r="G86" s="5" t="s">
@@ -6709,16 +6711,16 @@
         <v>2.25</v>
       </c>
       <c r="T86" s="57">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U86" s="57">
         <v>0</v>
       </c>
       <c r="V86" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W86" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="X86" s="57"/>
       <c r="Y86" s="5"/>
@@ -6742,13 +6744,13 @@
         <v>14</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E87" s="55" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="F87" s="55"/>
       <c r="G87" s="5" t="s">
@@ -6769,16 +6771,16 @@
         <v>2.25</v>
       </c>
       <c r="T87" s="57">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U87" s="57">
         <v>0</v>
       </c>
       <c r="V87" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W87" s="19" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="X87" s="57"/>
       <c r="Y87" s="5"/>
@@ -6802,13 +6804,13 @@
         <v>14</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E88" s="55" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="F88" s="55"/>
       <c r="G88" s="5" t="s">
@@ -6829,16 +6831,16 @@
         <v>2.25</v>
       </c>
       <c r="T88" s="57">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U88" s="57">
         <v>0</v>
       </c>
       <c r="V88" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W88" s="19" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="X88" s="57"/>
       <c r="Y88" s="5"/>
@@ -6862,13 +6864,13 @@
         <v>14</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E89" s="55" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="F89" s="55"/>
       <c r="G89" s="5" t="s">
@@ -6889,16 +6891,16 @@
         <v>2.25</v>
       </c>
       <c r="T89" s="57">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="U89" s="57">
         <v>0</v>
       </c>
       <c r="V89" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W89" s="19" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="X89" s="57"/>
       <c r="Y89" s="5"/>
@@ -6914,67 +6916,67 @@
       <c r="AI89" s="7"/>
       <c r="AJ89" s="13"/>
     </row>
-    <row r="90" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B90" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C90" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="D90" s="35" t="s">
+      <c r="B90" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E90" s="49" t="s">
-        <v>156</v>
-      </c>
-      <c r="F90" s="49"/>
-      <c r="G90" s="35" t="s">
+      <c r="E90" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="F90" s="55"/>
+      <c r="G90" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H90" s="35"/>
-      <c r="I90" s="35"/>
-      <c r="J90" s="35"/>
-      <c r="K90" s="35"/>
-      <c r="L90" s="35"/>
-      <c r="M90" s="35"/>
-      <c r="N90" s="35"/>
-      <c r="O90" s="35"/>
-      <c r="P90" s="50"/>
-      <c r="Q90" s="50"/>
-      <c r="R90" s="35"/>
-      <c r="S90" s="45">
-        <v>3.5</v>
-      </c>
-      <c r="T90" s="45">
-        <v>10.5</v>
-      </c>
-      <c r="U90" s="45">
-        <v>0</v>
-      </c>
-      <c r="V90" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="W90" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="X90" s="45"/>
-      <c r="Y90" s="35"/>
-      <c r="Z90" s="34"/>
+      <c r="H90" s="5"/>
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+      <c r="K90" s="5"/>
+      <c r="L90" s="5"/>
+      <c r="M90" s="5"/>
+      <c r="N90" s="5"/>
+      <c r="O90" s="5"/>
+      <c r="P90" s="19"/>
+      <c r="Q90" s="19"/>
+      <c r="R90" s="5"/>
+      <c r="S90" s="57">
+        <v>2.25</v>
+      </c>
+      <c r="T90" s="57">
+        <v>6.5</v>
+      </c>
+      <c r="U90" s="57">
+        <v>0</v>
+      </c>
+      <c r="V90" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="W90" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="X90" s="57"/>
+      <c r="Y90" s="5"/>
+      <c r="Z90" s="56"/>
       <c r="AA90" s="11"/>
       <c r="AB90" s="11"/>
-      <c r="AC90" s="11"/>
+      <c r="AC90" s="7"/>
       <c r="AD90" s="13"/>
-      <c r="AE90" s="11"/>
-      <c r="AF90" s="11"/>
+      <c r="AE90" s="7"/>
+      <c r="AF90" s="7"/>
       <c r="AG90" s="11"/>
       <c r="AH90" s="11"/>
-      <c r="AI90" s="11"/>
+      <c r="AI90" s="7"/>
       <c r="AJ90" s="13"/>
     </row>
-    <row r="91" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>321</v>
       </c>
@@ -6982,13 +6984,13 @@
         <v>14</v>
       </c>
       <c r="C91" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D91" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E91" s="49" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F91" s="49"/>
       <c r="G91" s="35" t="s">
@@ -7009,29 +7011,29 @@
         <v>3.5</v>
       </c>
       <c r="T91" s="45">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U91" s="45">
         <v>0</v>
       </c>
       <c r="V91" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W91" s="50" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="X91" s="45"/>
       <c r="Y91" s="35"/>
       <c r="Z91" s="34"/>
       <c r="AA91" s="11"/>
       <c r="AB91" s="11"/>
-      <c r="AC91" s="7"/>
+      <c r="AC91" s="11"/>
       <c r="AD91" s="13"/>
-      <c r="AE91" s="7"/>
-      <c r="AF91" s="7"/>
+      <c r="AE91" s="11"/>
+      <c r="AF91" s="11"/>
       <c r="AG91" s="11"/>
       <c r="AH91" s="11"/>
-      <c r="AI91" s="7"/>
+      <c r="AI91" s="11"/>
       <c r="AJ91" s="13"/>
     </row>
     <row r="92" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7042,13 +7044,13 @@
         <v>14</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D92" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E92" s="49" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="F92" s="49"/>
       <c r="G92" s="35" t="s">
@@ -7069,16 +7071,16 @@
         <v>3.5</v>
       </c>
       <c r="T92" s="45">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U92" s="45">
         <v>0</v>
       </c>
       <c r="V92" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W92" s="50" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="X92" s="45"/>
       <c r="Y92" s="35"/>
@@ -7102,13 +7104,13 @@
         <v>14</v>
       </c>
       <c r="C93" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D93" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E93" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F93" s="49"/>
       <c r="G93" s="35" t="s">
@@ -7129,16 +7131,16 @@
         <v>3.5</v>
       </c>
       <c r="T93" s="45">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U93" s="45">
         <v>0</v>
       </c>
       <c r="V93" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W93" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X93" s="45"/>
       <c r="Y93" s="35"/>
@@ -7162,13 +7164,13 @@
         <v>14</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D94" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E94" s="49" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F94" s="49"/>
       <c r="G94" s="35" t="s">
@@ -7189,16 +7191,16 @@
         <v>3.5</v>
       </c>
       <c r="T94" s="45">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U94" s="45">
         <v>0</v>
       </c>
       <c r="V94" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W94" s="50" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="X94" s="45"/>
       <c r="Y94" s="35"/>
@@ -7222,13 +7224,13 @@
         <v>14</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D95" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E95" s="49" t="s">
-        <v>226</v>
+        <v>142</v>
       </c>
       <c r="F95" s="49"/>
       <c r="G95" s="35" t="s">
@@ -7249,16 +7251,16 @@
         <v>3.5</v>
       </c>
       <c r="T95" s="45">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U95" s="45">
         <v>0</v>
       </c>
       <c r="V95" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W95" s="50" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="X95" s="45"/>
       <c r="Y95" s="35"/>
@@ -7282,13 +7284,13 @@
         <v>14</v>
       </c>
       <c r="C96" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D96" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E96" s="49" t="s">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="F96" s="49"/>
       <c r="G96" s="35" t="s">
@@ -7309,16 +7311,16 @@
         <v>3.5</v>
       </c>
       <c r="T96" s="45">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U96" s="45">
         <v>0</v>
       </c>
       <c r="V96" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W96" s="50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="X96" s="45"/>
       <c r="Y96" s="35"/>
@@ -7342,13 +7344,13 @@
         <v>14</v>
       </c>
       <c r="C97" s="35" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D97" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E97" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F97" s="49"/>
       <c r="G97" s="35" t="s">
@@ -7369,16 +7371,16 @@
         <v>3.5</v>
       </c>
       <c r="T97" s="45">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U97" s="45">
         <v>0</v>
       </c>
       <c r="V97" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W97" s="50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X97" s="45"/>
       <c r="Y97" s="35"/>
@@ -7402,13 +7404,13 @@
         <v>14</v>
       </c>
       <c r="C98" s="35" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="D98" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E98" s="49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F98" s="49"/>
       <c r="G98" s="35" t="s">
@@ -7429,16 +7431,16 @@
         <v>3.5</v>
       </c>
       <c r="T98" s="45">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="U98" s="45">
         <v>0</v>
       </c>
       <c r="V98" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W98" s="50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X98" s="45"/>
       <c r="Y98" s="35"/>
@@ -7462,13 +7464,13 @@
         <v>14</v>
       </c>
       <c r="C99" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D99" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E99" s="49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F99" s="49"/>
       <c r="G99" s="35" t="s">
@@ -7489,16 +7491,16 @@
         <v>3.5</v>
       </c>
       <c r="T99" s="45">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="U99" s="45">
         <v>0</v>
       </c>
       <c r="V99" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W99" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X99" s="45"/>
       <c r="Y99" s="35"/>
@@ -7522,13 +7524,13 @@
         <v>14</v>
       </c>
       <c r="C100" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D100" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E100" s="49" t="s">
-        <v>217</v>
+        <v>155</v>
       </c>
       <c r="F100" s="49"/>
       <c r="G100" s="35" t="s">
@@ -7549,16 +7551,16 @@
         <v>3.5</v>
       </c>
       <c r="T100" s="45">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="U100" s="45">
         <v>0</v>
       </c>
       <c r="V100" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W100" s="50" t="s">
-        <v>217</v>
+        <v>155</v>
       </c>
       <c r="X100" s="45"/>
       <c r="Y100" s="35"/>
@@ -7582,13 +7584,13 @@
         <v>14</v>
       </c>
       <c r="C101" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D101" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E101" s="49" t="s">
-        <v>18</v>
+        <v>217</v>
       </c>
       <c r="F101" s="49"/>
       <c r="G101" s="35" t="s">
@@ -7609,16 +7611,16 @@
         <v>3.5</v>
       </c>
       <c r="T101" s="45">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="U101" s="45">
         <v>0</v>
       </c>
       <c r="V101" s="10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W101" s="50" t="s">
-        <v>18</v>
+        <v>217</v>
       </c>
       <c r="X101" s="45"/>
       <c r="Y101" s="35"/>
@@ -7638,51 +7640,51 @@
       <c r="A102" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D102" s="5" t="s">
+      <c r="B102" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C102" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="D102" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="E102" s="55" t="s">
-        <v>158</v>
-      </c>
-      <c r="F102" s="55"/>
-      <c r="G102" s="5" t="s">
+      <c r="E102" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="F102" s="49"/>
+      <c r="G102" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="H102" s="5"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="5"/>
-      <c r="K102" s="5"/>
-      <c r="L102" s="5"/>
-      <c r="M102" s="5"/>
-      <c r="N102" s="5"/>
-      <c r="O102" s="5"/>
-      <c r="P102" s="19"/>
-      <c r="Q102" s="19"/>
-      <c r="R102" s="5"/>
-      <c r="S102" s="57">
-        <v>4.75</v>
-      </c>
-      <c r="T102" s="57">
-        <v>10.5</v>
-      </c>
-      <c r="U102" s="57">
-        <v>0</v>
-      </c>
-      <c r="V102" s="57">
-        <v>0.25</v>
-      </c>
-      <c r="W102" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="X102" s="57"/>
-      <c r="Y102" s="5"/>
-      <c r="Z102" s="56"/>
+      <c r="H102" s="35"/>
+      <c r="I102" s="35"/>
+      <c r="J102" s="35"/>
+      <c r="K102" s="35"/>
+      <c r="L102" s="35"/>
+      <c r="M102" s="35"/>
+      <c r="N102" s="35"/>
+      <c r="O102" s="35"/>
+      <c r="P102" s="50"/>
+      <c r="Q102" s="50"/>
+      <c r="R102" s="35"/>
+      <c r="S102" s="45">
+        <v>3.5</v>
+      </c>
+      <c r="T102" s="45">
+        <v>5</v>
+      </c>
+      <c r="U102" s="45">
+        <v>0</v>
+      </c>
+      <c r="V102" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="W102" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="X102" s="45"/>
+      <c r="Y102" s="35"/>
+      <c r="Z102" s="34"/>
       <c r="AA102" s="11"/>
       <c r="AB102" s="11"/>
       <c r="AC102" s="7"/>
@@ -7702,13 +7704,13 @@
         <v>14</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E103" s="55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F103" s="55"/>
       <c r="G103" s="5" t="s">
@@ -7729,16 +7731,16 @@
         <v>4.75</v>
       </c>
       <c r="T103" s="57">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U103" s="57">
         <v>0</v>
       </c>
       <c r="V103" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W103" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X103" s="57"/>
       <c r="Y103" s="5"/>
@@ -7762,13 +7764,13 @@
         <v>14</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E104" s="55" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="F104" s="55"/>
       <c r="G104" s="5" t="s">
@@ -7789,16 +7791,16 @@
         <v>4.75</v>
       </c>
       <c r="T104" s="57">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U104" s="57">
         <v>0</v>
       </c>
       <c r="V104" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W104" s="19" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="X104" s="57"/>
       <c r="Y104" s="5"/>
@@ -7822,13 +7824,13 @@
         <v>14</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E105" s="55" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="F105" s="55"/>
       <c r="G105" s="5" t="s">
@@ -7849,16 +7851,16 @@
         <v>4.75</v>
       </c>
       <c r="T105" s="57">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U105" s="57">
         <v>0</v>
       </c>
       <c r="V105" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W105" s="19" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="X105" s="57"/>
       <c r="Y105" s="5"/>
@@ -7882,13 +7884,13 @@
         <v>14</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E106" s="55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F106" s="55"/>
       <c r="G106" s="5" t="s">
@@ -7909,16 +7911,16 @@
         <v>4.75</v>
       </c>
       <c r="T106" s="57">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U106" s="57">
         <v>0</v>
       </c>
       <c r="V106" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W106" s="19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="X106" s="57"/>
       <c r="Y106" s="5"/>
@@ -7942,13 +7944,13 @@
         <v>14</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E107" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F107" s="55"/>
       <c r="G107" s="5" t="s">
@@ -7969,16 +7971,16 @@
         <v>4.75</v>
       </c>
       <c r="T107" s="57">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U107" s="57">
         <v>0</v>
       </c>
       <c r="V107" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W107" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X107" s="57"/>
       <c r="Y107" s="5"/>
@@ -8002,13 +8004,13 @@
         <v>14</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E108" s="55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F108" s="55"/>
       <c r="G108" s="5" t="s">
@@ -8029,16 +8031,16 @@
         <v>4.75</v>
       </c>
       <c r="T108" s="57">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U108" s="57">
         <v>0</v>
       </c>
       <c r="V108" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W108" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X108" s="57"/>
       <c r="Y108" s="5"/>
@@ -8062,13 +8064,13 @@
         <v>14</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E109" s="55" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="F109" s="55"/>
       <c r="G109" s="5" t="s">
@@ -8089,16 +8091,16 @@
         <v>4.75</v>
       </c>
       <c r="T109" s="57">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U109" s="57">
         <v>0</v>
       </c>
       <c r="V109" s="57">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="W109" s="19" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="X109" s="57"/>
       <c r="Y109" s="5"/>
@@ -8114,111 +8116,107 @@
       <c r="AI109" s="7"/>
       <c r="AJ109" s="13"/>
     </row>
-    <row r="110" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
+    <row r="110" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E110" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F110" s="55"/>
+      <c r="G110" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5"/>
+      <c r="M110" s="5"/>
+      <c r="N110" s="5"/>
+      <c r="O110" s="5"/>
+      <c r="P110" s="19"/>
+      <c r="Q110" s="19"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="57">
+        <v>4.75</v>
+      </c>
+      <c r="T110" s="57">
+        <v>7</v>
+      </c>
+      <c r="U110" s="57">
+        <v>0</v>
+      </c>
+      <c r="V110" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="W110" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="X110" s="57"/>
+      <c r="Y110" s="5"/>
+      <c r="Z110" s="56"/>
+      <c r="AA110" s="11"/>
+      <c r="AB110" s="11"/>
+      <c r="AC110" s="7"/>
+      <c r="AD110" s="13"/>
+      <c r="AE110" s="7"/>
+      <c r="AF110" s="7"/>
+      <c r="AG110" s="11"/>
+      <c r="AH110" s="11"/>
+      <c r="AI110" s="7"/>
+      <c r="AJ110" s="13"/>
+    </row>
+    <row r="111" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B111" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
-      <c r="H110" s="14"/>
-      <c r="I110" s="14"/>
-      <c r="J110" s="14"/>
-      <c r="K110" s="14"/>
-      <c r="L110" s="14"/>
-      <c r="M110" s="14"/>
-      <c r="N110" s="14"/>
-      <c r="O110" s="14"/>
-      <c r="P110" s="15"/>
-      <c r="Q110" s="15"/>
-      <c r="R110" s="16"/>
-      <c r="S110" s="17"/>
-      <c r="T110" s="17"/>
-      <c r="U110" s="17"/>
-      <c r="V110" s="17"/>
-      <c r="W110" s="17"/>
-      <c r="X110" s="17"/>
-      <c r="Y110" s="14"/>
-      <c r="Z110" s="16"/>
-      <c r="AA110" s="16"/>
-      <c r="AB110" s="16"/>
-      <c r="AC110" s="16"/>
-      <c r="AD110" s="16"/>
-      <c r="AE110" s="16"/>
-      <c r="AF110" s="16"/>
-      <c r="AG110" s="16"/>
-      <c r="AH110" s="16"/>
-      <c r="AI110" s="16"/>
-      <c r="AJ110" s="16"/>
-    </row>
-    <row r="111" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="B111" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C111" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="D111" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="E111" s="49"/>
-      <c r="F111" s="49"/>
-      <c r="G111" s="35"/>
-      <c r="H111" s="35"/>
-      <c r="I111" s="35"/>
-      <c r="J111" s="35"/>
-      <c r="K111" s="35"/>
-      <c r="L111" s="35"/>
-      <c r="M111" s="35"/>
-      <c r="N111" s="35"/>
-      <c r="O111" s="35"/>
-      <c r="P111" s="50"/>
-      <c r="Q111" s="50"/>
-      <c r="R111" s="35"/>
-      <c r="S111" s="45">
-        <v>1</v>
-      </c>
-      <c r="T111" s="45">
-        <v>4</v>
-      </c>
-      <c r="U111" s="45">
-        <v>0</v>
-      </c>
-      <c r="V111" s="45">
-        <v>0</v>
-      </c>
-      <c r="W111" s="50"/>
-      <c r="X111" s="45"/>
-      <c r="Y111" s="35"/>
-      <c r="Z111" s="34"/>
-      <c r="AA111" s="11"/>
-      <c r="AB111" s="11"/>
-      <c r="AC111" s="7"/>
-      <c r="AD111" s="13"/>
-      <c r="AE111" s="35" t="s">
-        <v>234</v>
-      </c>
-      <c r="AF111" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="AG111" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH111" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI111" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ111" s="13"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="14"/>
+      <c r="J111" s="14"/>
+      <c r="K111" s="14"/>
+      <c r="L111" s="14"/>
+      <c r="M111" s="14"/>
+      <c r="N111" s="14"/>
+      <c r="O111" s="14"/>
+      <c r="P111" s="15"/>
+      <c r="Q111" s="15"/>
+      <c r="R111" s="16"/>
+      <c r="S111" s="17"/>
+      <c r="T111" s="17"/>
+      <c r="U111" s="17"/>
+      <c r="V111" s="17"/>
+      <c r="W111" s="17"/>
+      <c r="X111" s="17"/>
+      <c r="Y111" s="14"/>
+      <c r="Z111" s="16"/>
+      <c r="AA111" s="16"/>
+      <c r="AB111" s="16"/>
+      <c r="AC111" s="16"/>
+      <c r="AD111" s="16"/>
+      <c r="AE111" s="16"/>
+      <c r="AF111" s="16"/>
+      <c r="AG111" s="16"/>
+      <c r="AH111" s="16"/>
+      <c r="AI111" s="16"/>
+      <c r="AJ111" s="16"/>
     </row>
     <row r="112" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
@@ -8228,10 +8226,10 @@
         <v>14</v>
       </c>
       <c r="C112" s="35" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D112" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E112" s="49"/>
       <c r="F112" s="49"/>
@@ -8248,10 +8246,10 @@
       <c r="Q112" s="50"/>
       <c r="R112" s="35"/>
       <c r="S112" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T112" s="45">
-        <v>3.9529999999999998</v>
+        <v>4.0069999999999997</v>
       </c>
       <c r="U112" s="45">
         <v>0</v>
@@ -8267,11 +8265,21 @@
       <c r="AB112" s="11"/>
       <c r="AC112" s="7"/>
       <c r="AD112" s="13"/>
-      <c r="AE112" s="7"/>
-      <c r="AF112" s="7"/>
-      <c r="AG112" s="11"/>
-      <c r="AH112" s="11"/>
-      <c r="AI112" s="7"/>
+      <c r="AE112" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF112" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AG112" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH112" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI112" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ112" s="13"/>
     </row>
     <row r="113" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8282,10 +8290,10 @@
         <v>14</v>
       </c>
       <c r="C113" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D113" s="35" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E113" s="49"/>
       <c r="F113" s="49"/>
@@ -8302,10 +8310,10 @@
       <c r="Q113" s="50"/>
       <c r="R113" s="35"/>
       <c r="S113" s="45">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="T113" s="45">
-        <v>3.5</v>
+        <v>3.9529999999999998</v>
       </c>
       <c r="U113" s="45">
         <v>0</v>
@@ -8321,24 +8329,12 @@
       <c r="AB113" s="11"/>
       <c r="AC113" s="7"/>
       <c r="AD113" s="13"/>
-      <c r="AE113" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="AF113" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="AG113" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH113" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI113" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ113" s="13" t="s">
-        <v>231</v>
-      </c>
+      <c r="AE113" s="7"/>
+      <c r="AF113" s="7"/>
+      <c r="AG113" s="11"/>
+      <c r="AH113" s="11"/>
+      <c r="AI113" s="7"/>
+      <c r="AJ113" s="13"/>
     </row>
     <row r="114" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
@@ -8348,10 +8344,10 @@
         <v>14</v>
       </c>
       <c r="C114" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D114" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E114" s="49"/>
       <c r="F114" s="49"/>
@@ -8368,10 +8364,10 @@
       <c r="Q114" s="50"/>
       <c r="R114" s="35"/>
       <c r="S114" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T114" s="45">
-        <v>3.4529999999999998</v>
+        <v>3.5070000000000001</v>
       </c>
       <c r="U114" s="45">
         <v>0</v>
@@ -8387,12 +8383,24 @@
       <c r="AB114" s="11"/>
       <c r="AC114" s="7"/>
       <c r="AD114" s="13"/>
-      <c r="AE114" s="7"/>
-      <c r="AF114" s="7"/>
-      <c r="AG114" s="11"/>
-      <c r="AH114" s="11"/>
-      <c r="AI114" s="7"/>
-      <c r="AJ114" s="13"/>
+      <c r="AE114" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF114" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG114" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH114" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI114" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ114" s="13" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="115" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
@@ -8402,10 +8410,10 @@
         <v>14</v>
       </c>
       <c r="C115" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D115" s="35" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E115" s="49"/>
       <c r="F115" s="49"/>
@@ -8422,10 +8430,10 @@
       <c r="Q115" s="50"/>
       <c r="R115" s="35"/>
       <c r="S115" s="45">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="T115" s="45">
-        <v>3</v>
+        <v>3.4529999999999998</v>
       </c>
       <c r="U115" s="45">
         <v>0</v>
@@ -8441,24 +8449,12 @@
       <c r="AB115" s="11"/>
       <c r="AC115" s="7"/>
       <c r="AD115" s="13"/>
-      <c r="AE115" s="35" t="s">
-        <v>239</v>
-      </c>
-      <c r="AF115" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="AG115" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH115" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI115" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ115" s="13" t="s">
-        <v>256</v>
-      </c>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="11"/>
+      <c r="AH115" s="11"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="13"/>
     </row>
     <row r="116" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
@@ -8468,10 +8464,10 @@
         <v>14</v>
       </c>
       <c r="C116" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D116" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E116" s="49"/>
       <c r="F116" s="49"/>
@@ -8488,10 +8484,10 @@
       <c r="Q116" s="50"/>
       <c r="R116" s="35"/>
       <c r="S116" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T116" s="45">
-        <v>2.9529999999999998</v>
+        <v>3.0070000000000001</v>
       </c>
       <c r="U116" s="45">
         <v>0</v>
@@ -8507,12 +8503,24 @@
       <c r="AB116" s="11"/>
       <c r="AC116" s="7"/>
       <c r="AD116" s="13"/>
-      <c r="AE116" s="7"/>
-      <c r="AF116" s="7"/>
-      <c r="AG116" s="11"/>
-      <c r="AH116" s="11"/>
-      <c r="AI116" s="7"/>
-      <c r="AJ116" s="13"/>
+      <c r="AE116" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="AF116" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="AG116" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH116" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI116" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ116" s="13" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="117" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
@@ -8522,10 +8530,10 @@
         <v>14</v>
       </c>
       <c r="C117" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D117" s="35" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E117" s="49"/>
       <c r="F117" s="49"/>
@@ -8542,10 +8550,10 @@
       <c r="Q117" s="50"/>
       <c r="R117" s="35"/>
       <c r="S117" s="45">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="T117" s="45">
-        <v>2.5</v>
+        <v>2.9529999999999998</v>
       </c>
       <c r="U117" s="45">
         <v>0</v>
@@ -8561,24 +8569,12 @@
       <c r="AB117" s="11"/>
       <c r="AC117" s="7"/>
       <c r="AD117" s="13"/>
-      <c r="AE117" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="AF117" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="AG117" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH117" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI117" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ117" s="13" t="s">
-        <v>232</v>
-      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="11"/>
+      <c r="AH117" s="11"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="13"/>
     </row>
     <row r="118" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
@@ -8588,10 +8584,10 @@
         <v>14</v>
       </c>
       <c r="C118" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D118" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E118" s="49"/>
       <c r="F118" s="49"/>
@@ -8608,10 +8604,10 @@
       <c r="Q118" s="50"/>
       <c r="R118" s="35"/>
       <c r="S118" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T118" s="45">
-        <v>2.4529999999999998</v>
+        <v>2.5070000000000001</v>
       </c>
       <c r="U118" s="45">
         <v>0</v>
@@ -8627,78 +8623,78 @@
       <c r="AB118" s="11"/>
       <c r="AC118" s="7"/>
       <c r="AD118" s="13"/>
-      <c r="AE118" s="7"/>
-      <c r="AF118" s="7"/>
-      <c r="AG118" s="11"/>
-      <c r="AH118" s="11"/>
-      <c r="AI118" s="7"/>
-      <c r="AJ118" s="13"/>
+      <c r="AE118" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="AF118" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="AG118" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH118" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI118" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ118" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="119" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B119" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E119" s="58"/>
-      <c r="F119" s="58"/>
-      <c r="G119" s="1"/>
-      <c r="H119" s="1"/>
-      <c r="I119" s="1"/>
-      <c r="J119" s="1"/>
-      <c r="K119" s="1"/>
-      <c r="L119" s="1"/>
-      <c r="M119" s="1"/>
-      <c r="N119" s="1"/>
-      <c r="O119" s="1"/>
-      <c r="P119" s="2"/>
-      <c r="Q119" s="2"/>
-      <c r="R119" s="1"/>
-      <c r="S119" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="T119" s="3">
-        <v>4</v>
-      </c>
-      <c r="U119" s="3">
-        <v>0</v>
-      </c>
-      <c r="V119" s="3">
-        <v>0</v>
-      </c>
-      <c r="W119" s="2"/>
-      <c r="X119" s="3"/>
-      <c r="Y119" s="1"/>
-      <c r="Z119" s="59"/>
+      <c r="B119" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D119" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E119" s="49"/>
+      <c r="F119" s="49"/>
+      <c r="G119" s="35"/>
+      <c r="H119" s="35"/>
+      <c r="I119" s="35"/>
+      <c r="J119" s="35"/>
+      <c r="K119" s="35"/>
+      <c r="L119" s="35"/>
+      <c r="M119" s="35"/>
+      <c r="N119" s="35"/>
+      <c r="O119" s="35"/>
+      <c r="P119" s="50"/>
+      <c r="Q119" s="50"/>
+      <c r="R119" s="35"/>
+      <c r="S119" s="45">
+        <v>2.25</v>
+      </c>
+      <c r="T119" s="45">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="U119" s="45">
+        <v>0</v>
+      </c>
+      <c r="V119" s="45">
+        <v>0</v>
+      </c>
+      <c r="W119" s="50"/>
+      <c r="X119" s="45"/>
+      <c r="Y119" s="35"/>
+      <c r="Z119" s="34"/>
       <c r="AA119" s="11"/>
       <c r="AB119" s="11"/>
       <c r="AC119" s="7"/>
       <c r="AD119" s="13"/>
-      <c r="AE119" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF119" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="AG119" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH119" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI119" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ119" s="13" t="s">
-        <v>257</v>
-      </c>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="11"/>
+      <c r="AH119" s="11"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="13"/>
     </row>
     <row r="120" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
@@ -8708,10 +8704,10 @@
         <v>14</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E120" s="58"/>
       <c r="F120" s="58"/>
@@ -8728,10 +8724,10 @@
       <c r="Q120" s="2"/>
       <c r="R120" s="1"/>
       <c r="S120" s="3">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="T120" s="3">
-        <v>3.9529999999999998</v>
+        <v>4.0069999999999997</v>
       </c>
       <c r="U120" s="3">
         <v>0</v>
@@ -8747,12 +8743,24 @@
       <c r="AB120" s="11"/>
       <c r="AC120" s="7"/>
       <c r="AD120" s="13"/>
-      <c r="AE120" s="7"/>
-      <c r="AF120" s="7"/>
-      <c r="AG120" s="11"/>
-      <c r="AH120" s="11"/>
-      <c r="AI120" s="7"/>
-      <c r="AJ120" s="13"/>
+      <c r="AE120" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF120" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG120" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH120" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI120" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ120" s="13" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="121" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
@@ -8762,10 +8770,10 @@
         <v>14</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E121" s="58"/>
       <c r="F121" s="58"/>
@@ -8782,10 +8790,10 @@
       <c r="Q121" s="2"/>
       <c r="R121" s="1"/>
       <c r="S121" s="3">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="T121" s="3">
-        <v>3.5</v>
+        <v>3.9529999999999998</v>
       </c>
       <c r="U121" s="3">
         <v>0</v>
@@ -8801,24 +8809,12 @@
       <c r="AB121" s="11"/>
       <c r="AC121" s="7"/>
       <c r="AD121" s="13"/>
-      <c r="AE121" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="AF121" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="AG121" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH121" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI121" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ121" s="13" t="s">
-        <v>258</v>
-      </c>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="11"/>
+      <c r="AH121" s="11"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="13"/>
     </row>
     <row r="122" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
@@ -8828,10 +8824,10 @@
         <v>14</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E122" s="58"/>
       <c r="F122" s="58"/>
@@ -8848,10 +8844,10 @@
       <c r="Q122" s="2"/>
       <c r="R122" s="1"/>
       <c r="S122" s="3">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="T122" s="3">
-        <v>3.4529999999999998</v>
+        <v>3.5070000000000001</v>
       </c>
       <c r="U122" s="3">
         <v>0</v>
@@ -8867,12 +8863,24 @@
       <c r="AB122" s="11"/>
       <c r="AC122" s="7"/>
       <c r="AD122" s="13"/>
-      <c r="AE122" s="7"/>
-      <c r="AF122" s="7"/>
-      <c r="AG122" s="11"/>
-      <c r="AH122" s="11"/>
-      <c r="AI122" s="7"/>
-      <c r="AJ122" s="13"/>
+      <c r="AE122" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="AF122" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AG122" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH122" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI122" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ122" s="13" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="123" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
@@ -8882,10 +8890,10 @@
         <v>14</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E123" s="58"/>
       <c r="F123" s="58"/>
@@ -8902,10 +8910,10 @@
       <c r="Q123" s="2"/>
       <c r="R123" s="1"/>
       <c r="S123" s="3">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="T123" s="3">
-        <v>3</v>
+        <v>3.4529999999999998</v>
       </c>
       <c r="U123" s="3">
         <v>0</v>
@@ -8921,24 +8929,12 @@
       <c r="AB123" s="11"/>
       <c r="AC123" s="7"/>
       <c r="AD123" s="13"/>
-      <c r="AE123" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="AF123" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="AG123" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH123" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI123" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ123" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="11"/>
+      <c r="AH123" s="11"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="13"/>
     </row>
     <row r="124" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
@@ -8948,10 +8944,10 @@
         <v>14</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E124" s="58"/>
       <c r="F124" s="58"/>
@@ -8968,10 +8964,10 @@
       <c r="Q124" s="2"/>
       <c r="R124" s="1"/>
       <c r="S124" s="3">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="T124" s="3">
-        <v>2.9529999999999998</v>
+        <v>3</v>
       </c>
       <c r="U124" s="3">
         <v>0</v>
@@ -8987,14 +8983,79 @@
       <c r="AB124" s="11"/>
       <c r="AC124" s="7"/>
       <c r="AD124" s="13"/>
-      <c r="AE124" s="7"/>
-      <c r="AF124" s="7"/>
-      <c r="AG124" s="11"/>
-      <c r="AH124" s="11"/>
-      <c r="AI124" s="7"/>
-      <c r="AJ124" s="13"/>
-    </row>
-    <row r="125" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AE124" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF124" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG124" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH124" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI124" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ124" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="125" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E125" s="58"/>
+      <c r="F125" s="58"/>
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+      <c r="J125" s="1"/>
+      <c r="K125" s="1"/>
+      <c r="L125" s="1"/>
+      <c r="M125" s="1"/>
+      <c r="N125" s="1"/>
+      <c r="O125" s="1"/>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="1"/>
+      <c r="S125" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="T125" s="3">
+        <v>2.9529999999999998</v>
+      </c>
+      <c r="U125" s="3">
+        <v>0</v>
+      </c>
+      <c r="V125" s="3">
+        <v>0</v>
+      </c>
+      <c r="W125" s="2"/>
+      <c r="X125" s="3"/>
+      <c r="Y125" s="1"/>
+      <c r="Z125" s="59"/>
+      <c r="AA125" s="11"/>
+      <c r="AB125" s="11"/>
+      <c r="AC125" s="7"/>
+      <c r="AD125" s="13"/>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="11"/>
+      <c r="AH125" s="11"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="13"/>
+    </row>
     <row r="126" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="127" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9002,10 +9063,11 @@
     <row r="130" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="131" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="132" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:AJ124" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}"/>
+  <autoFilter ref="A1:AJ125" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}"/>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X110 X68:X81 X2:X52 X55:X65 E1:E1048576" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X111 X69:X82 X2:X52 X55:X66 E1:E1048576" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9017,55 +9079,55 @@
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Y68 Y2:Y5 Y110 Y7</xm:sqref>
+          <xm:sqref>Y69 Y2:Y5 Y111 Y7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2:AA124 AG2:AG124</xm:sqref>
+          <xm:sqref>AA2:AA125 AG2:AG125</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AB2:AB124 AH2:AH124</xm:sqref>
+          <xm:sqref>AB2:AB125 AH2:AH125</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D20E3002-F58D-4FAD-9CC5-854E38BB1BD9}">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F124</xm:sqref>
+          <xm:sqref>F2:F125</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{0B95AA9E-6EAC-4E79-9737-4C4B42A3B143}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>AI2:AI124 W2:W124 AC2:AC124</xm:sqref>
+          <xm:sqref>AI2:AI125 W2:W125 AC2:AC125</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6AE078-B717-4B67-83B7-999D58BC2953}">
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G124</xm:sqref>
+          <xm:sqref>G2:G125</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{434DCAEE-02F3-44B7-8757-503F2F2EE546}">
           <x14:formula1>
             <xm:f>Tables!$M$2:$M$8</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD124 AJ2:AJ124</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
-          <x14:formula1>
-            <xm:f>Tables!$O$2:$O$54</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D124</xm:sqref>
+          <xm:sqref>AD2:AD125 AJ2:AJ125</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
           <x14:formula1>
             <xm:f>Tables!$K$2:$K$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B124</xm:sqref>
+          <xm:sqref>B2:B125</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
+          <x14:formula1>
+            <xm:f>Tables!$O$2:$O$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D125</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9400,7 +9462,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9776,16 +9838,16 @@
       <c r="A29" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="O29" s="42" t="s">
-        <v>112</v>
+      <c r="O29" s="47" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="O30" s="41" t="s">
-        <v>88</v>
+      <c r="O30" s="42" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9793,23 +9855,23 @@
         <v>155</v>
       </c>
       <c r="O31" s="41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="O32" s="42" t="s">
-        <v>117</v>
+      <c r="O32" s="41" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="O33" s="41" t="s">
-        <v>118</v>
+      <c r="O33" s="42" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9817,7 +9879,7 @@
         <v>157</v>
       </c>
       <c r="O34" s="41" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9825,7 +9887,7 @@
         <v>158</v>
       </c>
       <c r="O35" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9833,7 +9895,7 @@
         <v>25</v>
       </c>
       <c r="O36" s="41" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9841,7 +9903,7 @@
         <v>159</v>
       </c>
       <c r="O37" s="41" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9849,7 +9911,7 @@
         <v>160</v>
       </c>
       <c r="O38" s="41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9857,7 +9919,7 @@
         <v>161</v>
       </c>
       <c r="O39" s="41" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9865,7 +9927,7 @@
         <v>162</v>
       </c>
       <c r="O40" s="41" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9873,7 +9935,7 @@
         <v>163</v>
       </c>
       <c r="O41" s="41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9881,7 +9943,7 @@
         <v>164</v>
       </c>
       <c r="O42" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9889,65 +9951,69 @@
         <v>26</v>
       </c>
       <c r="O43" s="41" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O44" s="41" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O45" s="41" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O46" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O47" s="41" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O47" s="47" t="s">
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O48" s="47" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O48" s="41" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="49" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O49" s="41" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O50" s="41" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O51" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O52" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O53" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O54" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O55" s="41" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added the new shape OC_AngledTexzt
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
+++ b/Data/ScriptData/OC_ArchitectBlueprintingData_ColorTesting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF20822C-B2A2-4118-9750-CE29B6E4FB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D244D11-C85E-4BA6-9B86-424014C80134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1290" windowWidth="25665" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="1605" yWindow="1590" windowWidth="25665" windowHeight="14760" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Tables" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VisioData!$A$1:$AJ$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VisioData!$A$1:$AJ$126</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="326">
   <si>
     <t>mach_name</t>
   </si>
@@ -1244,6 +1244,12 @@
   </si>
   <si>
     <t>OC_LabelGreen:1</t>
+  </si>
+  <si>
+    <t>OC_AngledText</t>
+  </si>
+  <si>
+    <t>OC_AngledText:1</t>
   </si>
 </sst>
 </file>
@@ -1945,11 +1951,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ133"/>
+  <dimension ref="A1:AJ134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T124" sqref="T124"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U65" sqref="U65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5465,104 +5471,104 @@
       <c r="AJ64" s="54"/>
     </row>
     <row r="65" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="50">
+        <v>1</v>
+      </c>
+      <c r="B65" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="35" t="s">
+        <v>325</v>
+      </c>
+      <c r="D65" s="35" t="s">
+        <v>324</v>
+      </c>
+      <c r="E65" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="F65" s="49"/>
+      <c r="G65" s="35"/>
+      <c r="H65" s="35"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="35"/>
+      <c r="K65" s="35"/>
+      <c r="L65" s="35"/>
+      <c r="M65" s="35"/>
+      <c r="N65" s="35"/>
+      <c r="O65" s="35"/>
+      <c r="P65" s="50"/>
+      <c r="Q65" s="50"/>
+      <c r="R65" s="35"/>
+      <c r="S65" s="45">
+        <v>6.2149999999999999</v>
+      </c>
+      <c r="T65" s="45">
+        <v>3.3220000000000001</v>
+      </c>
+      <c r="U65" s="45">
+        <v>0</v>
+      </c>
+      <c r="V65" s="45">
+        <v>0</v>
+      </c>
+      <c r="W65" s="45"/>
+      <c r="X65" s="45"/>
+      <c r="Y65" s="35"/>
+      <c r="Z65" s="34"/>
+      <c r="AA65" s="34"/>
+      <c r="AB65" s="34"/>
+      <c r="AC65" s="34"/>
+      <c r="AD65" s="54"/>
+      <c r="AE65" s="34"/>
+      <c r="AF65" s="34"/>
+      <c r="AG65" s="34"/>
+      <c r="AH65" s="34"/>
+      <c r="AI65" s="34"/>
+      <c r="AJ65" s="54"/>
+    </row>
+    <row r="66" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B66" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="61"/>
-      <c r="F65" s="61"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="14"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
-      <c r="O65" s="14"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="14"/>
-      <c r="S65" s="17"/>
-      <c r="T65" s="17"/>
-      <c r="U65" s="17"/>
-      <c r="V65" s="17"/>
-      <c r="W65" s="17"/>
-      <c r="X65" s="17"/>
-      <c r="Y65" s="14"/>
-      <c r="Z65" s="16"/>
-      <c r="AA65" s="16"/>
-      <c r="AB65" s="16"/>
-      <c r="AC65" s="16"/>
-      <c r="AD65" s="62"/>
-      <c r="AE65" s="16"/>
-      <c r="AF65" s="16"/>
-      <c r="AG65" s="16"/>
-      <c r="AH65" s="16"/>
-      <c r="AI65" s="16"/>
-      <c r="AJ65" s="62"/>
-    </row>
-    <row r="66" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="50">
-        <v>1</v>
-      </c>
-      <c r="B66" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" s="35" t="s">
-        <v>297</v>
-      </c>
-      <c r="D66" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E66" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="F66" s="49"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
-      <c r="M66" s="35"/>
-      <c r="N66" s="35"/>
-      <c r="O66" s="35"/>
-      <c r="P66" s="50"/>
-      <c r="Q66" s="50"/>
-      <c r="R66" s="35"/>
-      <c r="S66" s="45">
-        <v>0.25</v>
-      </c>
-      <c r="T66" s="45">
-        <v>2.6829999999999998</v>
-      </c>
-      <c r="U66" s="45">
-        <v>0</v>
-      </c>
-      <c r="V66" s="45">
-        <v>0</v>
-      </c>
-      <c r="W66" s="45"/>
-      <c r="X66" s="45"/>
-      <c r="Y66" s="35"/>
-      <c r="Z66" s="34"/>
-      <c r="AA66" s="34"/>
-      <c r="AB66" s="34"/>
-      <c r="AC66" s="34"/>
-      <c r="AD66" s="54"/>
-      <c r="AE66" s="34"/>
-      <c r="AF66" s="34"/>
-      <c r="AG66" s="34"/>
-      <c r="AH66" s="34"/>
-      <c r="AI66" s="34"/>
-      <c r="AJ66" s="54"/>
-    </row>
-    <row r="67" spans="1:36" s="60" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="61"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
+      <c r="N66" s="14"/>
+      <c r="O66" s="14"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="14"/>
+      <c r="S66" s="17"/>
+      <c r="T66" s="17"/>
+      <c r="U66" s="17"/>
+      <c r="V66" s="17"/>
+      <c r="W66" s="17"/>
+      <c r="X66" s="17"/>
+      <c r="Y66" s="14"/>
+      <c r="Z66" s="16"/>
+      <c r="AA66" s="16"/>
+      <c r="AB66" s="16"/>
+      <c r="AC66" s="16"/>
+      <c r="AD66" s="62"/>
+      <c r="AE66" s="16"/>
+      <c r="AF66" s="16"/>
+      <c r="AG66" s="16"/>
+      <c r="AH66" s="16"/>
+      <c r="AI66" s="16"/>
+      <c r="AJ66" s="62"/>
+    </row>
+    <row r="67" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="50">
         <v>1</v>
       </c>
@@ -5570,13 +5576,13 @@
         <v>14</v>
       </c>
       <c r="C67" s="35" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E67" s="49" t="s">
-        <v>317</v>
+        <v>88</v>
       </c>
       <c r="F67" s="49"/>
       <c r="G67" s="35"/>
@@ -5592,10 +5598,10 @@
       <c r="Q67" s="50"/>
       <c r="R67" s="35"/>
       <c r="S67" s="45">
-        <v>2.3780000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="T67" s="45">
-        <v>2.887</v>
+        <v>2.6829999999999998</v>
       </c>
       <c r="U67" s="45">
         <v>0</v>
@@ -5618,7 +5624,7 @@
       <c r="AI67" s="34"/>
       <c r="AJ67" s="54"/>
     </row>
-    <row r="68" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" s="60" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="50">
         <v>1</v>
       </c>
@@ -5626,13 +5632,13 @@
         <v>14</v>
       </c>
       <c r="C68" s="35" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D68" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E68" s="49" t="s">
-        <v>90</v>
+        <v>317</v>
       </c>
       <c r="F68" s="49"/>
       <c r="G68" s="35"/>
@@ -5648,10 +5654,10 @@
       <c r="Q68" s="50"/>
       <c r="R68" s="35"/>
       <c r="S68" s="45">
-        <v>0.25</v>
+        <v>2.3780000000000001</v>
       </c>
       <c r="T68" s="45">
-        <v>0.625</v>
+        <v>2.887</v>
       </c>
       <c r="U68" s="45">
         <v>0</v>
@@ -5674,107 +5680,103 @@
       <c r="AI68" s="34"/>
       <c r="AJ68" s="54"/>
     </row>
-    <row r="69" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
+    <row r="69" spans="1:36" s="60" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="50">
+        <v>1</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D69" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E69" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="F69" s="49"/>
+      <c r="G69" s="35"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="35"/>
+      <c r="K69" s="35"/>
+      <c r="L69" s="35"/>
+      <c r="M69" s="35"/>
+      <c r="N69" s="35"/>
+      <c r="O69" s="35"/>
+      <c r="P69" s="50"/>
+      <c r="Q69" s="50"/>
+      <c r="R69" s="35"/>
+      <c r="S69" s="45">
+        <v>0.25</v>
+      </c>
+      <c r="T69" s="45">
+        <v>1.625</v>
+      </c>
+      <c r="U69" s="45">
+        <v>0</v>
+      </c>
+      <c r="V69" s="45">
+        <v>0</v>
+      </c>
+      <c r="W69" s="45"/>
+      <c r="X69" s="45"/>
+      <c r="Y69" s="35"/>
+      <c r="Z69" s="34"/>
+      <c r="AA69" s="34"/>
+      <c r="AB69" s="34"/>
+      <c r="AC69" s="34"/>
+      <c r="AD69" s="54"/>
+      <c r="AE69" s="34"/>
+      <c r="AF69" s="34"/>
+      <c r="AG69" s="34"/>
+      <c r="AH69" s="34"/>
+      <c r="AI69" s="34"/>
+      <c r="AJ69" s="54"/>
+    </row>
+    <row r="70" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B70" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
-      <c r="O69" s="14"/>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="16"/>
-      <c r="S69" s="17"/>
-      <c r="T69" s="17"/>
-      <c r="U69" s="17"/>
-      <c r="V69" s="17"/>
-      <c r="W69" s="17"/>
-      <c r="X69" s="17"/>
-      <c r="Y69" s="14"/>
-      <c r="Z69" s="16"/>
-      <c r="AA69" s="16"/>
-      <c r="AB69" s="16"/>
-      <c r="AC69" s="16"/>
-      <c r="AD69" s="16"/>
-      <c r="AE69" s="16"/>
-      <c r="AF69" s="16"/>
-      <c r="AG69" s="16"/>
-      <c r="AH69" s="16"/>
-      <c r="AI69" s="16"/>
-      <c r="AJ69" s="16"/>
-    </row>
-    <row r="70" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="E70" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="F70" s="21"/>
-      <c r="G70" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="9"/>
-      <c r="Q70" s="9"/>
-      <c r="R70" s="7"/>
-      <c r="S70" s="10">
-        <v>1</v>
-      </c>
-      <c r="T70" s="10">
-        <v>10.5</v>
-      </c>
-      <c r="U70" s="10">
-        <v>0</v>
-      </c>
-      <c r="V70" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="W70" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="X70" s="10"/>
-      <c r="Y70" s="8"/>
-      <c r="Z70" s="7"/>
-      <c r="AA70" s="11"/>
-      <c r="AB70" s="11"/>
-      <c r="AC70" s="7"/>
-      <c r="AD70" s="7"/>
-      <c r="AE70" s="7"/>
-      <c r="AF70" s="7"/>
-      <c r="AG70" s="11"/>
-      <c r="AH70" s="11"/>
-      <c r="AI70" s="7"/>
-      <c r="AJ70" s="7"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="14"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="16"/>
+      <c r="S70" s="17"/>
+      <c r="T70" s="17"/>
+      <c r="U70" s="17"/>
+      <c r="V70" s="17"/>
+      <c r="W70" s="17"/>
+      <c r="X70" s="17"/>
+      <c r="Y70" s="14"/>
+      <c r="Z70" s="16"/>
+      <c r="AA70" s="16"/>
+      <c r="AB70" s="16"/>
+      <c r="AC70" s="16"/>
+      <c r="AD70" s="16"/>
+      <c r="AE70" s="16"/>
+      <c r="AF70" s="16"/>
+      <c r="AG70" s="16"/>
+      <c r="AH70" s="16"/>
+      <c r="AI70" s="16"/>
+      <c r="AJ70" s="16"/>
     </row>
     <row r="71" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
@@ -5784,13 +5786,13 @@
         <v>14</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="F71" s="21"/>
       <c r="G71" s="8" t="s">
@@ -5811,7 +5813,7 @@
         <v>1</v>
       </c>
       <c r="T71" s="10">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U71" s="10">
         <v>0</v>
@@ -5820,7 +5822,7 @@
         <v>0.5</v>
       </c>
       <c r="W71" s="10" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="X71" s="10"/>
       <c r="Y71" s="8"/>
@@ -5844,13 +5846,13 @@
         <v>14</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="F72" s="21"/>
       <c r="G72" s="8" t="s">
@@ -5866,12 +5868,12 @@
       <c r="O72" s="8"/>
       <c r="P72" s="9"/>
       <c r="Q72" s="9"/>
-      <c r="R72" s="8"/>
+      <c r="R72" s="7"/>
       <c r="S72" s="10">
         <v>1</v>
       </c>
       <c r="T72" s="10">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U72" s="10">
         <v>0</v>
@@ -5879,10 +5881,10 @@
       <c r="V72" s="10">
         <v>0.5</v>
       </c>
-      <c r="W72" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="X72" s="8"/>
+      <c r="W72" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="X72" s="10"/>
       <c r="Y72" s="8"/>
       <c r="Z72" s="7"/>
       <c r="AA72" s="11"/>
@@ -5896,42 +5898,42 @@
       <c r="AI72" s="7"/>
       <c r="AJ72" s="7"/>
     </row>
-    <row r="73" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>321</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C73" s="43" t="s">
-        <v>179</v>
+      <c r="C73" s="8" t="s">
+        <v>177</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E73" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="F73" s="51"/>
+      <c r="E73" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F73" s="21"/>
       <c r="G73" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="43"/>
-      <c r="L73" s="43"/>
-      <c r="M73" s="43"/>
-      <c r="N73" s="43"/>
-      <c r="O73" s="43"/>
-      <c r="P73" s="52"/>
-      <c r="Q73" s="52"/>
-      <c r="R73" s="11"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="8"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="8"/>
       <c r="S73" s="10">
         <v>1</v>
       </c>
       <c r="T73" s="10">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U73" s="10">
         <v>0</v>
@@ -5939,21 +5941,21 @@
       <c r="V73" s="10">
         <v>0.5</v>
       </c>
-      <c r="W73" s="44" t="s">
-        <v>210</v>
-      </c>
-      <c r="X73" s="44"/>
-      <c r="Y73" s="43"/>
-      <c r="Z73" s="11"/>
+      <c r="W73" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="X73" s="8"/>
+      <c r="Y73" s="8"/>
+      <c r="Z73" s="7"/>
       <c r="AA73" s="11"/>
       <c r="AB73" s="11"/>
-      <c r="AC73" s="11"/>
+      <c r="AC73" s="7"/>
       <c r="AD73" s="7"/>
-      <c r="AE73" s="11"/>
-      <c r="AF73" s="11"/>
+      <c r="AE73" s="7"/>
+      <c r="AF73" s="7"/>
       <c r="AG73" s="11"/>
       <c r="AH73" s="11"/>
-      <c r="AI73" s="11"/>
+      <c r="AI73" s="7"/>
       <c r="AJ73" s="7"/>
     </row>
     <row r="74" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5964,15 +5966,15 @@
         <v>14</v>
       </c>
       <c r="C74" s="43" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E74" s="51" t="s">
-        <v>211</v>
-      </c>
-      <c r="F74" s="43"/>
+        <v>210</v>
+      </c>
+      <c r="F74" s="51"/>
       <c r="G74" s="8" t="s">
         <v>36</v>
       </c>
@@ -5991,7 +5993,7 @@
         <v>1</v>
       </c>
       <c r="T74" s="10">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U74" s="10">
         <v>0</v>
@@ -6000,7 +6002,7 @@
         <v>0.5</v>
       </c>
       <c r="W74" s="44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X74" s="44"/>
       <c r="Y74" s="43"/>
@@ -6009,7 +6011,7 @@
       <c r="AB74" s="11"/>
       <c r="AC74" s="11"/>
       <c r="AD74" s="7"/>
-      <c r="AE74" s="43"/>
+      <c r="AE74" s="11"/>
       <c r="AF74" s="11"/>
       <c r="AG74" s="11"/>
       <c r="AH74" s="11"/>
@@ -6024,13 +6026,13 @@
         <v>14</v>
       </c>
       <c r="C75" s="43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E75" s="51" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="F75" s="43"/>
       <c r="G75" s="8" t="s">
@@ -6051,7 +6053,7 @@
         <v>1</v>
       </c>
       <c r="T75" s="10">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U75" s="10">
         <v>0</v>
@@ -6060,7 +6062,7 @@
         <v>0.5</v>
       </c>
       <c r="W75" s="44" t="s">
-        <v>19</v>
+        <v>211</v>
       </c>
       <c r="X75" s="44"/>
       <c r="Y75" s="43"/>
@@ -6084,13 +6086,13 @@
         <v>14</v>
       </c>
       <c r="C76" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E76" s="51" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F76" s="43"/>
       <c r="G76" s="8" t="s">
@@ -6111,7 +6113,7 @@
         <v>1</v>
       </c>
       <c r="T76" s="10">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U76" s="10">
         <v>0</v>
@@ -6120,7 +6122,7 @@
         <v>0.5</v>
       </c>
       <c r="W76" s="44" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="X76" s="44"/>
       <c r="Y76" s="43"/>
@@ -6129,7 +6131,7 @@
       <c r="AB76" s="11"/>
       <c r="AC76" s="11"/>
       <c r="AD76" s="7"/>
-      <c r="AE76" s="11"/>
+      <c r="AE76" s="43"/>
       <c r="AF76" s="11"/>
       <c r="AG76" s="11"/>
       <c r="AH76" s="11"/>
@@ -6144,13 +6146,13 @@
         <v>14</v>
       </c>
       <c r="C77" s="43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E77" s="51" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="F77" s="43"/>
       <c r="G77" s="8" t="s">
@@ -6171,7 +6173,7 @@
         <v>1</v>
       </c>
       <c r="T77" s="10">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U77" s="10">
         <v>0</v>
@@ -6180,7 +6182,7 @@
         <v>0.5</v>
       </c>
       <c r="W77" s="44" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="X77" s="44"/>
       <c r="Y77" s="43"/>
@@ -6204,13 +6206,13 @@
         <v>14</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E78" s="51" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="F78" s="43"/>
       <c r="G78" s="8" t="s">
@@ -6231,7 +6233,7 @@
         <v>1</v>
       </c>
       <c r="T78" s="10">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="U78" s="10">
         <v>0</v>
@@ -6240,7 +6242,7 @@
         <v>0.5</v>
       </c>
       <c r="W78" s="44" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="X78" s="44"/>
       <c r="Y78" s="43"/>
@@ -6248,13 +6250,13 @@
       <c r="AA78" s="11"/>
       <c r="AB78" s="11"/>
       <c r="AC78" s="11"/>
-      <c r="AD78" s="34"/>
+      <c r="AD78" s="7"/>
       <c r="AE78" s="11"/>
       <c r="AF78" s="11"/>
       <c r="AG78" s="11"/>
       <c r="AH78" s="11"/>
       <c r="AI78" s="11"/>
-      <c r="AJ78" s="34"/>
+      <c r="AJ78" s="7"/>
     </row>
     <row r="79" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
@@ -6264,13 +6266,13 @@
         <v>14</v>
       </c>
       <c r="C79" s="43" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E79" s="51" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="F79" s="43"/>
       <c r="G79" s="8" t="s">
@@ -6291,7 +6293,7 @@
         <v>1</v>
       </c>
       <c r="T79" s="10">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="U79" s="10">
         <v>0</v>
@@ -6300,7 +6302,7 @@
         <v>0.5</v>
       </c>
       <c r="W79" s="44" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="X79" s="44"/>
       <c r="Y79" s="43"/>
@@ -6308,13 +6310,13 @@
       <c r="AA79" s="11"/>
       <c r="AB79" s="11"/>
       <c r="AC79" s="11"/>
-      <c r="AD79" s="7"/>
+      <c r="AD79" s="34"/>
       <c r="AE79" s="11"/>
       <c r="AF79" s="11"/>
       <c r="AG79" s="11"/>
       <c r="AH79" s="11"/>
       <c r="AI79" s="11"/>
-      <c r="AJ79" s="7"/>
+      <c r="AJ79" s="34"/>
     </row>
     <row r="80" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
@@ -6324,13 +6326,13 @@
         <v>14</v>
       </c>
       <c r="C80" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>183</v>
       </c>
       <c r="E80" s="51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F80" s="43"/>
       <c r="G80" s="8" t="s">
@@ -6351,7 +6353,7 @@
         <v>1</v>
       </c>
       <c r="T80" s="10">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="U80" s="10">
         <v>0</v>
@@ -6360,7 +6362,7 @@
         <v>0.5</v>
       </c>
       <c r="W80" s="44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X80" s="44"/>
       <c r="Y80" s="43"/>
@@ -6376,42 +6378,42 @@
       <c r="AI80" s="11"/>
       <c r="AJ80" s="7"/>
     </row>
-    <row r="81" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>321</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="8" t="s">
-        <v>185</v>
+      <c r="C81" s="43" t="s">
+        <v>224</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E81" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F81" s="21"/>
+      <c r="E81" s="51" t="s">
+        <v>213</v>
+      </c>
+      <c r="F81" s="43"/>
       <c r="G81" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
-      <c r="L81" s="8"/>
-      <c r="M81" s="8"/>
-      <c r="N81" s="8"/>
-      <c r="O81" s="8"/>
-      <c r="P81" s="9"/>
-      <c r="Q81" s="9"/>
-      <c r="R81" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="H81" s="43"/>
+      <c r="I81" s="43"/>
+      <c r="J81" s="43"/>
+      <c r="K81" s="43"/>
+      <c r="L81" s="43"/>
+      <c r="M81" s="43"/>
+      <c r="N81" s="43"/>
+      <c r="O81" s="43"/>
+      <c r="P81" s="52"/>
+      <c r="Q81" s="52"/>
+      <c r="R81" s="11"/>
       <c r="S81" s="10">
         <v>1</v>
       </c>
       <c r="T81" s="10">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="U81" s="10">
         <v>0</v>
@@ -6419,82 +6421,82 @@
       <c r="V81" s="10">
         <v>0.5</v>
       </c>
-      <c r="W81" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="X81" s="10"/>
-      <c r="Y81" s="8"/>
-      <c r="Z81" s="7"/>
+      <c r="W81" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="X81" s="44"/>
+      <c r="Y81" s="43"/>
+      <c r="Z81" s="11"/>
       <c r="AA81" s="11"/>
       <c r="AB81" s="11"/>
-      <c r="AC81" s="7"/>
+      <c r="AC81" s="11"/>
       <c r="AD81" s="7"/>
-      <c r="AE81" s="7"/>
-      <c r="AF81" s="7"/>
+      <c r="AE81" s="11"/>
+      <c r="AF81" s="11"/>
       <c r="AG81" s="11"/>
       <c r="AH81" s="11"/>
-      <c r="AI81" s="7"/>
+      <c r="AI81" s="11"/>
       <c r="AJ81" s="7"/>
     </row>
     <row r="82" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D82" s="5" t="s">
+      <c r="B82" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D82" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E82" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="F82" s="55"/>
-      <c r="G82" s="5" t="s">
+      <c r="E82" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F82" s="21"/>
+      <c r="G82" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5"/>
-      <c r="O82" s="5"/>
-      <c r="P82" s="19"/>
-      <c r="Q82" s="19"/>
-      <c r="R82" s="56"/>
-      <c r="S82" s="57">
-        <v>2.25</v>
-      </c>
-      <c r="T82" s="57">
-        <v>10.5</v>
-      </c>
-      <c r="U82" s="57">
-        <v>0</v>
-      </c>
-      <c r="V82" s="57">
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="8"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9"/>
+      <c r="R82" s="7"/>
+      <c r="S82" s="10">
+        <v>1</v>
+      </c>
+      <c r="T82" s="10">
+        <v>5</v>
+      </c>
+      <c r="U82" s="10">
+        <v>0</v>
+      </c>
+      <c r="V82" s="10">
         <v>0.5</v>
       </c>
-      <c r="W82" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="X82" s="57"/>
-      <c r="Y82" s="5"/>
-      <c r="Z82" s="56"/>
+      <c r="W82" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="X82" s="10"/>
+      <c r="Y82" s="8"/>
+      <c r="Z82" s="7"/>
       <c r="AA82" s="11"/>
       <c r="AB82" s="11"/>
       <c r="AC82" s="7"/>
-      <c r="AD82" s="13"/>
+      <c r="AD82" s="7"/>
       <c r="AE82" s="7"/>
       <c r="AF82" s="7"/>
       <c r="AG82" s="11"/>
       <c r="AH82" s="11"/>
       <c r="AI82" s="7"/>
-      <c r="AJ82" s="13"/>
+      <c r="AJ82" s="7"/>
     </row>
     <row r="83" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
@@ -6504,13 +6506,13 @@
         <v>14</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E83" s="55" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F83" s="55"/>
       <c r="G83" s="5" t="s">
@@ -6526,12 +6528,12 @@
       <c r="O83" s="5"/>
       <c r="P83" s="19"/>
       <c r="Q83" s="19"/>
-      <c r="R83" s="5"/>
+      <c r="R83" s="56"/>
       <c r="S83" s="57">
         <v>2.25</v>
       </c>
       <c r="T83" s="57">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U83" s="57">
         <v>0</v>
@@ -6539,8 +6541,8 @@
       <c r="V83" s="57">
         <v>0.5</v>
       </c>
-      <c r="W83" s="19" t="s">
-        <v>144</v>
+      <c r="W83" s="57" t="s">
+        <v>151</v>
       </c>
       <c r="X83" s="57"/>
       <c r="Y83" s="5"/>
@@ -6564,13 +6566,13 @@
         <v>14</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E84" s="55" t="s">
-        <v>225</v>
+        <v>144</v>
       </c>
       <c r="F84" s="55"/>
       <c r="G84" s="5" t="s">
@@ -6591,7 +6593,7 @@
         <v>2.25</v>
       </c>
       <c r="T84" s="57">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U84" s="57">
         <v>0</v>
@@ -6600,7 +6602,7 @@
         <v>0.5</v>
       </c>
       <c r="W84" s="19" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
       <c r="X84" s="57"/>
       <c r="Y84" s="5"/>
@@ -6624,13 +6626,13 @@
         <v>14</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E85" s="55" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="F85" s="55"/>
       <c r="G85" s="5" t="s">
@@ -6651,7 +6653,7 @@
         <v>2.25</v>
       </c>
       <c r="T85" s="57">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U85" s="57">
         <v>0</v>
@@ -6660,7 +6662,7 @@
         <v>0.5</v>
       </c>
       <c r="W85" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X85" s="57"/>
       <c r="Y85" s="5"/>
@@ -6684,13 +6686,13 @@
         <v>14</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E86" s="55" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="F86" s="55"/>
       <c r="G86" s="5" t="s">
@@ -6711,7 +6713,7 @@
         <v>2.25</v>
       </c>
       <c r="T86" s="57">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U86" s="57">
         <v>0</v>
@@ -6720,7 +6722,7 @@
         <v>0.5</v>
       </c>
       <c r="W86" s="19" t="s">
-        <v>145</v>
+        <v>215</v>
       </c>
       <c r="X86" s="57"/>
       <c r="Y86" s="5"/>
@@ -6744,13 +6746,13 @@
         <v>14</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E87" s="55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F87" s="55"/>
       <c r="G87" s="5" t="s">
@@ -6771,7 +6773,7 @@
         <v>2.25</v>
       </c>
       <c r="T87" s="57">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U87" s="57">
         <v>0</v>
@@ -6780,7 +6782,7 @@
         <v>0.5</v>
       </c>
       <c r="W87" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="X87" s="57"/>
       <c r="Y87" s="5"/>
@@ -6804,13 +6806,13 @@
         <v>14</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E88" s="55" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="F88" s="55"/>
       <c r="G88" s="5" t="s">
@@ -6831,7 +6833,7 @@
         <v>2.25</v>
       </c>
       <c r="T88" s="57">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U88" s="57">
         <v>0</v>
@@ -6840,7 +6842,7 @@
         <v>0.5</v>
       </c>
       <c r="W88" s="19" t="s">
-        <v>216</v>
+        <v>146</v>
       </c>
       <c r="X88" s="57"/>
       <c r="Y88" s="5"/>
@@ -6864,13 +6866,13 @@
         <v>14</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E89" s="55" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="F89" s="55"/>
       <c r="G89" s="5" t="s">
@@ -6891,7 +6893,7 @@
         <v>2.25</v>
       </c>
       <c r="T89" s="57">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U89" s="57">
         <v>0</v>
@@ -6900,7 +6902,7 @@
         <v>0.5</v>
       </c>
       <c r="W89" s="19" t="s">
-        <v>21</v>
+        <v>216</v>
       </c>
       <c r="X89" s="57"/>
       <c r="Y89" s="5"/>
@@ -6924,13 +6926,13 @@
         <v>14</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E90" s="55" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="F90" s="55"/>
       <c r="G90" s="5" t="s">
@@ -6951,7 +6953,7 @@
         <v>2.25</v>
       </c>
       <c r="T90" s="57">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="U90" s="57">
         <v>0</v>
@@ -6960,7 +6962,7 @@
         <v>0.5</v>
       </c>
       <c r="W90" s="19" t="s">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="X90" s="57"/>
       <c r="Y90" s="5"/>
@@ -6976,67 +6978,67 @@
       <c r="AI90" s="7"/>
       <c r="AJ90" s="13"/>
     </row>
-    <row r="91" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B91" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C91" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="D91" s="35" t="s">
+      <c r="B91" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="E91" s="49" t="s">
-        <v>156</v>
-      </c>
-      <c r="F91" s="49"/>
-      <c r="G91" s="35" t="s">
+      <c r="E91" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="F91" s="55"/>
+      <c r="G91" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H91" s="35"/>
-      <c r="I91" s="35"/>
-      <c r="J91" s="35"/>
-      <c r="K91" s="35"/>
-      <c r="L91" s="35"/>
-      <c r="M91" s="35"/>
-      <c r="N91" s="35"/>
-      <c r="O91" s="35"/>
-      <c r="P91" s="50"/>
-      <c r="Q91" s="50"/>
-      <c r="R91" s="35"/>
-      <c r="S91" s="45">
-        <v>3.5</v>
-      </c>
-      <c r="T91" s="45">
-        <v>10.5</v>
-      </c>
-      <c r="U91" s="45">
-        <v>0</v>
-      </c>
-      <c r="V91" s="10">
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+      <c r="K91" s="5"/>
+      <c r="L91" s="5"/>
+      <c r="M91" s="5"/>
+      <c r="N91" s="5"/>
+      <c r="O91" s="5"/>
+      <c r="P91" s="19"/>
+      <c r="Q91" s="19"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="57">
+        <v>2.25</v>
+      </c>
+      <c r="T91" s="57">
+        <v>6.5</v>
+      </c>
+      <c r="U91" s="57">
+        <v>0</v>
+      </c>
+      <c r="V91" s="57">
         <v>0.5</v>
       </c>
-      <c r="W91" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="X91" s="45"/>
-      <c r="Y91" s="35"/>
-      <c r="Z91" s="34"/>
+      <c r="W91" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="X91" s="57"/>
+      <c r="Y91" s="5"/>
+      <c r="Z91" s="56"/>
       <c r="AA91" s="11"/>
       <c r="AB91" s="11"/>
-      <c r="AC91" s="11"/>
+      <c r="AC91" s="7"/>
       <c r="AD91" s="13"/>
-      <c r="AE91" s="11"/>
-      <c r="AF91" s="11"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
       <c r="AG91" s="11"/>
       <c r="AH91" s="11"/>
-      <c r="AI91" s="11"/>
+      <c r="AI91" s="7"/>
       <c r="AJ91" s="13"/>
     </row>
-    <row r="92" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:36" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>321</v>
       </c>
@@ -7044,13 +7046,13 @@
         <v>14</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D92" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E92" s="49" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F92" s="49"/>
       <c r="G92" s="35" t="s">
@@ -7071,7 +7073,7 @@
         <v>3.5</v>
       </c>
       <c r="T92" s="45">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U92" s="45">
         <v>0</v>
@@ -7080,20 +7082,20 @@
         <v>0.5</v>
       </c>
       <c r="W92" s="50" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="X92" s="45"/>
       <c r="Y92" s="35"/>
       <c r="Z92" s="34"/>
       <c r="AA92" s="11"/>
       <c r="AB92" s="11"/>
-      <c r="AC92" s="7"/>
+      <c r="AC92" s="11"/>
       <c r="AD92" s="13"/>
-      <c r="AE92" s="7"/>
-      <c r="AF92" s="7"/>
+      <c r="AE92" s="11"/>
+      <c r="AF92" s="11"/>
       <c r="AG92" s="11"/>
       <c r="AH92" s="11"/>
-      <c r="AI92" s="7"/>
+      <c r="AI92" s="11"/>
       <c r="AJ92" s="13"/>
     </row>
     <row r="93" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7104,13 +7106,13 @@
         <v>14</v>
       </c>
       <c r="C93" s="35" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D93" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E93" s="49" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="F93" s="49"/>
       <c r="G93" s="35" t="s">
@@ -7131,7 +7133,7 @@
         <v>3.5</v>
       </c>
       <c r="T93" s="45">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U93" s="45">
         <v>0</v>
@@ -7140,7 +7142,7 @@
         <v>0.5</v>
       </c>
       <c r="W93" s="50" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="X93" s="45"/>
       <c r="Y93" s="35"/>
@@ -7164,13 +7166,13 @@
         <v>14</v>
       </c>
       <c r="C94" s="35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D94" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E94" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F94" s="49"/>
       <c r="G94" s="35" t="s">
@@ -7191,7 +7193,7 @@
         <v>3.5</v>
       </c>
       <c r="T94" s="45">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U94" s="45">
         <v>0</v>
@@ -7200,7 +7202,7 @@
         <v>0.5</v>
       </c>
       <c r="W94" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="X94" s="45"/>
       <c r="Y94" s="35"/>
@@ -7224,13 +7226,13 @@
         <v>14</v>
       </c>
       <c r="C95" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D95" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E95" s="49" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F95" s="49"/>
       <c r="G95" s="35" t="s">
@@ -7251,7 +7253,7 @@
         <v>3.5</v>
       </c>
       <c r="T95" s="45">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U95" s="45">
         <v>0</v>
@@ -7260,7 +7262,7 @@
         <v>0.5</v>
       </c>
       <c r="W95" s="50" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="X95" s="45"/>
       <c r="Y95" s="35"/>
@@ -7284,13 +7286,13 @@
         <v>14</v>
       </c>
       <c r="C96" s="35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D96" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E96" s="49" t="s">
-        <v>226</v>
+        <v>142</v>
       </c>
       <c r="F96" s="49"/>
       <c r="G96" s="35" t="s">
@@ -7311,7 +7313,7 @@
         <v>3.5</v>
       </c>
       <c r="T96" s="45">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U96" s="45">
         <v>0</v>
@@ -7320,7 +7322,7 @@
         <v>0.5</v>
       </c>
       <c r="W96" s="50" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="X96" s="45"/>
       <c r="Y96" s="35"/>
@@ -7344,13 +7346,13 @@
         <v>14</v>
       </c>
       <c r="C97" s="35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D97" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E97" s="49" t="s">
-        <v>152</v>
+        <v>226</v>
       </c>
       <c r="F97" s="49"/>
       <c r="G97" s="35" t="s">
@@ -7371,7 +7373,7 @@
         <v>3.5</v>
       </c>
       <c r="T97" s="45">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U97" s="45">
         <v>0</v>
@@ -7380,7 +7382,7 @@
         <v>0.5</v>
       </c>
       <c r="W97" s="50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="X97" s="45"/>
       <c r="Y97" s="35"/>
@@ -7404,13 +7406,13 @@
         <v>14</v>
       </c>
       <c r="C98" s="35" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D98" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E98" s="49" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F98" s="49"/>
       <c r="G98" s="35" t="s">
@@ -7431,7 +7433,7 @@
         <v>3.5</v>
       </c>
       <c r="T98" s="45">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U98" s="45">
         <v>0</v>
@@ -7440,7 +7442,7 @@
         <v>0.5</v>
       </c>
       <c r="W98" s="50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="X98" s="45"/>
       <c r="Y98" s="35"/>
@@ -7464,13 +7466,13 @@
         <v>14</v>
       </c>
       <c r="C99" s="35" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="D99" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E99" s="49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F99" s="49"/>
       <c r="G99" s="35" t="s">
@@ -7491,7 +7493,7 @@
         <v>3.5</v>
       </c>
       <c r="T99" s="45">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="U99" s="45">
         <v>0</v>
@@ -7500,7 +7502,7 @@
         <v>0.5</v>
       </c>
       <c r="W99" s="50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="X99" s="45"/>
       <c r="Y99" s="35"/>
@@ -7524,13 +7526,13 @@
         <v>14</v>
       </c>
       <c r="C100" s="35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D100" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E100" s="49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F100" s="49"/>
       <c r="G100" s="35" t="s">
@@ -7551,7 +7553,7 @@
         <v>3.5</v>
       </c>
       <c r="T100" s="45">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="U100" s="45">
         <v>0</v>
@@ -7560,7 +7562,7 @@
         <v>0.5</v>
       </c>
       <c r="W100" s="50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="X100" s="45"/>
       <c r="Y100" s="35"/>
@@ -7584,13 +7586,13 @@
         <v>14</v>
       </c>
       <c r="C101" s="35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D101" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E101" s="49" t="s">
-        <v>217</v>
+        <v>155</v>
       </c>
       <c r="F101" s="49"/>
       <c r="G101" s="35" t="s">
@@ -7611,7 +7613,7 @@
         <v>3.5</v>
       </c>
       <c r="T101" s="45">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="U101" s="45">
         <v>0</v>
@@ -7620,7 +7622,7 @@
         <v>0.5</v>
       </c>
       <c r="W101" s="50" t="s">
-        <v>217</v>
+        <v>155</v>
       </c>
       <c r="X101" s="45"/>
       <c r="Y101" s="35"/>
@@ -7644,13 +7646,13 @@
         <v>14</v>
       </c>
       <c r="C102" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D102" s="35" t="s">
         <v>183</v>
       </c>
       <c r="E102" s="49" t="s">
-        <v>18</v>
+        <v>217</v>
       </c>
       <c r="F102" s="49"/>
       <c r="G102" s="35" t="s">
@@ -7671,7 +7673,7 @@
         <v>3.5</v>
       </c>
       <c r="T102" s="45">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="U102" s="45">
         <v>0</v>
@@ -7680,7 +7682,7 @@
         <v>0.5</v>
       </c>
       <c r="W102" s="50" t="s">
-        <v>18</v>
+        <v>217</v>
       </c>
       <c r="X102" s="45"/>
       <c r="Y102" s="35"/>
@@ -7700,51 +7702,51 @@
       <c r="A103" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B103" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D103" s="5" t="s">
+      <c r="B103" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C103" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="D103" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="E103" s="55" t="s">
-        <v>158</v>
-      </c>
-      <c r="F103" s="55"/>
-      <c r="G103" s="5" t="s">
+      <c r="E103" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="F103" s="49"/>
+      <c r="G103" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
-      <c r="J103" s="5"/>
-      <c r="K103" s="5"/>
-      <c r="L103" s="5"/>
-      <c r="M103" s="5"/>
-      <c r="N103" s="5"/>
-      <c r="O103" s="5"/>
-      <c r="P103" s="19"/>
-      <c r="Q103" s="19"/>
-      <c r="R103" s="5"/>
-      <c r="S103" s="57">
-        <v>4.75</v>
-      </c>
-      <c r="T103" s="57">
-        <v>10.5</v>
-      </c>
-      <c r="U103" s="57">
-        <v>0</v>
-      </c>
-      <c r="V103" s="57">
+      <c r="H103" s="35"/>
+      <c r="I103" s="35"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="35"/>
+      <c r="L103" s="35"/>
+      <c r="M103" s="35"/>
+      <c r="N103" s="35"/>
+      <c r="O103" s="35"/>
+      <c r="P103" s="50"/>
+      <c r="Q103" s="50"/>
+      <c r="R103" s="35"/>
+      <c r="S103" s="45">
+        <v>3.5</v>
+      </c>
+      <c r="T103" s="45">
+        <v>5</v>
+      </c>
+      <c r="U103" s="45">
+        <v>0</v>
+      </c>
+      <c r="V103" s="10">
         <v>0.5</v>
       </c>
-      <c r="W103" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="X103" s="57"/>
-      <c r="Y103" s="5"/>
-      <c r="Z103" s="56"/>
+      <c r="W103" s="50" t="s">
+        <v>18</v>
+      </c>
+      <c r="X103" s="45"/>
+      <c r="Y103" s="35"/>
+      <c r="Z103" s="34"/>
       <c r="AA103" s="11"/>
       <c r="AB103" s="11"/>
       <c r="AC103" s="7"/>
@@ -7764,13 +7766,13 @@
         <v>14</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E104" s="55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F104" s="55"/>
       <c r="G104" s="5" t="s">
@@ -7791,7 +7793,7 @@
         <v>4.75</v>
       </c>
       <c r="T104" s="57">
-        <v>10</v>
+        <v>10.5</v>
       </c>
       <c r="U104" s="57">
         <v>0</v>
@@ -7800,7 +7802,7 @@
         <v>0.5</v>
       </c>
       <c r="W104" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="X104" s="57"/>
       <c r="Y104" s="5"/>
@@ -7824,13 +7826,13 @@
         <v>14</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E105" s="55" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="F105" s="55"/>
       <c r="G105" s="5" t="s">
@@ -7851,7 +7853,7 @@
         <v>4.75</v>
       </c>
       <c r="T105" s="57">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="U105" s="57">
         <v>0</v>
@@ -7860,7 +7862,7 @@
         <v>0.5</v>
       </c>
       <c r="W105" s="19" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="X105" s="57"/>
       <c r="Y105" s="5"/>
@@ -7884,13 +7886,13 @@
         <v>14</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E106" s="55" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="F106" s="55"/>
       <c r="G106" s="5" t="s">
@@ -7911,7 +7913,7 @@
         <v>4.75</v>
       </c>
       <c r="T106" s="57">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="U106" s="57">
         <v>0</v>
@@ -7920,7 +7922,7 @@
         <v>0.5</v>
       </c>
       <c r="W106" s="19" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="X106" s="57"/>
       <c r="Y106" s="5"/>
@@ -7944,13 +7946,13 @@
         <v>14</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E107" s="55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F107" s="55"/>
       <c r="G107" s="5" t="s">
@@ -7971,7 +7973,7 @@
         <v>4.75</v>
       </c>
       <c r="T107" s="57">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="U107" s="57">
         <v>0</v>
@@ -7980,7 +7982,7 @@
         <v>0.5</v>
       </c>
       <c r="W107" s="19" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="X107" s="57"/>
       <c r="Y107" s="5"/>
@@ -8004,13 +8006,13 @@
         <v>14</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E108" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F108" s="55"/>
       <c r="G108" s="5" t="s">
@@ -8031,7 +8033,7 @@
         <v>4.75</v>
       </c>
       <c r="T108" s="57">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U108" s="57">
         <v>0</v>
@@ -8040,7 +8042,7 @@
         <v>0.5</v>
       </c>
       <c r="W108" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X108" s="57"/>
       <c r="Y108" s="5"/>
@@ -8064,13 +8066,13 @@
         <v>14</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E109" s="55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F109" s="55"/>
       <c r="G109" s="5" t="s">
@@ -8091,7 +8093,7 @@
         <v>4.75</v>
       </c>
       <c r="T109" s="57">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="U109" s="57">
         <v>0</v>
@@ -8100,7 +8102,7 @@
         <v>0.5</v>
       </c>
       <c r="W109" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X109" s="57"/>
       <c r="Y109" s="5"/>
@@ -8124,13 +8126,13 @@
         <v>14</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>183</v>
       </c>
       <c r="E110" s="55" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="F110" s="55"/>
       <c r="G110" s="5" t="s">
@@ -8151,7 +8153,7 @@
         <v>4.75</v>
       </c>
       <c r="T110" s="57">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="U110" s="57">
         <v>0</v>
@@ -8160,7 +8162,7 @@
         <v>0.5</v>
       </c>
       <c r="W110" s="19" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="X110" s="57"/>
       <c r="Y110" s="5"/>
@@ -8176,111 +8178,107 @@
       <c r="AI110" s="7"/>
       <c r="AJ110" s="13"/>
     </row>
-    <row r="111" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
+    <row r="111" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E111" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F111" s="55"/>
+      <c r="G111" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5"/>
+      <c r="M111" s="5"/>
+      <c r="N111" s="5"/>
+      <c r="O111" s="5"/>
+      <c r="P111" s="19"/>
+      <c r="Q111" s="19"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="57">
+        <v>4.75</v>
+      </c>
+      <c r="T111" s="57">
+        <v>7</v>
+      </c>
+      <c r="U111" s="57">
+        <v>0</v>
+      </c>
+      <c r="V111" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="W111" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="X111" s="57"/>
+      <c r="Y111" s="5"/>
+      <c r="Z111" s="56"/>
+      <c r="AA111" s="11"/>
+      <c r="AB111" s="11"/>
+      <c r="AC111" s="7"/>
+      <c r="AD111" s="13"/>
+      <c r="AE111" s="7"/>
+      <c r="AF111" s="7"/>
+      <c r="AG111" s="11"/>
+      <c r="AH111" s="11"/>
+      <c r="AI111" s="7"/>
+      <c r="AJ111" s="13"/>
+    </row>
+    <row r="112" spans="1:36" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B112" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
-      <c r="H111" s="14"/>
-      <c r="I111" s="14"/>
-      <c r="J111" s="14"/>
-      <c r="K111" s="14"/>
-      <c r="L111" s="14"/>
-      <c r="M111" s="14"/>
-      <c r="N111" s="14"/>
-      <c r="O111" s="14"/>
-      <c r="P111" s="15"/>
-      <c r="Q111" s="15"/>
-      <c r="R111" s="16"/>
-      <c r="S111" s="17"/>
-      <c r="T111" s="17"/>
-      <c r="U111" s="17"/>
-      <c r="V111" s="17"/>
-      <c r="W111" s="17"/>
-      <c r="X111" s="17"/>
-      <c r="Y111" s="14"/>
-      <c r="Z111" s="16"/>
-      <c r="AA111" s="16"/>
-      <c r="AB111" s="16"/>
-      <c r="AC111" s="16"/>
-      <c r="AD111" s="16"/>
-      <c r="AE111" s="16"/>
-      <c r="AF111" s="16"/>
-      <c r="AG111" s="16"/>
-      <c r="AH111" s="16"/>
-      <c r="AI111" s="16"/>
-      <c r="AJ111" s="16"/>
-    </row>
-    <row r="112" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="B112" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C112" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="D112" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="E112" s="49"/>
-      <c r="F112" s="49"/>
-      <c r="G112" s="35"/>
-      <c r="H112" s="35"/>
-      <c r="I112" s="35"/>
-      <c r="J112" s="35"/>
-      <c r="K112" s="35"/>
-      <c r="L112" s="35"/>
-      <c r="M112" s="35"/>
-      <c r="N112" s="35"/>
-      <c r="O112" s="35"/>
-      <c r="P112" s="50"/>
-      <c r="Q112" s="50"/>
-      <c r="R112" s="35"/>
-      <c r="S112" s="45">
-        <v>1</v>
-      </c>
-      <c r="T112" s="45">
-        <v>4.0069999999999997</v>
-      </c>
-      <c r="U112" s="45">
-        <v>0</v>
-      </c>
-      <c r="V112" s="45">
-        <v>0</v>
-      </c>
-      <c r="W112" s="50"/>
-      <c r="X112" s="45"/>
-      <c r="Y112" s="35"/>
-      <c r="Z112" s="34"/>
-      <c r="AA112" s="11"/>
-      <c r="AB112" s="11"/>
-      <c r="AC112" s="7"/>
-      <c r="AD112" s="13"/>
-      <c r="AE112" s="35" t="s">
-        <v>234</v>
-      </c>
-      <c r="AF112" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="AG112" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH112" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI112" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ112" s="13"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
+      <c r="J112" s="14"/>
+      <c r="K112" s="14"/>
+      <c r="L112" s="14"/>
+      <c r="M112" s="14"/>
+      <c r="N112" s="14"/>
+      <c r="O112" s="14"/>
+      <c r="P112" s="15"/>
+      <c r="Q112" s="15"/>
+      <c r="R112" s="16"/>
+      <c r="S112" s="17"/>
+      <c r="T112" s="17"/>
+      <c r="U112" s="17"/>
+      <c r="V112" s="17"/>
+      <c r="W112" s="17"/>
+      <c r="X112" s="17"/>
+      <c r="Y112" s="14"/>
+      <c r="Z112" s="16"/>
+      <c r="AA112" s="16"/>
+      <c r="AB112" s="16"/>
+      <c r="AC112" s="16"/>
+      <c r="AD112" s="16"/>
+      <c r="AE112" s="16"/>
+      <c r="AF112" s="16"/>
+      <c r="AG112" s="16"/>
+      <c r="AH112" s="16"/>
+      <c r="AI112" s="16"/>
+      <c r="AJ112" s="16"/>
     </row>
     <row r="113" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="9" t="s">
@@ -8290,10 +8288,10 @@
         <v>14</v>
       </c>
       <c r="C113" s="35" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D113" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E113" s="49"/>
       <c r="F113" s="49"/>
@@ -8310,10 +8308,10 @@
       <c r="Q113" s="50"/>
       <c r="R113" s="35"/>
       <c r="S113" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T113" s="45">
-        <v>3.9529999999999998</v>
+        <v>4.0069999999999997</v>
       </c>
       <c r="U113" s="45">
         <v>0</v>
@@ -8329,11 +8327,21 @@
       <c r="AB113" s="11"/>
       <c r="AC113" s="7"/>
       <c r="AD113" s="13"/>
-      <c r="AE113" s="7"/>
-      <c r="AF113" s="7"/>
-      <c r="AG113" s="11"/>
-      <c r="AH113" s="11"/>
-      <c r="AI113" s="7"/>
+      <c r="AE113" s="35" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF113" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AG113" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH113" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI113" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="AJ113" s="13"/>
     </row>
     <row r="114" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8344,10 +8352,10 @@
         <v>14</v>
       </c>
       <c r="C114" s="35" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D114" s="35" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E114" s="49"/>
       <c r="F114" s="49"/>
@@ -8364,10 +8372,10 @@
       <c r="Q114" s="50"/>
       <c r="R114" s="35"/>
       <c r="S114" s="45">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="T114" s="45">
-        <v>3.5070000000000001</v>
+        <v>3.9529999999999998</v>
       </c>
       <c r="U114" s="45">
         <v>0</v>
@@ -8383,24 +8391,12 @@
       <c r="AB114" s="11"/>
       <c r="AC114" s="7"/>
       <c r="AD114" s="13"/>
-      <c r="AE114" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="AF114" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="AG114" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH114" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI114" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="AJ114" s="13" t="s">
-        <v>231</v>
-      </c>
+      <c r="AE114" s="7"/>
+      <c r="AF114" s="7"/>
+      <c r="AG114" s="11"/>
+      <c r="AH114" s="11"/>
+      <c r="AI114" s="7"/>
+      <c r="AJ114" s="13"/>
     </row>
     <row r="115" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="9" t="s">
@@ -8410,10 +8406,10 @@
         <v>14</v>
       </c>
       <c r="C115" s="35" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D115" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E115" s="49"/>
       <c r="F115" s="49"/>
@@ -8430,10 +8426,10 @@
       <c r="Q115" s="50"/>
       <c r="R115" s="35"/>
       <c r="S115" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T115" s="45">
-        <v>3.4529999999999998</v>
+        <v>3.5070000000000001</v>
       </c>
       <c r="U115" s="45">
         <v>0</v>
@@ -8449,12 +8445,24 @@
       <c r="AB115" s="11"/>
       <c r="AC115" s="7"/>
       <c r="AD115" s="13"/>
-      <c r="AE115" s="7"/>
-      <c r="AF115" s="7"/>
-      <c r="AG115" s="11"/>
-      <c r="AH115" s="11"/>
-      <c r="AI115" s="7"/>
-      <c r="AJ115" s="13"/>
+      <c r="AE115" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF115" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="AG115" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH115" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI115" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AJ115" s="13" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="116" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
@@ -8464,10 +8472,10 @@
         <v>14</v>
       </c>
       <c r="C116" s="35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D116" s="35" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E116" s="49"/>
       <c r="F116" s="49"/>
@@ -8484,10 +8492,10 @@
       <c r="Q116" s="50"/>
       <c r="R116" s="35"/>
       <c r="S116" s="45">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="T116" s="45">
-        <v>3.0070000000000001</v>
+        <v>3.4529999999999998</v>
       </c>
       <c r="U116" s="45">
         <v>0</v>
@@ -8503,24 +8511,12 @@
       <c r="AB116" s="11"/>
       <c r="AC116" s="7"/>
       <c r="AD116" s="13"/>
-      <c r="AE116" s="35" t="s">
-        <v>239</v>
-      </c>
-      <c r="AF116" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="AG116" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH116" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI116" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ116" s="13" t="s">
-        <v>256</v>
-      </c>
+      <c r="AE116" s="7"/>
+      <c r="AF116" s="7"/>
+      <c r="AG116" s="11"/>
+      <c r="AH116" s="11"/>
+      <c r="AI116" s="7"/>
+      <c r="AJ116" s="13"/>
     </row>
     <row r="117" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="9" t="s">
@@ -8530,10 +8526,10 @@
         <v>14</v>
       </c>
       <c r="C117" s="35" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D117" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E117" s="49"/>
       <c r="F117" s="49"/>
@@ -8550,10 +8546,10 @@
       <c r="Q117" s="50"/>
       <c r="R117" s="35"/>
       <c r="S117" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T117" s="45">
-        <v>2.9529999999999998</v>
+        <v>3.0070000000000001</v>
       </c>
       <c r="U117" s="45">
         <v>0</v>
@@ -8569,12 +8565,24 @@
       <c r="AB117" s="11"/>
       <c r="AC117" s="7"/>
       <c r="AD117" s="13"/>
-      <c r="AE117" s="7"/>
-      <c r="AF117" s="7"/>
-      <c r="AG117" s="11"/>
-      <c r="AH117" s="11"/>
-      <c r="AI117" s="7"/>
-      <c r="AJ117" s="13"/>
+      <c r="AE117" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="AF117" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="AG117" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH117" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI117" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ117" s="13" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="118" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
@@ -8584,10 +8592,10 @@
         <v>14</v>
       </c>
       <c r="C118" s="35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D118" s="35" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E118" s="49"/>
       <c r="F118" s="49"/>
@@ -8604,10 +8612,10 @@
       <c r="Q118" s="50"/>
       <c r="R118" s="35"/>
       <c r="S118" s="45">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="T118" s="45">
-        <v>2.5070000000000001</v>
+        <v>2.9529999999999998</v>
       </c>
       <c r="U118" s="45">
         <v>0</v>
@@ -8623,24 +8631,12 @@
       <c r="AB118" s="11"/>
       <c r="AC118" s="7"/>
       <c r="AD118" s="13"/>
-      <c r="AE118" s="35" t="s">
-        <v>241</v>
-      </c>
-      <c r="AF118" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="AG118" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH118" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI118" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ118" s="13" t="s">
-        <v>232</v>
-      </c>
+      <c r="AE118" s="7"/>
+      <c r="AF118" s="7"/>
+      <c r="AG118" s="11"/>
+      <c r="AH118" s="11"/>
+      <c r="AI118" s="7"/>
+      <c r="AJ118" s="13"/>
     </row>
     <row r="119" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="9" t="s">
@@ -8650,10 +8646,10 @@
         <v>14</v>
       </c>
       <c r="C119" s="35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D119" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E119" s="49"/>
       <c r="F119" s="49"/>
@@ -8670,10 +8666,10 @@
       <c r="Q119" s="50"/>
       <c r="R119" s="35"/>
       <c r="S119" s="45">
-        <v>2.25</v>
+        <v>1</v>
       </c>
       <c r="T119" s="45">
-        <v>2.4529999999999998</v>
+        <v>2.5070000000000001</v>
       </c>
       <c r="U119" s="45">
         <v>0</v>
@@ -8689,78 +8685,78 @@
       <c r="AB119" s="11"/>
       <c r="AC119" s="7"/>
       <c r="AD119" s="13"/>
-      <c r="AE119" s="7"/>
-      <c r="AF119" s="7"/>
-      <c r="AG119" s="11"/>
-      <c r="AH119" s="11"/>
-      <c r="AI119" s="7"/>
-      <c r="AJ119" s="13"/>
+      <c r="AE119" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="AF119" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="AG119" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH119" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI119" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ119" s="13" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="120" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B120" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E120" s="58"/>
-      <c r="F120" s="58"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
-      <c r="I120" s="1"/>
-      <c r="J120" s="1"/>
-      <c r="K120" s="1"/>
-      <c r="L120" s="1"/>
-      <c r="M120" s="1"/>
-      <c r="N120" s="1"/>
-      <c r="O120" s="1"/>
-      <c r="P120" s="2"/>
-      <c r="Q120" s="2"/>
-      <c r="R120" s="1"/>
-      <c r="S120" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="T120" s="3">
-        <v>4.0069999999999997</v>
-      </c>
-      <c r="U120" s="3">
-        <v>0</v>
-      </c>
-      <c r="V120" s="3">
-        <v>0</v>
-      </c>
-      <c r="W120" s="2"/>
-      <c r="X120" s="3"/>
-      <c r="Y120" s="1"/>
-      <c r="Z120" s="59"/>
+      <c r="B120" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D120" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E120" s="49"/>
+      <c r="F120" s="49"/>
+      <c r="G120" s="35"/>
+      <c r="H120" s="35"/>
+      <c r="I120" s="35"/>
+      <c r="J120" s="35"/>
+      <c r="K120" s="35"/>
+      <c r="L120" s="35"/>
+      <c r="M120" s="35"/>
+      <c r="N120" s="35"/>
+      <c r="O120" s="35"/>
+      <c r="P120" s="50"/>
+      <c r="Q120" s="50"/>
+      <c r="R120" s="35"/>
+      <c r="S120" s="45">
+        <v>2.25</v>
+      </c>
+      <c r="T120" s="45">
+        <v>2.4529999999999998</v>
+      </c>
+      <c r="U120" s="45">
+        <v>0</v>
+      </c>
+      <c r="V120" s="45">
+        <v>0</v>
+      </c>
+      <c r="W120" s="50"/>
+      <c r="X120" s="45"/>
+      <c r="Y120" s="35"/>
+      <c r="Z120" s="34"/>
       <c r="AA120" s="11"/>
       <c r="AB120" s="11"/>
       <c r="AC120" s="7"/>
       <c r="AD120" s="13"/>
-      <c r="AE120" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="AF120" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="AG120" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH120" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI120" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ120" s="13" t="s">
-        <v>257</v>
-      </c>
+      <c r="AE120" s="7"/>
+      <c r="AF120" s="7"/>
+      <c r="AG120" s="11"/>
+      <c r="AH120" s="11"/>
+      <c r="AI120" s="7"/>
+      <c r="AJ120" s="13"/>
     </row>
     <row r="121" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
@@ -8770,10 +8766,10 @@
         <v>14</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E121" s="58"/>
       <c r="F121" s="58"/>
@@ -8790,10 +8786,10 @@
       <c r="Q121" s="2"/>
       <c r="R121" s="1"/>
       <c r="S121" s="3">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="T121" s="3">
-        <v>3.9529999999999998</v>
+        <v>4.0069999999999997</v>
       </c>
       <c r="U121" s="3">
         <v>0</v>
@@ -8809,12 +8805,24 @@
       <c r="AB121" s="11"/>
       <c r="AC121" s="7"/>
       <c r="AD121" s="13"/>
-      <c r="AE121" s="7"/>
-      <c r="AF121" s="7"/>
-      <c r="AG121" s="11"/>
-      <c r="AH121" s="11"/>
-      <c r="AI121" s="7"/>
-      <c r="AJ121" s="13"/>
+      <c r="AE121" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="AF121" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG121" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH121" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI121" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ121" s="13" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="122" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
@@ -8824,10 +8832,10 @@
         <v>14</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E122" s="58"/>
       <c r="F122" s="58"/>
@@ -8844,10 +8852,10 @@
       <c r="Q122" s="2"/>
       <c r="R122" s="1"/>
       <c r="S122" s="3">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="T122" s="3">
-        <v>3.5070000000000001</v>
+        <v>3.9529999999999998</v>
       </c>
       <c r="U122" s="3">
         <v>0</v>
@@ -8863,24 +8871,12 @@
       <c r="AB122" s="11"/>
       <c r="AC122" s="7"/>
       <c r="AD122" s="13"/>
-      <c r="AE122" s="35" t="s">
-        <v>245</v>
-      </c>
-      <c r="AF122" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="AG122" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH122" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI122" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ122" s="13" t="s">
-        <v>258</v>
-      </c>
+      <c r="AE122" s="7"/>
+      <c r="AF122" s="7"/>
+      <c r="AG122" s="11"/>
+      <c r="AH122" s="11"/>
+      <c r="AI122" s="7"/>
+      <c r="AJ122" s="13"/>
     </row>
     <row r="123" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
@@ -8890,10 +8886,10 @@
         <v>14</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E123" s="58"/>
       <c r="F123" s="58"/>
@@ -8910,10 +8906,10 @@
       <c r="Q123" s="2"/>
       <c r="R123" s="1"/>
       <c r="S123" s="3">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="T123" s="3">
-        <v>3.4529999999999998</v>
+        <v>3.5070000000000001</v>
       </c>
       <c r="U123" s="3">
         <v>0</v>
@@ -8929,12 +8925,24 @@
       <c r="AB123" s="11"/>
       <c r="AC123" s="7"/>
       <c r="AD123" s="13"/>
-      <c r="AE123" s="7"/>
-      <c r="AF123" s="7"/>
-      <c r="AG123" s="11"/>
-      <c r="AH123" s="11"/>
-      <c r="AI123" s="7"/>
-      <c r="AJ123" s="13"/>
+      <c r="AE123" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="AF123" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AG123" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH123" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI123" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ123" s="13" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="124" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="9" t="s">
@@ -8944,10 +8952,10 @@
         <v>14</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E124" s="58"/>
       <c r="F124" s="58"/>
@@ -8964,10 +8972,10 @@
       <c r="Q124" s="2"/>
       <c r="R124" s="1"/>
       <c r="S124" s="3">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="T124" s="3">
-        <v>3</v>
+        <v>3.4529999999999998</v>
       </c>
       <c r="U124" s="3">
         <v>0</v>
@@ -8983,24 +8991,12 @@
       <c r="AB124" s="11"/>
       <c r="AC124" s="7"/>
       <c r="AD124" s="13"/>
-      <c r="AE124" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="AF124" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="AG124" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AH124" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="AI124" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ124" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="AE124" s="7"/>
+      <c r="AF124" s="7"/>
+      <c r="AG124" s="11"/>
+      <c r="AH124" s="11"/>
+      <c r="AI124" s="7"/>
+      <c r="AJ124" s="13"/>
     </row>
     <row r="125" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
@@ -9010,10 +9006,10 @@
         <v>14</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E125" s="58"/>
       <c r="F125" s="58"/>
@@ -9030,10 +9026,10 @@
       <c r="Q125" s="2"/>
       <c r="R125" s="1"/>
       <c r="S125" s="3">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="T125" s="3">
-        <v>2.9529999999999998</v>
+        <v>3</v>
       </c>
       <c r="U125" s="3">
         <v>0</v>
@@ -9049,14 +9045,79 @@
       <c r="AB125" s="11"/>
       <c r="AC125" s="7"/>
       <c r="AD125" s="13"/>
-      <c r="AE125" s="7"/>
-      <c r="AF125" s="7"/>
-      <c r="AG125" s="11"/>
-      <c r="AH125" s="11"/>
-      <c r="AI125" s="7"/>
-      <c r="AJ125" s="13"/>
-    </row>
-    <row r="126" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AE125" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF125" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AG125" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH125" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI125" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ125" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="126" spans="1:36" s="12" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E126" s="58"/>
+      <c r="F126" s="58"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+      <c r="J126" s="1"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="1"/>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
+      <c r="O126" s="1"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+      <c r="R126" s="1"/>
+      <c r="S126" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="T126" s="3">
+        <v>2.9529999999999998</v>
+      </c>
+      <c r="U126" s="3">
+        <v>0</v>
+      </c>
+      <c r="V126" s="3">
+        <v>0</v>
+      </c>
+      <c r="W126" s="2"/>
+      <c r="X126" s="3"/>
+      <c r="Y126" s="1"/>
+      <c r="Z126" s="59"/>
+      <c r="AA126" s="11"/>
+      <c r="AB126" s="11"/>
+      <c r="AC126" s="7"/>
+      <c r="AD126" s="13"/>
+      <c r="AE126" s="7"/>
+      <c r="AF126" s="7"/>
+      <c r="AG126" s="11"/>
+      <c r="AH126" s="11"/>
+      <c r="AI126" s="7"/>
+      <c r="AJ126" s="13"/>
+    </row>
     <row r="127" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="1:36" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="129" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9064,10 +9125,11 @@
     <row r="131" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="132" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="133" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:AJ125" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}"/>
+  <autoFilter ref="A1:AJ126" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}"/>
   <dataValidations count="1">
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X111 X69:X82 X2:X52 X55:X66 E1:E1048576" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="X112 X70:X83 X2:X52 E1:E1048576 X55:X67" xr:uid="{F8EA18B6-58A3-4BFA-B288-9FBEC18F1231}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9079,55 +9141,55 @@
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>Y69 Y2:Y5 Y111 Y7</xm:sqref>
+          <xm:sqref>Y70 Y2:Y5 Y112 Y7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2:AA125 AG2:AG125</xm:sqref>
+          <xm:sqref>AG2:AG126 AA2:AA126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AB2:AB125 AH2:AH125</xm:sqref>
+          <xm:sqref>AH2:AH126 AB2:AB126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D20E3002-F58D-4FAD-9CC5-854E38BB1BD9}">
           <x14:formula1>
             <xm:f>Tables!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F125</xm:sqref>
+          <xm:sqref>F2:F126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{0B95AA9E-6EAC-4E79-9737-4C4B42A3B143}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$43</xm:f>
           </x14:formula1>
-          <xm:sqref>AI2:AI125 W2:W125 AC2:AC125</xm:sqref>
+          <xm:sqref>AC2:AC126 W2:W126 AI2:AI126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{8B6AE078-B717-4B67-83B7-999D58BC2953}">
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G125</xm:sqref>
+          <xm:sqref>G2:G126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{434DCAEE-02F3-44B7-8757-503F2F2EE546}">
           <x14:formula1>
             <xm:f>Tables!$M$2:$M$8</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD125 AJ2:AJ125</xm:sqref>
+          <xm:sqref>AJ2:AJ126 AD2:AD126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{144C7DAB-B2EC-4CB7-AB17-A3FF60790568}">
           <x14:formula1>
             <xm:f>Tables!$K$2:$K$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B125</xm:sqref>
+          <xm:sqref>B2:B126</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{72B07BB6-2E46-454E-98E1-28DF9333D6FA}">
           <x14:formula1>
-            <xm:f>Tables!$O$2:$O$55</xm:f>
+            <xm:f>Tables!$O$2:$O$56</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D125</xm:sqref>
+          <xm:sqref>D2:D126</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9462,7 +9524,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -9567,8 +9629,8 @@
       <c r="M4" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="O4" s="41" t="s">
-        <v>94</v>
+      <c r="O4" s="47" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9592,7 +9654,7 @@
         <v>232</v>
       </c>
       <c r="O5" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9616,7 +9678,7 @@
         <v>257</v>
       </c>
       <c r="O6" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9633,7 +9695,7 @@
         <v>258</v>
       </c>
       <c r="O7" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9647,7 +9709,7 @@
         <v>259</v>
       </c>
       <c r="O8" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9658,7 +9720,7 @@
         <v>10</v>
       </c>
       <c r="O9" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9668,8 +9730,8 @@
       <c r="E10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="42" t="s">
-        <v>100</v>
+      <c r="O10" s="41" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9679,8 +9741,8 @@
       <c r="E11" s="11">
         <v>11</v>
       </c>
-      <c r="O11" s="41" t="s">
-        <v>101</v>
+      <c r="O11" s="42" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9691,7 +9753,7 @@
         <v>37</v>
       </c>
       <c r="O12" s="41" t="s">
-        <v>165</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9702,7 +9764,7 @@
         <v>12</v>
       </c>
       <c r="O13" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9713,7 +9775,7 @@
         <v>38</v>
       </c>
       <c r="O14" s="41" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9724,7 +9786,7 @@
         <v>14</v>
       </c>
       <c r="O15" s="41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9734,16 +9796,16 @@
       <c r="E16" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="42" t="s">
-        <v>104</v>
+      <c r="O16" s="41" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="O17" s="41" t="s">
-        <v>113</v>
+      <c r="O17" s="42" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9751,7 +9813,7 @@
         <v>215</v>
       </c>
       <c r="O18" s="41" t="s">
-        <v>318</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9759,7 +9821,7 @@
         <v>216</v>
       </c>
       <c r="O19" s="41" t="s">
-        <v>167</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9767,7 +9829,7 @@
         <v>145</v>
       </c>
       <c r="O20" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9775,7 +9837,7 @@
         <v>146</v>
       </c>
       <c r="O21" s="41" t="s">
-        <v>105</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9783,7 +9845,7 @@
         <v>147</v>
       </c>
       <c r="O22" s="41" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9791,7 +9853,7 @@
         <v>148</v>
       </c>
       <c r="O23" s="41" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9799,7 +9861,7 @@
         <v>149</v>
       </c>
       <c r="O24" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9807,7 +9869,7 @@
         <v>150</v>
       </c>
       <c r="O25" s="41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9815,7 +9877,7 @@
         <v>151</v>
       </c>
       <c r="O26" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9823,7 +9885,7 @@
         <v>152</v>
       </c>
       <c r="O27" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9831,31 +9893,31 @@
         <v>153</v>
       </c>
       <c r="O28" s="41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="O29" s="47" t="s">
-        <v>322</v>
+      <c r="O29" s="41" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="O30" s="42" t="s">
-        <v>112</v>
+      <c r="O30" s="47" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="O31" s="41" t="s">
-        <v>88</v>
+      <c r="O31" s="42" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9863,23 +9925,23 @@
         <v>217</v>
       </c>
       <c r="O32" s="41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="O33" s="42" t="s">
-        <v>117</v>
+      <c r="O33" s="41" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="O34" s="41" t="s">
-        <v>118</v>
+      <c r="O34" s="42" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9887,7 +9949,7 @@
         <v>158</v>
       </c>
       <c r="O35" s="41" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9895,7 +9957,7 @@
         <v>25</v>
       </c>
       <c r="O36" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9903,7 +9965,7 @@
         <v>159</v>
       </c>
       <c r="O37" s="41" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9911,7 +9973,7 @@
         <v>160</v>
       </c>
       <c r="O38" s="41" t="s">
-        <v>169</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9919,7 +9981,7 @@
         <v>161</v>
       </c>
       <c r="O39" s="41" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9927,7 +9989,7 @@
         <v>162</v>
       </c>
       <c r="O40" s="41" t="s">
-        <v>91</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9935,7 +9997,7 @@
         <v>163</v>
       </c>
       <c r="O41" s="41" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9943,7 +10005,7 @@
         <v>164</v>
       </c>
       <c r="O42" s="41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9951,70 +10013,74 @@
         <v>26</v>
       </c>
       <c r="O43" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O44" s="41" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O45" s="41" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O46" s="41" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O47" s="41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O48" s="41" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O48" s="47" t="s">
+    <row r="49" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O49" s="47" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O49" s="41" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="50" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O50" s="41" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O51" s="41" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O52" s="41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O53" s="41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O54" s="41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O55" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O56" s="41" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="15:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>